<commit_message>
rough section 4.B structure with all prompts and choices
</commit_message>
<xml_diff>
--- a/tables/actor/forms/actor/actor.xlsx
+++ b/tables/actor/forms/actor/actor.xlsx
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="361" uniqueCount="214">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="391" uniqueCount="229">
   <si>
     <t xml:space="preserve">clause</t>
   </si>
@@ -1316,6 +1316,51 @@
     <t xml:space="preserve">migrantDebt</t>
   </si>
   <si>
+    <t xml:space="preserve">myanmarNational</t>
+  </si>
+  <si>
+    <t xml:space="preserve">thailandNational</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sameEthnicity</t>
+  </si>
+  <si>
+    <t xml:space="preserve">migratedThailandBeforeMigrant</t>
+  </si>
+  <si>
+    <t xml:space="preserve">migratedThailandAfterMigrant</t>
+  </si>
+  <si>
+    <t xml:space="preserve">currentlyInThailand</t>
+  </si>
+  <si>
+    <t xml:space="preserve">remittances</t>
+  </si>
+  <si>
+    <t xml:space="preserve">arrangedForOthers</t>
+  </si>
+  <si>
+    <t xml:space="preserve">previousRecruiter</t>
+  </si>
+  <si>
+    <t xml:space="preserve">brokerForMigrant</t>
+  </si>
+  <si>
+    <t xml:space="preserve">agentForMigrant</t>
+  </si>
+  <si>
+    <t xml:space="preserve">recruiterAgentForMigrant</t>
+  </si>
+  <si>
+    <t xml:space="preserve">seekHelpAgain</t>
+  </si>
+  <si>
+    <t xml:space="preserve">mostValuableHelp</t>
+  </si>
+  <si>
+    <t xml:space="preserve">causedProblems</t>
+  </si>
+  <si>
     <t xml:space="preserve">calculation_name</t>
   </si>
 </sst>
@@ -1424,7 +1469,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="13">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1469,10 +1514,6 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1501,16 +1542,14 @@
   <dimension ref="1:6"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B13" activeCellId="1" sqref="B40:C40 B13"/>
+      <selection pane="topLeft" activeCell="B13" activeCellId="0" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="16.5"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="7.34848484848485"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="20.979797979798"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="46.1010101010101"/>
-    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="7.34848484848485"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="16.0353535353535"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="20.4444444444444"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="45.1666666666667"/>
   </cols>
   <sheetData>
     <row r="1" s="2" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1562,18 +1601,18 @@
   <dimension ref="A1:I11"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C9" activeCellId="1" sqref="B40:C40 C9"/>
+      <selection pane="topLeft" activeCell="C9" activeCellId="0" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="16.0353535353535"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="15.5"/>
-    <col collapsed="false" hidden="false" max="4" min="3" style="0" width="21.8636363636364"/>
-    <col collapsed="false" hidden="false" max="7" min="5" style="0" width="7.61616161616162"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="24.0555555555556"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="23.9191919191919"/>
-    <col collapsed="false" hidden="false" max="1025" min="10" style="0" width="7.61616161616162"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="15.6363636363636"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="15.1010101010101"/>
+    <col collapsed="false" hidden="false" max="4" min="3" style="0" width="21.3787878787879"/>
+    <col collapsed="false" hidden="false" max="7" min="5" style="0" width="7.34848484848485"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="23.3838383838384"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="23.2525252525253"/>
+    <col collapsed="false" hidden="false" max="1025" min="10" style="0" width="7.34848484848485"/>
   </cols>
   <sheetData>
     <row r="1" s="2" customFormat="true" ht="18.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1694,16 +1733,16 @@
   <dimension ref="1:59"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A10" activeCellId="1" sqref="B40:C40 A10"/>
+      <selection pane="topLeft" activeCell="A10" activeCellId="0" sqref="A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="3" width="35.2777777777778"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="3" width="53.8535353535354"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="3" width="54.4646464646465"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="3" width="91.7424242424243"/>
-    <col collapsed="false" hidden="false" max="1025" min="5" style="3" width="5.47979797979798"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="3" width="34.4747474747475"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="3" width="52.6515151515152"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="3" width="53.1818181818182"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="3" width="89.7979797979798"/>
+    <col collapsed="false" hidden="false" max="1025" min="5" style="3" width="5.21212121212121"/>
   </cols>
   <sheetData>
     <row r="1" s="1" customFormat="true" ht="14.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -30584,52 +30623,52 @@
       <c r="C49" s="8"/>
     </row>
     <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A50" s="11"/>
+      <c r="A50" s="7"/>
       <c r="B50" s="8"/>
       <c r="C50" s="8"/>
     </row>
     <row r="51" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A51" s="11"/>
+      <c r="A51" s="7"/>
       <c r="B51" s="8"/>
       <c r="C51" s="8"/>
     </row>
     <row r="52" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A52" s="11"/>
+      <c r="A52" s="7"/>
       <c r="B52" s="8"/>
       <c r="C52" s="8"/>
     </row>
     <row r="53" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A53" s="11"/>
+      <c r="A53" s="7"/>
       <c r="B53" s="8"/>
       <c r="C53" s="8"/>
     </row>
     <row r="54" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A54" s="11"/>
+      <c r="A54" s="7"/>
       <c r="B54" s="8"/>
       <c r="C54" s="8"/>
     </row>
     <row r="55" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A55" s="11"/>
+      <c r="A55" s="7"/>
       <c r="B55" s="8"/>
       <c r="C55" s="8"/>
     </row>
     <row r="56" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A56" s="11"/>
+      <c r="A56" s="7"/>
       <c r="B56" s="8"/>
       <c r="C56" s="8"/>
     </row>
     <row r="57" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A57" s="11"/>
+      <c r="A57" s="7"/>
       <c r="B57" s="8"/>
       <c r="C57" s="8"/>
     </row>
     <row r="58" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A58" s="11"/>
+      <c r="A58" s="7"/>
       <c r="B58" s="8"/>
       <c r="C58" s="8"/>
     </row>
     <row r="59" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A59" s="12"/>
+      <c r="A59" s="11"/>
       <c r="B59" s="8"/>
       <c r="C59" s="8"/>
     </row>
@@ -30652,26 +30691,25 @@
   <dimension ref="1:10"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E11" activeCellId="1" sqref="B40:C40 E11"/>
+      <selection pane="topLeft" activeCell="E11" activeCellId="0" sqref="E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="10.6919191919192"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="14.5656565656566"/>
-    <col collapsed="false" hidden="false" max="4" min="3" style="0" width="12.3737373737374"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="18.6969696969697"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="22.5555555555556"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="33.969696969697"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="25.7171717171717"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="7.34848484848485"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="12.2929292929293"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="9.08585858585859"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="15.9040404040404"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="21.3787878787879"/>
-    <col collapsed="false" hidden="false" max="19" min="14" style="0" width="7.61616161616162"/>
-    <col collapsed="false" hidden="false" max="20" min="20" style="0" width="23.520202020202"/>
-    <col collapsed="false" hidden="false" max="1025" min="21" style="0" width="7.61616161616162"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="10.4242424242424"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="14.1666666666667"/>
+    <col collapsed="false" hidden="false" max="4" min="3" style="0" width="12.1616161616162"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="18.3080808080808"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="22.0505050505051"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="33.2727272727273"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="25.1212121212121"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="12.0252525252525"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="8.95454545454546"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="15.5"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="20.979797979798"/>
+    <col collapsed="false" hidden="false" max="19" min="14" style="0" width="7.34848484848485"/>
+    <col collapsed="false" hidden="false" max="20" min="20" style="0" width="22.9848484848485"/>
+    <col collapsed="false" hidden="false" max="1025" min="21" style="0" width="7.34848484848485"/>
   </cols>
   <sheetData>
     <row r="1" s="6" customFormat="true" ht="17.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -30741,7 +30779,7 @@
       <c r="V1" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="AMJ1" s="11"/>
+      <c r="AMJ1" s="7"/>
     </row>
     <row r="2" customFormat="false" ht="17.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="C2" s="3"/>
@@ -30887,17 +30925,17 @@
   <dimension ref="A1:E51"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B39" activeCellId="1" sqref="B40:C40 B39"/>
+      <selection pane="topLeft" activeCell="B39" activeCellId="0" sqref="B39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="18.9747474747475"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="24.7222222222222"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="27.0909090909091"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="37.6818181818182"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="56.1161616161616"/>
-    <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="7.61616161616162"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="18.5757575757576"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="24.1868686868687"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="26.459595959596"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="36.8838383838384"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="54.9191919191919"/>
+    <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="7.34848484848485"/>
   </cols>
   <sheetData>
     <row r="1" s="1" customFormat="true" ht="22.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -31002,10 +31040,10 @@
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B9" s="11"/>
-      <c r="C9" s="11"/>
-      <c r="D9" s="11"/>
-      <c r="E9" s="11"/>
+      <c r="B9" s="7"/>
+      <c r="C9" s="7"/>
+      <c r="D9" s="7"/>
+      <c r="E9" s="7"/>
     </row>
     <row r="10" customFormat="false" ht="14.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B10" s="9" t="s">
@@ -31386,10 +31424,10 @@
       </c>
     </row>
     <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B38" s="11"/>
-      <c r="C38" s="11"/>
-      <c r="D38" s="11"/>
-      <c r="E38" s="11"/>
+      <c r="B38" s="7"/>
+      <c r="C38" s="7"/>
+      <c r="D38" s="7"/>
+      <c r="E38" s="7"/>
     </row>
     <row r="39" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B39" s="9" t="s">
@@ -31575,30 +31613,30 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="1:39"/>
+  <dimension ref="1:54"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A17" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B40" activeCellId="0" sqref="B40:C40"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A34" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C46" activeCellId="0" sqref="C46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="17.6414141414141"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="19.9090909090909"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="38.0909090909091"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="18.1717171717172"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="30.469696969697"/>
-    <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="7.61616161616162"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="17.1060606060606"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="19.3737373737374"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="37.2828282828283"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="17.6414141414141"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="29.7979797979798"/>
+    <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="7.34848484848485"/>
   </cols>
   <sheetData>
     <row r="1" s="6" customFormat="true" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
         <v>181</v>
       </c>
-      <c r="B1" s="13" t="s">
+      <c r="B1" s="12" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="13" t="s">
+      <c r="C1" s="12" t="s">
         <v>24</v>
       </c>
       <c r="AMJ1" s="0"/>
@@ -31896,6 +31934,126 @@
       </c>
       <c r="C39" s="3" t="s">
         <v>212</v>
+      </c>
+    </row>
+    <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B40" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="C40" s="3" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B41" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="C41" s="3" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B42" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="C42" s="3" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B43" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="C43" s="3" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B44" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="C44" s="3" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B45" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="C45" s="3" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B46" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="C46" s="3" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B47" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="C47" s="3" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B48" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="C48" s="3" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B49" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="C49" s="3" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B50" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="C50" s="3" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="51" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B51" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="C51" s="3" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="52" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B52" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="C52" s="3" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="53" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B53" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="C53" s="3" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="54" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B54" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="C54" s="3" t="s">
+        <v>227</v>
       </c>
     </row>
   </sheetData>
@@ -31917,19 +32075,19 @@
   <dimension ref="A1:B1"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B6" activeCellId="1" sqref="B40:C40 B6"/>
+      <selection pane="topLeft" activeCell="B6" activeCellId="0" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="18.4393939393939"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="29.2626262626263"/>
-    <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="7.61616161616162"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="18.040404040404"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="28.5959595959596"/>
+    <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="7.34848484848485"/>
   </cols>
   <sheetData>
     <row r="1" s="2" customFormat="true" ht="13.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
-        <v>213</v>
+        <v>228</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>52</v>

</xml_diff>

<commit_message>
completes section 8 structure with all prompts, choices, and flow control
</commit_message>
<xml_diff>
--- a/tables/actor/forms/actor/actor.xlsx
+++ b/tables/actor/forms/actor/actor.xlsx
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="391" uniqueCount="229">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="431" uniqueCount="249">
   <si>
     <t xml:space="preserve">clause</t>
   </si>
@@ -1361,6 +1361,66 @@
     <t xml:space="preserve">causedProblems</t>
   </si>
   <si>
+    <t xml:space="preserve">expectationsDestination</t>
+  </si>
+  <si>
+    <t xml:space="preserve">expectationsWorkType</t>
+  </si>
+  <si>
+    <t xml:space="preserve">expectationsJobSite</t>
+  </si>
+  <si>
+    <t xml:space="preserve">expectationsCompanyName</t>
+  </si>
+  <si>
+    <t xml:space="preserve">expectationsLivingArrangements</t>
+  </si>
+  <si>
+    <t xml:space="preserve">expectationsAmountPaid</t>
+  </si>
+  <si>
+    <t xml:space="preserve">expectationsOftenPaid</t>
+  </si>
+  <si>
+    <t xml:space="preserve">expectationsWorkingHours</t>
+  </si>
+  <si>
+    <t xml:space="preserve">expectationsOvertimeHours</t>
+  </si>
+  <si>
+    <t xml:space="preserve">expectationsOvertimePay</t>
+  </si>
+  <si>
+    <t xml:space="preserve">expectationsTimeOff</t>
+  </si>
+  <si>
+    <t xml:space="preserve">expectationsLawfulDeductions</t>
+  </si>
+  <si>
+    <t xml:space="preserve">expectationsForeignWorkerRights</t>
+  </si>
+  <si>
+    <t xml:space="preserve">expectationsContractDuration</t>
+  </si>
+  <si>
+    <t xml:space="preserve">expectationsEarlyTerminationPenalties</t>
+  </si>
+  <si>
+    <t xml:space="preserve">expectationsRecruitmentFees</t>
+  </si>
+  <si>
+    <t xml:space="preserve">expectationsTransportationCosts</t>
+  </si>
+  <si>
+    <t xml:space="preserve">expectationsTransportationPlan</t>
+  </si>
+  <si>
+    <t xml:space="preserve">expectationsTransportationDocumentationPlan</t>
+  </si>
+  <si>
+    <t xml:space="preserve">expectationsTransportationDocumentationCosts</t>
+  </si>
+  <si>
     <t xml:space="preserve">calculation_name</t>
   </si>
 </sst>
@@ -1547,9 +1607,11 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="16.0353535353535"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="20.4444444444444"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="45.1666666666667"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="15.6363636363636"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="8.41919191919192"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="19.9090909090909"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="44.0959595959596"/>
+    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="8.41919191919192"/>
   </cols>
   <sheetData>
     <row r="1" s="2" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1606,13 +1668,11 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="15.6363636363636"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="15.1010101010101"/>
-    <col collapsed="false" hidden="false" max="4" min="3" style="0" width="21.3787878787879"/>
-    <col collapsed="false" hidden="false" max="7" min="5" style="0" width="7.34848484848485"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="23.3838383838384"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="23.2525252525253"/>
-    <col collapsed="false" hidden="false" max="1025" min="10" style="0" width="7.34848484848485"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="15.2323232323232"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="14.6969696969697"/>
+    <col collapsed="false" hidden="false" max="4" min="3" style="0" width="20.979797979798"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="22.8484848484848"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="22.7171717171717"/>
   </cols>
   <sheetData>
     <row r="1" s="2" customFormat="true" ht="18.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1738,11 +1798,11 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="3" width="34.4747474747475"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="3" width="52.6515151515152"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="3" width="53.1818181818182"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="3" width="89.7979797979798"/>
-    <col collapsed="false" hidden="false" max="1025" min="5" style="3" width="5.21212121212121"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="3" width="33.6767676767677"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="3" width="51.5808080808081"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="3" width="51.979797979798"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="3" width="87.9292929292929"/>
+    <col collapsed="false" hidden="false" max="1025" min="5" style="3" width="4.94444444444444"/>
   </cols>
   <sheetData>
     <row r="1" s="1" customFormat="true" ht="14.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -30696,20 +30756,19 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="10.4242424242424"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="14.1666666666667"/>
-    <col collapsed="false" hidden="false" max="4" min="3" style="0" width="12.1616161616162"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="18.3080808080808"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="22.0505050505051"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="33.2727272727273"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="25.1212121212121"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="12.0252525252525"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="8.95454545454546"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="15.5"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="20.979797979798"/>
-    <col collapsed="false" hidden="false" max="19" min="14" style="0" width="7.34848484848485"/>
-    <col collapsed="false" hidden="false" max="20" min="20" style="0" width="22.9848484848485"/>
-    <col collapsed="false" hidden="false" max="1025" min="21" style="0" width="7.34848484848485"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="10.1565656565657"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="13.7626262626263"/>
+    <col collapsed="false" hidden="false" max="4" min="3" style="0" width="11.7575757575758"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="17.9040404040404"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="21.5151515151515"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="32.469696969697"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="24.5858585858586"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="8.41919191919192"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="11.6262626262626"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="8.68686868686869"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="15.1010101010101"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="20.4444444444444"/>
+    <col collapsed="false" hidden="false" max="20" min="20" style="0" width="22.4494949494949"/>
   </cols>
   <sheetData>
     <row r="1" s="6" customFormat="true" ht="17.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -30930,12 +30989,11 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="18.5757575757576"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="24.1868686868687"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="26.459595959596"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="36.8838383838384"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="54.9191919191919"/>
-    <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="7.34848484848485"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="18.1717171717172"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="23.520202020202"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="25.7878787878788"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="36.0808080808081"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="53.7171717171717"/>
   </cols>
   <sheetData>
     <row r="1" s="1" customFormat="true" ht="22.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -31613,20 +31671,19 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="1:54"/>
+  <dimension ref="1:75"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A34" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="C46" activeCellId="0" sqref="C46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="17.1060606060606"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="19.3737373737374"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="37.2828282828283"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="17.6414141414141"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="29.7979797979798"/>
-    <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="7.34848484848485"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="16.7020202020202"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="18.9747474747475"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="42.8939393939394"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="17.1060606060606"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="29.1313131313131"/>
   </cols>
   <sheetData>
     <row r="1" s="6" customFormat="true" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -32054,6 +32111,166 @@
       </c>
       <c r="C54" s="3" t="s">
         <v>227</v>
+      </c>
+    </row>
+    <row r="56" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B56" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="C56" s="3" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="57" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B57" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="C57" s="3" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="58" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B58" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="C58" s="3" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="59" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B59" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="C59" s="3" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="60" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B60" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="C60" s="3" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="61" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B61" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="C61" s="3" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="62" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B62" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="C62" s="3" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="63" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B63" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="C63" s="3" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="64" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B64" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="C64" s="3" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="65" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B65" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="C65" s="3" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="66" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B66" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="C66" s="3" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="67" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B67" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="C67" s="3" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="68" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B68" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="C68" s="3" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="69" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B69" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="C69" s="3" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="70" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B70" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="C70" s="3" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="71" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B71" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="C71" s="3" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="72" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B72" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="C72" s="3" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="73" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B73" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="C73" s="3" t="s">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="74" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B74" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="C74" s="3" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="75" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B75" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="C75" s="3" t="s">
+        <v>247</v>
       </c>
     </row>
   </sheetData>
@@ -32080,14 +32297,13 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="18.040404040404"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="28.5959595959596"/>
-    <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="7.34848484848485"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="17.5050505050505"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="27.9292929292929"/>
   </cols>
   <sheetData>
     <row r="1" s="2" customFormat="true" ht="13.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
-        <v>228</v>
+        <v>248</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>52</v>

</xml_diff>

<commit_message>
rough section 9 structure with top level prompts and choices
</commit_message>
<xml_diff>
--- a/tables/actor/forms/actor/actor.xlsx
+++ b/tables/actor/forms/actor/actor.xlsx
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="431" uniqueCount="249">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="471" uniqueCount="269">
   <si>
     <t xml:space="preserve">clause</t>
   </si>
@@ -1419,6 +1419,66 @@
   </si>
   <si>
     <t xml:space="preserve">expectationsTransportationDocumentationCosts</t>
+  </si>
+  <si>
+    <t xml:space="preserve">deductions</t>
+  </si>
+  <si>
+    <t xml:space="preserve">lockedInRoom</t>
+  </si>
+  <si>
+    <t xml:space="preserve">refusedOvertimePay</t>
+  </si>
+  <si>
+    <t xml:space="preserve">limitedBreaks</t>
+  </si>
+  <si>
+    <t xml:space="preserve">workWhenSick</t>
+  </si>
+  <si>
+    <t xml:space="preserve">dangerousWork</t>
+  </si>
+  <si>
+    <t xml:space="preserve">workedLonger</t>
+  </si>
+  <si>
+    <t xml:space="preserve">restrictedMovement</t>
+  </si>
+  <si>
+    <t xml:space="preserve">threatenNoPay</t>
+  </si>
+  <si>
+    <t xml:space="preserve">threatenDismissal</t>
+  </si>
+  <si>
+    <t xml:space="preserve">takenPassport</t>
+  </si>
+  <si>
+    <t xml:space="preserve">threatenInjury</t>
+  </si>
+  <si>
+    <t xml:space="preserve">damagedBelongings</t>
+  </si>
+  <si>
+    <t xml:space="preserve">slappedHitThrowSomething</t>
+  </si>
+  <si>
+    <t xml:space="preserve">pushedKickedBeaten</t>
+  </si>
+  <si>
+    <t xml:space="preserve">tiedUpChoked</t>
+  </si>
+  <si>
+    <t xml:space="preserve">threatenWeaponUse</t>
+  </si>
+  <si>
+    <t xml:space="preserve">burnYou</t>
+  </si>
+  <si>
+    <t xml:space="preserve">forcedSex</t>
+  </si>
+  <si>
+    <t xml:space="preserve">forcedSubstances</t>
   </si>
   <si>
     <t xml:space="preserve">calculation_name</t>
@@ -31671,10 +31731,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="1:75"/>
+  <dimension ref="1:96"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C46" activeCellId="0" sqref="C46"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A78" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B98" activeCellId="0" sqref="B98"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -32271,6 +32331,166 @@
       </c>
       <c r="C75" s="3" t="s">
         <v>247</v>
+      </c>
+    </row>
+    <row r="77" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B77" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="C77" s="3" t="s">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="78" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B78" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="C78" s="3" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="79" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B79" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="C79" s="3" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="80" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B80" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="C80" s="3" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="81" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B81" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="C81" s="3" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="82" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B82" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="C82" s="3" t="s">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="83" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B83" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="C83" s="3" t="s">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="84" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B84" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="C84" s="3" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="85" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B85" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="C85" s="3" t="s">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="86" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B86" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="C86" s="3" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="87" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B87" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="C87" s="3" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="88" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B88" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="C88" s="3" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="89" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B89" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="C89" s="3" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="90" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B90" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="C90" s="3" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="91" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B91" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="C91" s="3" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="92" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B92" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="C92" s="3" t="s">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="93" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B93" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="C93" s="3" t="s">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="94" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B94" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="C94" s="3" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="95" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B95" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="C95" s="3" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="96" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B96" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="C96" s="3" t="s">
+        <v>267</v>
       </c>
     </row>
   </sheetData>
@@ -32303,7 +32523,7 @@
   <sheetData>
     <row r="1" s="2" customFormat="true" ht="13.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
-        <v>248</v>
+        <v>268</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>52</v>

</xml_diff>

<commit_message>
removes age answer options for actors
</commit_message>
<xml_diff>
--- a/tables/actor/forms/actor/actor.xlsx
+++ b/tables/actor/forms/actor/actor.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="988" firstSheet="0" activeTab="2"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="988" firstSheet="0" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="initial" sheetId="1" state="visible" r:id="rId2"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="549" uniqueCount="301">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="519" uniqueCount="295">
   <si>
     <t xml:space="preserve">clause</t>
   </si>
@@ -669,24 +669,6 @@
     <t xml:space="preserve">end if</t>
   </si>
   <si>
-    <t xml:space="preserve">calculates.age_is_birth_year_myanmar()</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ageBirthYearMyanmar</t>
-  </si>
-  <si>
-    <t xml:space="preserve">calculates.age_is_birth_year_thailand()</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ageBirthYearThailand</t>
-  </si>
-  <si>
-    <t xml:space="preserve">calculates.age_is_birth_year_english()</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ageBirthYearEnglish</t>
-  </si>
-  <si>
     <t xml:space="preserve">gender</t>
   </si>
   <si>
@@ -730,15 +712,6 @@
   </si>
   <si>
     <t xml:space="preserve">approximate age</t>
-  </si>
-  <si>
-    <t xml:space="preserve">birth year myanmar</t>
-  </si>
-  <si>
-    <t xml:space="preserve">birth year thailand</t>
-  </si>
-  <si>
-    <t xml:space="preserve">birth year english</t>
   </si>
   <si>
     <t xml:space="preserve">don't know</t>
@@ -1292,6 +1265,15 @@
     <t xml:space="preserve">migrantId</t>
   </si>
   <si>
+    <t xml:space="preserve">ageBirthYearMyanmar</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ageBirthYearThailand</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ageBirthYearEnglish</t>
+  </si>
+  <si>
     <t xml:space="preserve">firstSuggestion</t>
   </si>
   <si>
@@ -1766,11 +1748,11 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="14.9646464646465"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="7.88383838383838"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="18.9747474747475"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="42.2272727272727"/>
-    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="7.88383838383838"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="14.5656565656566"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="7.61616161616162"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="18.5757575757576"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="41.2929292929293"/>
+    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="7.61616161616162"/>
   </cols>
   <sheetData>
     <row r="1" s="2" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1827,13 +1809,12 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="14.5656565656566"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="13.8989898989899"/>
-    <col collapsed="false" hidden="false" max="4" min="3" style="0" width="19.9090909090909"/>
-    <col collapsed="false" hidden="false" max="7" min="5" style="0" width="8.15151515151515"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="21.7828282828283"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="21.6464646464646"/>
-    <col collapsed="false" hidden="false" max="1025" min="10" style="0" width="8.15151515151515"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="14.1666666666667"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="13.4949494949495"/>
+    <col collapsed="false" hidden="false" max="4" min="3" style="0" width="19.3737373737374"/>
+    <col collapsed="false" hidden="false" max="7" min="5" style="0" width="7.88383838383838"/>
+    <col collapsed="false" hidden="false" max="9" min="8" style="0" width="21.2474747474747"/>
+    <col collapsed="false" hidden="false" max="1025" min="10" style="0" width="7.88383838383838"/>
   </cols>
   <sheetData>
     <row r="1" s="2" customFormat="true" ht="18.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1953,17 +1934,17 @@
   </sheetPr>
   <dimension ref="1:65"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="C18" activeCellId="0" sqref="C18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="3" width="32.2020202020202"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="3" width="49.3080808080808"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="3" width="49.7121212121212"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="3" width="84.0505050505051"/>
-    <col collapsed="false" hidden="false" max="1025" min="5" style="3" width="4.67676767676768"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="3" width="31.4040404040404"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="3" width="48.2373737373737"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="3" width="48.6414141414141"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="3" width="82.1818181818182"/>
+    <col collapsed="false" hidden="false" max="1025" min="5" style="3" width="4.54545454545455"/>
   </cols>
   <sheetData>
     <row r="1" s="1" customFormat="true" ht="14.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -37101,30 +37082,30 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="1:28"/>
+  <dimension ref="1:19"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A10" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E25" activeCellId="0" sqref="E25"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D21" activeCellId="0" sqref="D21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="9.62121212121212"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="13.0959595959596"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="11.0909090909091"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="39.4191919191919"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="22.9646464646465"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="20.5808080808081"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="31"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="23.3838383838384"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="7.88383838383838"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="10.959595959596"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="8.15151515151515"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="14.2979797979798"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="19.3737373737374"/>
-    <col collapsed="false" hidden="false" max="19" min="14" style="0" width="8.15151515151515"/>
-    <col collapsed="false" hidden="false" max="20" min="20" style="0" width="21.3787878787879"/>
-    <col collapsed="false" hidden="false" max="1025" min="21" style="0" width="8.15151515151515"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="9.35353535353535"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="12.8282828282828"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="10.8232323232323"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="38.4848484848485"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="22.4494949494949"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="20.0454545454545"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="30.3333333333333"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="22.8484848484848"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="7.61616161616162"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="10.6919191919192"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="7.88383838383838"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="13.8989898989899"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="18.9747474747475"/>
+    <col collapsed="false" hidden="false" max="19" min="14" style="0" width="7.88383838383838"/>
+    <col collapsed="false" hidden="false" max="20" min="20" style="0" width="20.979797979798"/>
+    <col collapsed="false" hidden="false" max="1025" min="21" style="0" width="7.88383838383838"/>
   </cols>
   <sheetData>
     <row r="1" s="6" customFormat="true" ht="17.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -37294,219 +37275,117 @@
       <c r="I8" s="3"/>
       <c r="L8" s="3"/>
     </row>
-    <row r="9" customFormat="false" ht="21.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C9" s="7" t="s">
+    <row r="9" customFormat="false" ht="20.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="E9" s="9" t="s">
+        <v>46</v>
+      </c>
+      <c r="F9" s="3" t="s">
+        <v>80</v>
+      </c>
+      <c r="G9" s="7" t="s">
+        <v>87</v>
+      </c>
+      <c r="H9" s="7" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C10" s="7" t="s">
         <v>82</v>
       </c>
-      <c r="D9" s="7" t="s">
-        <v>87</v>
-      </c>
-      <c r="E9" s="8"/>
-      <c r="F9" s="7"/>
-      <c r="I9" s="3"/>
-      <c r="L9" s="3"/>
+      <c r="D10" s="7" t="s">
+        <v>88</v>
+      </c>
+      <c r="E10" s="8"/>
     </row>
-    <row r="10" customFormat="false" ht="21.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="E10" s="9" t="s">
-        <v>37</v>
-      </c>
-      <c r="F10" s="7" t="s">
-        <v>84</v>
-      </c>
-      <c r="G10" s="7" t="s">
-        <v>88</v>
-      </c>
-      <c r="I10" s="3"/>
-      <c r="L10" s="3"/>
+    <row r="11" customFormat="false" ht="14.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E11" s="9" t="s">
+        <v>49</v>
+      </c>
+      <c r="F11" s="7" t="s">
+        <v>79</v>
+      </c>
+      <c r="G11" s="7" t="s">
+        <v>89</v>
+      </c>
     </row>
-    <row r="11" customFormat="false" ht="21.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C11" s="7" t="s">
+    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C12" s="7" t="s">
         <v>86</v>
       </c>
-      <c r="E11" s="8"/>
-      <c r="F11" s="7"/>
-      <c r="I11" s="3"/>
-      <c r="L11" s="3"/>
+      <c r="E12" s="8"/>
     </row>
-    <row r="12" customFormat="false" ht="21.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C12" s="7" t="s">
+    <row r="13" customFormat="false" ht="17.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="E13" s="9" t="s">
+        <v>52</v>
+      </c>
+      <c r="F13" s="3" t="s">
+        <v>90</v>
+      </c>
+      <c r="G13" s="7" t="s">
+        <v>91</v>
+      </c>
+      <c r="H13" s="7" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C14" s="7" t="s">
         <v>82</v>
       </c>
-      <c r="D12" s="7" t="s">
-        <v>89</v>
-      </c>
-      <c r="E12" s="8"/>
-      <c r="F12" s="7"/>
-      <c r="I12" s="3"/>
-      <c r="L12" s="3"/>
+      <c r="D14" s="7" t="s">
+        <v>92</v>
+      </c>
+      <c r="E14" s="8"/>
     </row>
-    <row r="13" customFormat="false" ht="21.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="E13" s="9" t="s">
-        <v>40</v>
-      </c>
-      <c r="F13" s="7" t="s">
-        <v>84</v>
-      </c>
-      <c r="G13" s="7" t="s">
-        <v>90</v>
-      </c>
-      <c r="I13" s="3"/>
-      <c r="L13" s="3"/>
+    <row r="15" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E15" s="9" t="s">
+        <v>55</v>
+      </c>
+      <c r="F15" s="7" t="s">
+        <v>79</v>
+      </c>
+      <c r="G15" s="7" t="s">
+        <v>93</v>
+      </c>
     </row>
-    <row r="14" customFormat="false" ht="21.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C14" s="7" t="s">
+    <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C16" s="7" t="s">
         <v>86</v>
       </c>
-      <c r="E14" s="8"/>
-      <c r="F14" s="7"/>
-      <c r="I14" s="3"/>
-      <c r="L14" s="3"/>
+      <c r="E16" s="8"/>
     </row>
-    <row r="15" customFormat="false" ht="21.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C15" s="7" t="s">
-        <v>82</v>
-      </c>
-      <c r="D15" s="7" t="s">
-        <v>91</v>
-      </c>
-      <c r="E15" s="8"/>
-      <c r="F15" s="7"/>
-      <c r="I15" s="3"/>
-      <c r="L15" s="3"/>
+    <row r="17" customFormat="false" ht="17.2" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="E17" s="9" t="s">
+        <v>56</v>
+      </c>
+      <c r="F17" s="3" t="s">
+        <v>80</v>
+      </c>
+      <c r="G17" s="7" t="s">
+        <v>94</v>
+      </c>
+      <c r="H17" s="9" t="s">
+        <v>95</v>
+      </c>
     </row>
-    <row r="16" customFormat="false" ht="21.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="E16" s="9" t="s">
-        <v>43</v>
-      </c>
-      <c r="F16" s="7" t="s">
-        <v>84</v>
-      </c>
-      <c r="G16" s="7" t="s">
-        <v>92</v>
-      </c>
-      <c r="I16" s="3"/>
-      <c r="L16" s="3"/>
-    </row>
-    <row r="17" customFormat="false" ht="21.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C17" s="7" t="s">
-        <v>86</v>
-      </c>
-      <c r="E17" s="8"/>
-      <c r="F17" s="7"/>
-      <c r="I17" s="3"/>
-      <c r="L17" s="3"/>
-    </row>
-    <row r="18" customFormat="false" ht="20.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="18" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E18" s="9" t="s">
-        <v>46</v>
+        <v>59</v>
       </c>
       <c r="F18" s="3" t="s">
         <v>80</v>
       </c>
       <c r="G18" s="7" t="s">
-        <v>93</v>
+        <v>96</v>
       </c>
       <c r="H18" s="7" t="s">
-        <v>93</v>
+        <v>97</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C19" s="7" t="s">
-        <v>82</v>
-      </c>
-      <c r="D19" s="7" t="s">
-        <v>94</v>
-      </c>
-      <c r="E19" s="8"/>
-    </row>
-    <row r="20" customFormat="false" ht="14.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E20" s="9" t="s">
-        <v>49</v>
-      </c>
-      <c r="F20" s="7" t="s">
-        <v>79</v>
-      </c>
-      <c r="G20" s="7" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C21" s="7" t="s">
-        <v>86</v>
-      </c>
-      <c r="E21" s="8"/>
-    </row>
-    <row r="22" customFormat="false" ht="17.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="E22" s="9" t="s">
-        <v>52</v>
-      </c>
-      <c r="F22" s="3" t="s">
-        <v>96</v>
-      </c>
-      <c r="G22" s="7" t="s">
-        <v>97</v>
-      </c>
-      <c r="H22" s="7" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C23" s="7" t="s">
-        <v>82</v>
-      </c>
-      <c r="D23" s="7" t="s">
+      <c r="C19" s="3" t="s">
         <v>98</v>
-      </c>
-      <c r="E23" s="8"/>
-    </row>
-    <row r="24" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E24" s="9" t="s">
-        <v>55</v>
-      </c>
-      <c r="F24" s="7" t="s">
-        <v>79</v>
-      </c>
-      <c r="G24" s="7" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C25" s="7" t="s">
-        <v>86</v>
-      </c>
-      <c r="E25" s="8"/>
-    </row>
-    <row r="26" customFormat="false" ht="17.2" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="E26" s="9" t="s">
-        <v>56</v>
-      </c>
-      <c r="F26" s="3" t="s">
-        <v>80</v>
-      </c>
-      <c r="G26" s="7" t="s">
-        <v>100</v>
-      </c>
-      <c r="H26" s="9" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="27" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E27" s="9" t="s">
-        <v>59</v>
-      </c>
-      <c r="F27" s="3" t="s">
-        <v>80</v>
-      </c>
-      <c r="G27" s="7" t="s">
-        <v>102</v>
-      </c>
-      <c r="H27" s="7" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C28" s="3" t="s">
-        <v>104</v>
       </c>
     </row>
   </sheetData>
@@ -37525,20 +37404,20 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:E51"/>
+  <dimension ref="A1:E48"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E6" activeCellId="0" sqref="E6"/>
+      <selection pane="topLeft" activeCell="A4" activeCellId="0" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="17.1060606060606"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="25.9242424242424"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="24.7222222222222"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="34.4747474747475"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="51.4444444444444"/>
-    <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="8.15151515151515"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="16.7020202020202"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="25.2575757575758"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="24.1868686868687"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="33.6767676767677"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="50.2424242424242"/>
+    <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="7.88383838383838"/>
   </cols>
   <sheetData>
     <row r="1" s="1" customFormat="true" ht="22.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -37546,10 +37425,10 @@
         <v>3</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>105</v>
+        <v>99</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>106</v>
+        <v>100</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>10</v>
@@ -37563,7 +37442,7 @@
         <v>81</v>
       </c>
       <c r="C3" s="9" t="s">
-        <v>107</v>
+        <v>101</v>
       </c>
       <c r="D3" s="9" t="s">
         <v>35</v>
@@ -37572,18 +37451,18 @@
         <v>36</v>
       </c>
     </row>
-    <row r="4" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="4" customFormat="false" ht="15.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B4" s="9" t="s">
         <v>81</v>
       </c>
       <c r="C4" s="9" t="s">
-        <v>108</v>
+        <v>102</v>
       </c>
       <c r="D4" s="9" t="s">
-        <v>38</v>
+        <v>103</v>
       </c>
       <c r="E4" s="8" t="s">
-        <v>39</v>
+        <v>104</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="16.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -37591,450 +37470,450 @@
         <v>81</v>
       </c>
       <c r="C5" s="9" t="s">
+        <v>105</v>
+      </c>
+      <c r="D5" s="9" t="s">
+        <v>106</v>
+      </c>
+      <c r="E5" s="8" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B6" s="7"/>
+      <c r="C6" s="7"/>
+      <c r="D6" s="7"/>
+      <c r="E6" s="7"/>
+    </row>
+    <row r="7" customFormat="false" ht="14.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B7" s="9" t="s">
+        <v>87</v>
+      </c>
+      <c r="C7" s="9" t="s">
+        <v>108</v>
+      </c>
+      <c r="D7" s="9" t="s">
         <v>109</v>
       </c>
-      <c r="D5" s="9" t="s">
-        <v>41</v>
-      </c>
-      <c r="E5" s="8" t="s">
-        <v>42</v>
+      <c r="E7" s="8" t="s">
+        <v>110</v>
       </c>
     </row>
-    <row r="6" customFormat="false" ht="18.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B6" s="9" t="s">
-        <v>81</v>
-      </c>
-      <c r="C6" s="9" t="s">
-        <v>110</v>
-      </c>
-      <c r="D6" s="9" t="s">
-        <v>44</v>
-      </c>
-      <c r="E6" s="8" t="s">
-        <v>45</v>
+    <row r="8" customFormat="false" ht="14.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B8" s="9" t="s">
+        <v>87</v>
+      </c>
+      <c r="C8" s="9" t="s">
+        <v>111</v>
+      </c>
+      <c r="D8" s="9" t="s">
+        <v>112</v>
+      </c>
+      <c r="E8" s="8" t="s">
+        <v>113</v>
       </c>
     </row>
-    <row r="7" customFormat="false" ht="15.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B7" s="9" t="s">
-        <v>81</v>
-      </c>
-      <c r="C7" s="9" t="s">
-        <v>111</v>
-      </c>
-      <c r="D7" s="9" t="s">
-        <v>112</v>
-      </c>
-      <c r="E7" s="8" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="8" customFormat="false" ht="16.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B8" s="9" t="s">
-        <v>81</v>
-      </c>
-      <c r="C8" s="9" t="s">
+    <row r="9" customFormat="false" ht="14.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B9" s="9" t="s">
+        <v>87</v>
+      </c>
+      <c r="C9" s="9" t="s">
         <v>114</v>
       </c>
-      <c r="D8" s="9" t="s">
-        <v>115</v>
-      </c>
-      <c r="E8" s="8" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B9" s="7"/>
-      <c r="C9" s="7"/>
-      <c r="D9" s="7"/>
-      <c r="E9" s="7"/>
+      <c r="D9" s="9" t="s">
+        <v>50</v>
+      </c>
+      <c r="E9" s="8" t="s">
+        <v>51</v>
+      </c>
     </row>
     <row r="10" customFormat="false" ht="14.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B10" s="9" t="s">
-        <v>93</v>
+        <v>87</v>
       </c>
       <c r="C10" s="9" t="s">
+        <v>105</v>
+      </c>
+      <c r="D10" s="9" t="s">
+        <v>106</v>
+      </c>
+      <c r="E10" s="8" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B12" s="9" t="s">
+        <v>91</v>
+      </c>
+      <c r="C12" s="9" t="s">
+        <v>115</v>
+      </c>
+      <c r="D12" s="9" t="s">
+        <v>115</v>
+      </c>
+      <c r="E12" s="9" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="13.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B13" s="9" t="s">
+        <v>91</v>
+      </c>
+      <c r="C13" s="9" t="s">
         <v>117</v>
       </c>
-      <c r="D10" s="9" t="s">
+      <c r="D13" s="9" t="s">
         <v>118</v>
       </c>
-      <c r="E10" s="8" t="s">
+      <c r="E13" s="8" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="11" customFormat="false" ht="14.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B11" s="9" t="s">
-        <v>93</v>
-      </c>
-      <c r="C11" s="9" t="s">
+    <row r="14" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B14" s="9" t="s">
+        <v>91</v>
+      </c>
+      <c r="C14" s="9" t="s">
         <v>120</v>
       </c>
-      <c r="D11" s="9" t="s">
+      <c r="D14" s="9" t="s">
+        <v>120</v>
+      </c>
+      <c r="E14" s="8" t="s">
         <v>121</v>
-      </c>
-      <c r="E11" s="8" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="12" customFormat="false" ht="14.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B12" s="9" t="s">
-        <v>93</v>
-      </c>
-      <c r="C12" s="9" t="s">
-        <v>123</v>
-      </c>
-      <c r="D12" s="9" t="s">
-        <v>50</v>
-      </c>
-      <c r="E12" s="8" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="13" customFormat="false" ht="14.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B13" s="9" t="s">
-        <v>93</v>
-      </c>
-      <c r="C13" s="9" t="s">
-        <v>114</v>
-      </c>
-      <c r="D13" s="9" t="s">
-        <v>115</v>
-      </c>
-      <c r="E13" s="8" t="s">
-        <v>116</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B15" s="9" t="s">
-        <v>97</v>
+        <v>91</v>
       </c>
       <c r="C15" s="9" t="s">
+        <v>122</v>
+      </c>
+      <c r="D15" s="9" t="s">
+        <v>122</v>
+      </c>
+      <c r="E15" s="8" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B16" s="9" t="s">
+        <v>91</v>
+      </c>
+      <c r="C16" s="9" t="s">
         <v>124</v>
       </c>
-      <c r="D15" s="9" t="s">
+      <c r="D16" s="9" t="s">
         <v>124</v>
       </c>
-      <c r="E15" s="9" t="s">
+      <c r="E16" s="8" t="s">
         <v>125</v>
-      </c>
-    </row>
-    <row r="16" customFormat="false" ht="13.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B16" s="9" t="s">
-        <v>97</v>
-      </c>
-      <c r="C16" s="9" t="s">
-        <v>126</v>
-      </c>
-      <c r="D16" s="9" t="s">
-        <v>127</v>
-      </c>
-      <c r="E16" s="8" t="s">
-        <v>128</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B17" s="9" t="s">
-        <v>97</v>
+        <v>91</v>
       </c>
       <c r="C17" s="9" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="D17" s="9" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="E17" s="8" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B18" s="9" t="s">
-        <v>97</v>
+        <v>91</v>
       </c>
       <c r="C18" s="9" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="D18" s="9" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="E18" s="8" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B19" s="9" t="s">
-        <v>97</v>
+        <v>91</v>
       </c>
       <c r="C19" s="9" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="D19" s="9" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="E19" s="8" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B20" s="9" t="s">
-        <v>97</v>
+        <v>91</v>
       </c>
       <c r="C20" s="9" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="D20" s="9" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="E20" s="8" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B21" s="9" t="s">
-        <v>97</v>
+        <v>91</v>
       </c>
       <c r="C21" s="9" t="s">
+        <v>134</v>
+      </c>
+      <c r="D21" s="9" t="s">
+        <v>134</v>
+      </c>
+      <c r="E21" s="8" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="22" customFormat="false" ht="14.2" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B22" s="9" t="s">
+        <v>91</v>
+      </c>
+      <c r="C22" s="9" t="s">
+        <v>136</v>
+      </c>
+      <c r="D22" s="9" t="s">
+        <v>136</v>
+      </c>
+      <c r="E22" s="8" t="s">
         <v>137</v>
-      </c>
-      <c r="D21" s="9" t="s">
-        <v>137</v>
-      </c>
-      <c r="E21" s="8" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="22" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B22" s="9" t="s">
-        <v>97</v>
-      </c>
-      <c r="C22" s="9" t="s">
-        <v>139</v>
-      </c>
-      <c r="D22" s="9" t="s">
-        <v>139</v>
-      </c>
-      <c r="E22" s="8" t="s">
-        <v>140</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B23" s="9" t="s">
-        <v>97</v>
+        <v>91</v>
       </c>
       <c r="C23" s="9" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="D23" s="9" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="E23" s="8" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B24" s="9" t="s">
-        <v>97</v>
+        <v>91</v>
       </c>
       <c r="C24" s="9" t="s">
+        <v>140</v>
+      </c>
+      <c r="D24" s="9" t="s">
+        <v>141</v>
+      </c>
+      <c r="E24" s="8" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="25" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B25" s="9" t="s">
+        <v>91</v>
+      </c>
+      <c r="C25" s="9" t="s">
         <v>143</v>
       </c>
-      <c r="D24" s="9" t="s">
+      <c r="D25" s="9" t="s">
         <v>143</v>
       </c>
-      <c r="E24" s="8" t="s">
+      <c r="E25" s="8" t="s">
         <v>144</v>
-      </c>
-    </row>
-    <row r="25" customFormat="false" ht="14.2" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B25" s="9" t="s">
-        <v>97</v>
-      </c>
-      <c r="C25" s="9" t="s">
-        <v>145</v>
-      </c>
-      <c r="D25" s="9" t="s">
-        <v>145</v>
-      </c>
-      <c r="E25" s="8" t="s">
-        <v>146</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B26" s="9" t="s">
-        <v>97</v>
+        <v>91</v>
       </c>
       <c r="C26" s="9" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="D26" s="9" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="E26" s="8" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B27" s="9" t="s">
-        <v>97</v>
+        <v>91</v>
       </c>
       <c r="C27" s="9" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="D27" s="9" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
       <c r="E27" s="8" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B28" s="9" t="s">
-        <v>97</v>
+        <v>91</v>
       </c>
       <c r="C28" s="9" t="s">
+        <v>149</v>
+      </c>
+      <c r="D28" s="9" t="s">
+        <v>149</v>
+      </c>
+      <c r="E28" s="8" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="29" customFormat="false" ht="15.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B29" s="9" t="s">
+        <v>91</v>
+      </c>
+      <c r="C29" s="9" t="s">
+        <v>151</v>
+      </c>
+      <c r="D29" s="9" t="s">
+        <v>151</v>
+      </c>
+      <c r="E29" s="8" t="s">
         <v>152</v>
       </c>
-      <c r="D28" s="9" t="s">
-        <v>152</v>
-      </c>
-      <c r="E28" s="8" t="s">
+    </row>
+    <row r="30" customFormat="false" ht="16.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B30" s="9" t="s">
+        <v>91</v>
+      </c>
+      <c r="C30" s="9" t="s">
         <v>153</v>
       </c>
+      <c r="D30" s="9" t="s">
+        <v>154</v>
+      </c>
+      <c r="E30" s="8" t="s">
+        <v>155</v>
+      </c>
     </row>
-    <row r="29" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B29" s="9" t="s">
-        <v>97</v>
-      </c>
-      <c r="C29" s="9" t="s">
-        <v>154</v>
-      </c>
-      <c r="D29" s="9" t="s">
-        <v>154</v>
-      </c>
-      <c r="E29" s="8" t="s">
-        <v>155</v>
+    <row r="31" customFormat="false" ht="17.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B31" s="9" t="s">
+        <v>91</v>
+      </c>
+      <c r="C31" s="9" t="s">
+        <v>156</v>
+      </c>
+      <c r="D31" s="9" t="s">
+        <v>156</v>
+      </c>
+      <c r="E31" s="8" t="s">
+        <v>157</v>
       </c>
     </row>
-    <row r="30" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B30" s="9" t="s">
-        <v>97</v>
-      </c>
-      <c r="C30" s="9" t="s">
-        <v>156</v>
-      </c>
-      <c r="D30" s="9" t="s">
-        <v>156</v>
-      </c>
-      <c r="E30" s="8" t="s">
-        <v>157</v>
+    <row r="32" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B32" s="9" t="s">
+        <v>91</v>
+      </c>
+      <c r="C32" s="9" t="s">
+        <v>158</v>
+      </c>
+      <c r="D32" s="9" t="s">
+        <v>158</v>
+      </c>
+      <c r="E32" s="8" t="s">
+        <v>159</v>
       </c>
     </row>
-    <row r="31" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B31" s="9" t="s">
-        <v>97</v>
-      </c>
-      <c r="C31" s="9" t="s">
-        <v>158</v>
-      </c>
-      <c r="D31" s="9" t="s">
-        <v>158</v>
-      </c>
-      <c r="E31" s="8" t="s">
-        <v>159</v>
+    <row r="33" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B33" s="9" t="s">
+        <v>91</v>
+      </c>
+      <c r="C33" s="9" t="s">
+        <v>114</v>
+      </c>
+      <c r="D33" s="9" t="s">
+        <v>50</v>
+      </c>
+      <c r="E33" s="8" t="s">
+        <v>51</v>
       </c>
     </row>
-    <row r="32" customFormat="false" ht="15.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B32" s="9" t="s">
-        <v>97</v>
-      </c>
-      <c r="C32" s="9" t="s">
-        <v>160</v>
-      </c>
-      <c r="D32" s="9" t="s">
-        <v>160</v>
-      </c>
-      <c r="E32" s="8" t="s">
-        <v>161</v>
+    <row r="34" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B34" s="9" t="s">
+        <v>91</v>
+      </c>
+      <c r="C34" s="9" t="s">
+        <v>105</v>
+      </c>
+      <c r="D34" s="9" t="s">
+        <v>106</v>
+      </c>
+      <c r="E34" s="8" t="s">
+        <v>107</v>
       </c>
     </row>
-    <row r="33" customFormat="false" ht="16.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B33" s="9" t="s">
-        <v>97</v>
-      </c>
-      <c r="C33" s="9" t="s">
-        <v>162</v>
-      </c>
-      <c r="D33" s="9" t="s">
-        <v>163</v>
-      </c>
-      <c r="E33" s="8" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="34" customFormat="false" ht="17.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B34" s="9" t="s">
-        <v>97</v>
-      </c>
-      <c r="C34" s="9" t="s">
-        <v>165</v>
-      </c>
-      <c r="D34" s="9" t="s">
-        <v>165</v>
-      </c>
-      <c r="E34" s="8" t="s">
-        <v>166</v>
-      </c>
-    </row>
-    <row r="35" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B35" s="9" t="s">
-        <v>97</v>
-      </c>
-      <c r="C35" s="9" t="s">
-        <v>167</v>
-      </c>
-      <c r="D35" s="9" t="s">
-        <v>167</v>
-      </c>
-      <c r="E35" s="8" t="s">
-        <v>168</v>
-      </c>
+    <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B35" s="7"/>
+      <c r="C35" s="7"/>
+      <c r="D35" s="7"/>
+      <c r="E35" s="7"/>
     </row>
     <row r="36" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B36" s="9" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="C36" s="9" t="s">
-        <v>123</v>
+        <v>160</v>
       </c>
       <c r="D36" s="9" t="s">
-        <v>50</v>
+        <v>161</v>
       </c>
       <c r="E36" s="8" t="s">
-        <v>51</v>
+        <v>162</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B37" s="9" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="C37" s="9" t="s">
-        <v>114</v>
+        <v>163</v>
       </c>
       <c r="D37" s="9" t="s">
-        <v>115</v>
+        <v>164</v>
       </c>
       <c r="E37" s="8" t="s">
-        <v>116</v>
+        <v>165</v>
       </c>
     </row>
-    <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B38" s="7"/>
-      <c r="C38" s="7"/>
-      <c r="D38" s="7"/>
-      <c r="E38" s="7"/>
+    <row r="38" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B38" s="9" t="s">
+        <v>95</v>
+      </c>
+      <c r="C38" s="9" t="s">
+        <v>166</v>
+      </c>
+      <c r="D38" s="9" t="s">
+        <v>167</v>
+      </c>
+      <c r="E38" s="8" t="s">
+        <v>168</v>
+      </c>
     </row>
     <row r="39" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B39" s="9" t="s">
-        <v>101</v>
+        <v>95</v>
       </c>
       <c r="C39" s="9" t="s">
         <v>169</v>
@@ -38048,7 +37927,7 @@
     </row>
     <row r="40" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B40" s="9" t="s">
-        <v>101</v>
+        <v>95</v>
       </c>
       <c r="C40" s="9" t="s">
         <v>172</v>
@@ -38060,51 +37939,51 @@
         <v>174</v>
       </c>
     </row>
-    <row r="41" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B41" s="9" t="s">
-        <v>101</v>
-      </c>
-      <c r="C41" s="9" t="s">
+    <row r="42" customFormat="false" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B42" s="9" t="s">
+        <v>97</v>
+      </c>
+      <c r="C42" s="9" t="s">
         <v>175</v>
       </c>
-      <c r="D41" s="9" t="s">
+      <c r="D42" s="9" t="s">
         <v>176</v>
       </c>
-      <c r="E41" s="8" t="s">
+      <c r="E42" s="8" t="s">
         <v>177</v>
       </c>
     </row>
-    <row r="42" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B42" s="9" t="s">
-        <v>101</v>
-      </c>
-      <c r="C42" s="9" t="s">
+    <row r="43" customFormat="false" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B43" s="9" t="s">
+        <v>97</v>
+      </c>
+      <c r="C43" s="9" t="s">
         <v>178</v>
       </c>
-      <c r="D42" s="9" t="s">
+      <c r="D43" s="9" t="s">
         <v>179</v>
       </c>
-      <c r="E42" s="8" t="s">
+      <c r="E43" s="8" t="s">
         <v>180</v>
       </c>
     </row>
-    <row r="43" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B43" s="9" t="s">
-        <v>101</v>
-      </c>
-      <c r="C43" s="9" t="s">
+    <row r="44" customFormat="false" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B44" s="9" t="s">
+        <v>97</v>
+      </c>
+      <c r="C44" s="9" t="s">
         <v>181</v>
       </c>
-      <c r="D43" s="9" t="s">
+      <c r="D44" s="9" t="s">
         <v>182</v>
       </c>
-      <c r="E43" s="8" t="s">
+      <c r="E44" s="8" t="s">
         <v>183</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B45" s="9" t="s">
-        <v>103</v>
+        <v>97</v>
       </c>
       <c r="C45" s="9" t="s">
         <v>184</v>
@@ -38118,7 +37997,7 @@
     </row>
     <row r="46" customFormat="false" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B46" s="9" t="s">
-        <v>103</v>
+        <v>97</v>
       </c>
       <c r="C46" s="9" t="s">
         <v>187</v>
@@ -38130,74 +38009,32 @@
         <v>189</v>
       </c>
     </row>
-    <row r="47" customFormat="false" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="47" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B47" s="9" t="s">
-        <v>103</v>
+        <v>97</v>
       </c>
       <c r="C47" s="9" t="s">
         <v>190</v>
       </c>
       <c r="D47" s="9" t="s">
+        <v>103</v>
+      </c>
+      <c r="E47" s="8" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="48" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B48" s="9" t="s">
+        <v>97</v>
+      </c>
+      <c r="C48" s="9" t="s">
         <v>191</v>
       </c>
-      <c r="E47" s="8" t="s">
-        <v>192</v>
-      </c>
-    </row>
-    <row r="48" customFormat="false" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B48" s="9" t="s">
-        <v>103</v>
-      </c>
-      <c r="C48" s="9" t="s">
-        <v>193</v>
-      </c>
       <c r="D48" s="9" t="s">
-        <v>194</v>
+        <v>106</v>
       </c>
       <c r="E48" s="8" t="s">
-        <v>195</v>
-      </c>
-    </row>
-    <row r="49" customFormat="false" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B49" s="9" t="s">
-        <v>103</v>
-      </c>
-      <c r="C49" s="9" t="s">
-        <v>196</v>
-      </c>
-      <c r="D49" s="9" t="s">
-        <v>197</v>
-      </c>
-      <c r="E49" s="8" t="s">
-        <v>198</v>
-      </c>
-    </row>
-    <row r="50" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B50" s="9" t="s">
-        <v>103</v>
-      </c>
-      <c r="C50" s="9" t="s">
-        <v>199</v>
-      </c>
-      <c r="D50" s="9" t="s">
-        <v>112</v>
-      </c>
-      <c r="E50" s="8" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="51" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B51" s="9" t="s">
-        <v>103</v>
-      </c>
-      <c r="C51" s="9" t="s">
-        <v>200</v>
-      </c>
-      <c r="D51" s="9" t="s">
-        <v>115</v>
-      </c>
-      <c r="E51" s="8" t="s">
-        <v>116</v>
+        <v>107</v>
       </c>
     </row>
   </sheetData>
@@ -38224,17 +38061,17 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="15.9040404040404"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="18.1717171717172"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="41.0252525252525"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="16.3030303030303"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="27.7929292929293"/>
-    <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="8.15151515151515"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="15.5"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="17.6414141414141"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="40.0909090909091"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="15.9040404040404"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="27.2626262626263"/>
+    <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="7.88383838383838"/>
   </cols>
   <sheetData>
     <row r="1" s="6" customFormat="true" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
-        <v>201</v>
+        <v>192</v>
       </c>
       <c r="B1" s="12" t="s">
         <v>1</v>
@@ -38246,13 +38083,13 @@
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="3" t="s">
-        <v>202</v>
+        <v>193</v>
       </c>
       <c r="B2" s="3" t="s">
         <v>79</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>203</v>
+        <v>194</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -38288,7 +38125,7 @@
         <v>84</v>
       </c>
       <c r="C7" s="7" t="s">
-        <v>88</v>
+        <v>195</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -38296,7 +38133,7 @@
         <v>84</v>
       </c>
       <c r="C8" s="7" t="s">
-        <v>90</v>
+        <v>196</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -38304,7 +38141,7 @@
         <v>84</v>
       </c>
       <c r="C9" s="7" t="s">
-        <v>92</v>
+        <v>197</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -38316,7 +38153,7 @@
         <v>80</v>
       </c>
       <c r="C11" s="7" t="s">
-        <v>93</v>
+        <v>87</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -38324,15 +38161,15 @@
         <v>79</v>
       </c>
       <c r="C12" s="7" t="s">
-        <v>95</v>
+        <v>89</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B13" s="3" t="s">
-        <v>96</v>
+        <v>90</v>
       </c>
       <c r="C13" s="7" t="s">
-        <v>97</v>
+        <v>91</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -38340,7 +38177,7 @@
         <v>79</v>
       </c>
       <c r="C14" s="7" t="s">
-        <v>99</v>
+        <v>93</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -38348,7 +38185,7 @@
         <v>80</v>
       </c>
       <c r="C15" s="7" t="s">
-        <v>100</v>
+        <v>94</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -38356,7 +38193,7 @@
         <v>80</v>
       </c>
       <c r="C16" s="7" t="s">
-        <v>102</v>
+        <v>96</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -38364,7 +38201,7 @@
         <v>80</v>
       </c>
       <c r="C18" s="3" t="s">
-        <v>204</v>
+        <v>198</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -38372,7 +38209,7 @@
         <v>80</v>
       </c>
       <c r="C19" s="3" t="s">
-        <v>205</v>
+        <v>199</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -38380,7 +38217,7 @@
         <v>80</v>
       </c>
       <c r="C20" s="3" t="s">
-        <v>206</v>
+        <v>200</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -38388,7 +38225,7 @@
         <v>80</v>
       </c>
       <c r="C21" s="3" t="s">
-        <v>207</v>
+        <v>201</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -38396,7 +38233,7 @@
         <v>80</v>
       </c>
       <c r="C22" s="3" t="s">
-        <v>208</v>
+        <v>202</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -38404,7 +38241,7 @@
         <v>80</v>
       </c>
       <c r="C23" s="3" t="s">
-        <v>209</v>
+        <v>203</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -38412,7 +38249,7 @@
         <v>80</v>
       </c>
       <c r="C24" s="3" t="s">
-        <v>210</v>
+        <v>204</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -38420,7 +38257,7 @@
         <v>80</v>
       </c>
       <c r="C25" s="3" t="s">
-        <v>211</v>
+        <v>205</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -38428,7 +38265,7 @@
         <v>80</v>
       </c>
       <c r="C26" s="3" t="s">
-        <v>212</v>
+        <v>206</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -38436,7 +38273,7 @@
         <v>80</v>
       </c>
       <c r="C27" s="3" t="s">
-        <v>213</v>
+        <v>207</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -38444,7 +38281,7 @@
         <v>80</v>
       </c>
       <c r="C28" s="3" t="s">
-        <v>214</v>
+        <v>208</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -38452,7 +38289,7 @@
         <v>80</v>
       </c>
       <c r="C29" s="3" t="s">
-        <v>215</v>
+        <v>209</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -38460,7 +38297,7 @@
         <v>80</v>
       </c>
       <c r="C30" s="3" t="s">
-        <v>216</v>
+        <v>210</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -38468,7 +38305,7 @@
         <v>80</v>
       </c>
       <c r="C31" s="3" t="s">
-        <v>217</v>
+        <v>211</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -38476,7 +38313,7 @@
         <v>80</v>
       </c>
       <c r="C32" s="3" t="s">
-        <v>218</v>
+        <v>212</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -38484,7 +38321,7 @@
         <v>80</v>
       </c>
       <c r="C33" s="3" t="s">
-        <v>219</v>
+        <v>213</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -38492,7 +38329,7 @@
         <v>80</v>
       </c>
       <c r="C34" s="3" t="s">
-        <v>220</v>
+        <v>214</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -38500,7 +38337,7 @@
         <v>80</v>
       </c>
       <c r="C35" s="3" t="s">
-        <v>221</v>
+        <v>215</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -38508,7 +38345,7 @@
         <v>80</v>
       </c>
       <c r="C36" s="3" t="s">
-        <v>222</v>
+        <v>216</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -38516,7 +38353,7 @@
         <v>80</v>
       </c>
       <c r="C37" s="3" t="s">
-        <v>223</v>
+        <v>217</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -38524,7 +38361,7 @@
         <v>80</v>
       </c>
       <c r="C38" s="3" t="s">
-        <v>224</v>
+        <v>218</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -38532,7 +38369,7 @@
         <v>80</v>
       </c>
       <c r="C39" s="3" t="s">
-        <v>225</v>
+        <v>219</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -38540,7 +38377,7 @@
         <v>80</v>
       </c>
       <c r="C40" s="3" t="s">
-        <v>226</v>
+        <v>220</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -38548,7 +38385,7 @@
         <v>80</v>
       </c>
       <c r="C41" s="3" t="s">
-        <v>227</v>
+        <v>221</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -38556,7 +38393,7 @@
         <v>80</v>
       </c>
       <c r="C42" s="3" t="s">
-        <v>228</v>
+        <v>222</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -38564,7 +38401,7 @@
         <v>80</v>
       </c>
       <c r="C43" s="3" t="s">
-        <v>229</v>
+        <v>223</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -38572,7 +38409,7 @@
         <v>80</v>
       </c>
       <c r="C44" s="3" t="s">
-        <v>230</v>
+        <v>224</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -38580,7 +38417,7 @@
         <v>80</v>
       </c>
       <c r="C45" s="3" t="s">
-        <v>231</v>
+        <v>225</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -38588,7 +38425,7 @@
         <v>80</v>
       </c>
       <c r="C46" s="3" t="s">
-        <v>232</v>
+        <v>226</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -38596,7 +38433,7 @@
         <v>80</v>
       </c>
       <c r="C47" s="3" t="s">
-        <v>233</v>
+        <v>227</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -38604,7 +38441,7 @@
         <v>80</v>
       </c>
       <c r="C48" s="3" t="s">
-        <v>234</v>
+        <v>228</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -38612,7 +38449,7 @@
         <v>80</v>
       </c>
       <c r="C49" s="3" t="s">
-        <v>235</v>
+        <v>229</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -38620,7 +38457,7 @@
         <v>80</v>
       </c>
       <c r="C50" s="3" t="s">
-        <v>236</v>
+        <v>230</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -38628,7 +38465,7 @@
         <v>80</v>
       </c>
       <c r="C51" s="3" t="s">
-        <v>237</v>
+        <v>231</v>
       </c>
     </row>
     <row r="52" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -38636,7 +38473,7 @@
         <v>80</v>
       </c>
       <c r="C52" s="3" t="s">
-        <v>238</v>
+        <v>232</v>
       </c>
     </row>
     <row r="53" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -38644,7 +38481,7 @@
         <v>80</v>
       </c>
       <c r="C53" s="3" t="s">
-        <v>239</v>
+        <v>233</v>
       </c>
     </row>
     <row r="54" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -38652,7 +38489,7 @@
         <v>80</v>
       </c>
       <c r="C54" s="3" t="s">
-        <v>240</v>
+        <v>234</v>
       </c>
     </row>
     <row r="55" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -38660,7 +38497,7 @@
         <v>80</v>
       </c>
       <c r="C55" s="3" t="s">
-        <v>241</v>
+        <v>235</v>
       </c>
     </row>
     <row r="56" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -38668,7 +38505,7 @@
         <v>80</v>
       </c>
       <c r="C56" s="3" t="s">
-        <v>242</v>
+        <v>236</v>
       </c>
     </row>
     <row r="57" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -38676,7 +38513,7 @@
         <v>80</v>
       </c>
       <c r="C57" s="3" t="s">
-        <v>243</v>
+        <v>237</v>
       </c>
     </row>
     <row r="58" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -38684,7 +38521,7 @@
         <v>80</v>
       </c>
       <c r="C58" s="3" t="s">
-        <v>244</v>
+        <v>238</v>
       </c>
     </row>
     <row r="59" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -38692,7 +38529,7 @@
         <v>80</v>
       </c>
       <c r="C59" s="3" t="s">
-        <v>245</v>
+        <v>239</v>
       </c>
     </row>
     <row r="60" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -38700,7 +38537,7 @@
         <v>80</v>
       </c>
       <c r="C60" s="3" t="s">
-        <v>246</v>
+        <v>240</v>
       </c>
     </row>
     <row r="61" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -38708,7 +38545,7 @@
         <v>80</v>
       </c>
       <c r="C61" s="3" t="s">
-        <v>247</v>
+        <v>241</v>
       </c>
     </row>
     <row r="63" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -38716,7 +38553,7 @@
         <v>80</v>
       </c>
       <c r="C63" s="3" t="s">
-        <v>248</v>
+        <v>242</v>
       </c>
     </row>
     <row r="64" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -38724,7 +38561,7 @@
         <v>80</v>
       </c>
       <c r="C64" s="3" t="s">
-        <v>249</v>
+        <v>243</v>
       </c>
     </row>
     <row r="65" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -38732,7 +38569,7 @@
         <v>80</v>
       </c>
       <c r="C65" s="3" t="s">
-        <v>250</v>
+        <v>244</v>
       </c>
     </row>
     <row r="66" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -38740,7 +38577,7 @@
         <v>80</v>
       </c>
       <c r="C66" s="3" t="s">
-        <v>251</v>
+        <v>245</v>
       </c>
     </row>
     <row r="67" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -38748,7 +38585,7 @@
         <v>80</v>
       </c>
       <c r="C67" s="3" t="s">
-        <v>252</v>
+        <v>246</v>
       </c>
     </row>
     <row r="68" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -38756,7 +38593,7 @@
         <v>80</v>
       </c>
       <c r="C68" s="3" t="s">
-        <v>253</v>
+        <v>247</v>
       </c>
     </row>
     <row r="69" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -38764,7 +38601,7 @@
         <v>80</v>
       </c>
       <c r="C69" s="3" t="s">
-        <v>254</v>
+        <v>248</v>
       </c>
     </row>
     <row r="70" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -38772,7 +38609,7 @@
         <v>80</v>
       </c>
       <c r="C70" s="3" t="s">
-        <v>255</v>
+        <v>249</v>
       </c>
     </row>
     <row r="71" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -38780,7 +38617,7 @@
         <v>80</v>
       </c>
       <c r="C71" s="3" t="s">
-        <v>256</v>
+        <v>250</v>
       </c>
     </row>
     <row r="72" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -38788,7 +38625,7 @@
         <v>80</v>
       </c>
       <c r="C72" s="3" t="s">
-        <v>257</v>
+        <v>251</v>
       </c>
     </row>
     <row r="73" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -38796,7 +38633,7 @@
         <v>80</v>
       </c>
       <c r="C73" s="3" t="s">
-        <v>258</v>
+        <v>252</v>
       </c>
     </row>
     <row r="74" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -38804,7 +38641,7 @@
         <v>80</v>
       </c>
       <c r="C74" s="3" t="s">
-        <v>259</v>
+        <v>253</v>
       </c>
     </row>
     <row r="75" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -38812,7 +38649,7 @@
         <v>80</v>
       </c>
       <c r="C75" s="3" t="s">
-        <v>260</v>
+        <v>254</v>
       </c>
     </row>
     <row r="76" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -38820,7 +38657,7 @@
         <v>80</v>
       </c>
       <c r="C76" s="3" t="s">
-        <v>261</v>
+        <v>255</v>
       </c>
     </row>
     <row r="77" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -38828,7 +38665,7 @@
         <v>80</v>
       </c>
       <c r="C77" s="3" t="s">
-        <v>262</v>
+        <v>256</v>
       </c>
     </row>
     <row r="78" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -38836,7 +38673,7 @@
         <v>80</v>
       </c>
       <c r="C78" s="3" t="s">
-        <v>263</v>
+        <v>257</v>
       </c>
     </row>
     <row r="79" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -38844,7 +38681,7 @@
         <v>80</v>
       </c>
       <c r="C79" s="3" t="s">
-        <v>264</v>
+        <v>258</v>
       </c>
     </row>
     <row r="80" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -38852,7 +38689,7 @@
         <v>80</v>
       </c>
       <c r="C80" s="3" t="s">
-        <v>265</v>
+        <v>259</v>
       </c>
     </row>
     <row r="81" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -38860,7 +38697,7 @@
         <v>80</v>
       </c>
       <c r="C81" s="3" t="s">
-        <v>266</v>
+        <v>260</v>
       </c>
     </row>
     <row r="82" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -38868,7 +38705,7 @@
         <v>80</v>
       </c>
       <c r="C82" s="3" t="s">
-        <v>267</v>
+        <v>261</v>
       </c>
     </row>
     <row r="84" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -38876,7 +38713,7 @@
         <v>80</v>
       </c>
       <c r="C84" s="3" t="s">
-        <v>268</v>
+        <v>262</v>
       </c>
     </row>
     <row r="85" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -38884,7 +38721,7 @@
         <v>80</v>
       </c>
       <c r="C85" s="3" t="s">
-        <v>269</v>
+        <v>263</v>
       </c>
     </row>
     <row r="86" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -38892,7 +38729,7 @@
         <v>80</v>
       </c>
       <c r="C86" s="3" t="s">
-        <v>270</v>
+        <v>264</v>
       </c>
     </row>
     <row r="87" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -38900,7 +38737,7 @@
         <v>80</v>
       </c>
       <c r="C87" s="3" t="s">
-        <v>271</v>
+        <v>265</v>
       </c>
     </row>
     <row r="88" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -38908,7 +38745,7 @@
         <v>80</v>
       </c>
       <c r="C88" s="3" t="s">
-        <v>272</v>
+        <v>266</v>
       </c>
     </row>
     <row r="89" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -38916,7 +38753,7 @@
         <v>80</v>
       </c>
       <c r="C89" s="3" t="s">
-        <v>273</v>
+        <v>267</v>
       </c>
     </row>
     <row r="90" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -38924,7 +38761,7 @@
         <v>80</v>
       </c>
       <c r="C90" s="3" t="s">
-        <v>274</v>
+        <v>268</v>
       </c>
     </row>
     <row r="91" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -38932,7 +38769,7 @@
         <v>80</v>
       </c>
       <c r="C91" s="3" t="s">
-        <v>275</v>
+        <v>269</v>
       </c>
     </row>
     <row r="92" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -38940,7 +38777,7 @@
         <v>80</v>
       </c>
       <c r="C92" s="3" t="s">
-        <v>276</v>
+        <v>270</v>
       </c>
     </row>
     <row r="93" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -38948,7 +38785,7 @@
         <v>80</v>
       </c>
       <c r="C93" s="3" t="s">
-        <v>277</v>
+        <v>271</v>
       </c>
     </row>
     <row r="94" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -38956,7 +38793,7 @@
         <v>80</v>
       </c>
       <c r="C94" s="3" t="s">
-        <v>278</v>
+        <v>272</v>
       </c>
     </row>
     <row r="95" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -38964,7 +38801,7 @@
         <v>80</v>
       </c>
       <c r="C95" s="3" t="s">
-        <v>279</v>
+        <v>273</v>
       </c>
     </row>
     <row r="96" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -38972,7 +38809,7 @@
         <v>80</v>
       </c>
       <c r="C96" s="3" t="s">
-        <v>280</v>
+        <v>274</v>
       </c>
     </row>
     <row r="97" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -38980,7 +38817,7 @@
         <v>80</v>
       </c>
       <c r="C97" s="3" t="s">
-        <v>281</v>
+        <v>275</v>
       </c>
     </row>
     <row r="98" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -38988,7 +38825,7 @@
         <v>80</v>
       </c>
       <c r="C98" s="3" t="s">
-        <v>282</v>
+        <v>276</v>
       </c>
     </row>
     <row r="99" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -38996,7 +38833,7 @@
         <v>80</v>
       </c>
       <c r="C99" s="3" t="s">
-        <v>283</v>
+        <v>277</v>
       </c>
     </row>
     <row r="100" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -39004,7 +38841,7 @@
         <v>80</v>
       </c>
       <c r="C100" s="3" t="s">
-        <v>284</v>
+        <v>278</v>
       </c>
     </row>
     <row r="101" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -39012,7 +38849,7 @@
         <v>80</v>
       </c>
       <c r="C101" s="3" t="s">
-        <v>285</v>
+        <v>279</v>
       </c>
     </row>
     <row r="102" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -39020,7 +38857,7 @@
         <v>80</v>
       </c>
       <c r="C102" s="3" t="s">
-        <v>286</v>
+        <v>280</v>
       </c>
     </row>
     <row r="103" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -39028,7 +38865,7 @@
         <v>80</v>
       </c>
       <c r="C103" s="3" t="s">
-        <v>287</v>
+        <v>281</v>
       </c>
     </row>
   </sheetData>
@@ -39055,14 +38892,14 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="39.9545454545454"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="46.8939393939394"/>
-    <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="8.15151515151515"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="39.1515151515151"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="45.8333333333333"/>
+    <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="7.88383838383838"/>
   </cols>
   <sheetData>
     <row r="1" s="2" customFormat="true" ht="13.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
-        <v>288</v>
+        <v>282</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>68</v>
@@ -39070,50 +38907,50 @@
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="7" t="s">
-        <v>289</v>
+        <v>283</v>
       </c>
       <c r="B3" s="7" t="s">
-        <v>290</v>
+        <v>284</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="7" t="s">
-        <v>291</v>
+        <v>285</v>
       </c>
       <c r="B4" s="7" t="s">
-        <v>292</v>
+        <v>286</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="7" t="s">
-        <v>293</v>
+        <v>287</v>
       </c>
       <c r="B5" s="7" t="s">
-        <v>294</v>
+        <v>288</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="7" t="s">
-        <v>295</v>
+        <v>289</v>
       </c>
       <c r="B6" s="7" t="s">
-        <v>296</v>
+        <v>290</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="7" t="s">
-        <v>297</v>
+        <v>291</v>
       </c>
       <c r="B7" s="7" t="s">
-        <v>298</v>
+        <v>292</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="7" t="s">
-        <v>299</v>
+        <v>293</v>
       </c>
       <c r="B8" s="7" t="s">
-        <v>300</v>
+        <v>294</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
separates organization and attendees
</commit_message>
<xml_diff>
--- a/tables/actor/forms/actor/actor.xlsx
+++ b/tables/actor/forms/actor/actor.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="988" firstSheet="0" activeTab="3"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="976" firstSheet="0" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="initial" sheetId="1" state="visible" r:id="rId2"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="519" uniqueCount="295">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="521" uniqueCount="296">
   <si>
     <t xml:space="preserve">clause</t>
   </si>
@@ -1526,6 +1526,9 @@
     <t xml:space="preserve">forcedSubstances</t>
   </si>
   <si>
+    <t xml:space="preserve">organization</t>
+  </si>
+  <si>
     <t xml:space="preserve">calculation_name</t>
   </si>
   <si>
@@ -1748,11 +1751,11 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="14.5656565656566"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="7.61616161616162"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="18.5757575757576"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="41.2929292929293"/>
-    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="7.61616161616162"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="14.1666666666667"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="7.34848484848485"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="18.1717171717172"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="40.3535353535354"/>
+    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="7.34848484848485"/>
   </cols>
   <sheetData>
     <row r="1" s="2" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1809,12 +1812,12 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="14.1666666666667"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="13.4949494949495"/>
-    <col collapsed="false" hidden="false" max="4" min="3" style="0" width="19.3737373737374"/>
-    <col collapsed="false" hidden="false" max="7" min="5" style="0" width="7.88383838383838"/>
-    <col collapsed="false" hidden="false" max="9" min="8" style="0" width="21.2474747474747"/>
-    <col collapsed="false" hidden="false" max="1025" min="10" style="0" width="7.88383838383838"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="13.7626262626263"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="13.0959595959596"/>
+    <col collapsed="false" hidden="false" max="4" min="3" style="0" width="18.9747474747475"/>
+    <col collapsed="false" hidden="false" max="7" min="5" style="0" width="7.61616161616162"/>
+    <col collapsed="false" hidden="false" max="9" min="8" style="0" width="20.8484848484848"/>
+    <col collapsed="false" hidden="false" max="1025" min="10" style="0" width="7.61616161616162"/>
   </cols>
   <sheetData>
     <row r="1" s="2" customFormat="true" ht="18.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1940,11 +1943,11 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="3" width="31.4040404040404"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="3" width="48.2373737373737"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="3" width="48.6414141414141"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="3" width="82.1818181818182"/>
-    <col collapsed="false" hidden="false" max="1025" min="5" style="3" width="4.54545454545455"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="3" width="30.7323232323232"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="3" width="47.1717171717172"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="3" width="47.4393939393939"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="3" width="80.4444444444444"/>
+    <col collapsed="false" hidden="false" max="1025" min="5" style="3" width="4.40909090909091"/>
   </cols>
   <sheetData>
     <row r="1" s="1" customFormat="true" ht="14.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -37084,28 +37087,28 @@
   </sheetPr>
   <dimension ref="1:19"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="D21" activeCellId="0" sqref="D21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="9.35353535353535"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="12.8282828282828"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="10.8232323232323"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="38.4848484848485"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="22.4494949494949"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="20.0454545454545"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="30.3333333333333"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="22.8484848484848"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="7.61616161616162"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="10.6919191919192"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="7.88383838383838"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="13.8989898989899"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="18.9747474747475"/>
-    <col collapsed="false" hidden="false" max="19" min="14" style="0" width="7.88383838383838"/>
-    <col collapsed="false" hidden="false" max="20" min="20" style="0" width="20.979797979798"/>
-    <col collapsed="false" hidden="false" max="1025" min="21" style="0" width="7.88383838383838"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="9.08585858585859"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="12.5606060606061"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="10.5555555555556"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="37.5505050505051"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="21.9141414141414"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="19.510101010101"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="29.530303030303"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="22.3181818181818"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="7.34848484848485"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="10.4242424242424"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="7.61616161616162"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="13.4949494949495"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="18.5757575757576"/>
+    <col collapsed="false" hidden="false" max="19" min="14" style="0" width="7.61616161616162"/>
+    <col collapsed="false" hidden="false" max="20" min="20" style="0" width="20.4444444444444"/>
+    <col collapsed="false" hidden="false" max="1025" min="21" style="0" width="7.61616161616162"/>
   </cols>
   <sheetData>
     <row r="1" s="6" customFormat="true" ht="17.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -37412,12 +37415,12 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="16.7020202020202"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="25.2575757575758"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="24.1868686868687"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="33.6767676767677"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="50.2424242424242"/>
-    <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="7.88383838383838"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="16.3030303030303"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="24.7222222222222"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="23.520202020202"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="33.0050505050505"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="49.1767676767677"/>
+    <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="7.61616161616162"/>
   </cols>
   <sheetData>
     <row r="1" s="1" customFormat="true" ht="22.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -38053,20 +38056,20 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="1:103"/>
+  <dimension ref="1:104"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B18" activeCellId="0" sqref="B18"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A88" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C106" activeCellId="0" sqref="C106"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="15.5"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="17.6414141414141"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="40.0909090909091"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="15.9040404040404"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="27.2626262626263"/>
-    <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="7.88383838383838"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="15.1010101010101"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="17.1060606060606"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="39.2878787878788"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="15.5"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="26.5909090909091"/>
+    <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="7.61616161616162"/>
   </cols>
   <sheetData>
     <row r="1" s="6" customFormat="true" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -38866,6 +38869,14 @@
       </c>
       <c r="C103" s="3" t="s">
         <v>281</v>
+      </c>
+    </row>
+    <row r="104" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B104" s="7" t="s">
+        <v>80</v>
+      </c>
+      <c r="C104" s="7" t="s">
+        <v>282</v>
       </c>
     </row>
   </sheetData>
@@ -38892,14 +38903,14 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="39.1515151515151"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="45.8333333333333"/>
-    <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="7.88383838383838"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="38.2171717171717"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="44.8989898989899"/>
+    <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="7.61616161616162"/>
   </cols>
   <sheetData>
     <row r="1" s="2" customFormat="true" ht="13.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
-        <v>282</v>
+        <v>283</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>68</v>
@@ -38907,50 +38918,50 @@
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="7" t="s">
-        <v>283</v>
+        <v>284</v>
       </c>
       <c r="B3" s="7" t="s">
-        <v>284</v>
+        <v>285</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="7" t="s">
-        <v>285</v>
+        <v>286</v>
       </c>
       <c r="B4" s="7" t="s">
-        <v>286</v>
+        <v>287</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="7" t="s">
-        <v>287</v>
+        <v>288</v>
       </c>
       <c r="B5" s="7" t="s">
-        <v>288</v>
+        <v>289</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="7" t="s">
-        <v>289</v>
+        <v>290</v>
       </c>
       <c r="B6" s="7" t="s">
-        <v>290</v>
+        <v>291</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="7" t="s">
-        <v>291</v>
+        <v>292</v>
       </c>
       <c r="B7" s="7" t="s">
-        <v>292</v>
+        <v>293</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="7" t="s">
-        <v>293</v>
+        <v>294</v>
       </c>
       <c r="B8" s="7" t="s">
-        <v>294</v>
+        <v>295</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
update RAs and make actor name required
</commit_message>
<xml_diff>
--- a/tables/actor/forms/actor/actor.xlsx
+++ b/tables/actor/forms/actor/actor.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="976" firstSheet="0" activeTab="5"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="988" firstSheet="0" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="initial" sheetId="1" state="visible" r:id="rId2"/>
@@ -1751,11 +1751,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="14.1666666666667"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="7.34848484848485"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="18.1717171717172"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="40.3535353535354"/>
-    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="7.34848484848485"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="13.7626262626263"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="17.6414141414141"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="39.4191919191919"/>
   </cols>
   <sheetData>
     <row r="1" s="2" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1812,12 +1810,12 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="13.7626262626263"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="13.0959595959596"/>
-    <col collapsed="false" hidden="false" max="4" min="3" style="0" width="18.9747474747475"/>
-    <col collapsed="false" hidden="false" max="7" min="5" style="0" width="7.61616161616162"/>
-    <col collapsed="false" hidden="false" max="9" min="8" style="0" width="20.8484848484848"/>
-    <col collapsed="false" hidden="false" max="1025" min="10" style="0" width="7.61616161616162"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="13.3636363636364"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="12.8282828282828"/>
+    <col collapsed="false" hidden="false" max="4" min="3" style="0" width="18.5757575757576"/>
+    <col collapsed="false" hidden="false" max="7" min="5" style="0" width="7.34848484848485"/>
+    <col collapsed="false" hidden="false" max="9" min="8" style="0" width="20.3131313131313"/>
+    <col collapsed="false" hidden="false" max="1025" min="10" style="0" width="7.34848484848485"/>
   </cols>
   <sheetData>
     <row r="1" s="2" customFormat="true" ht="18.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1943,11 +1941,11 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="3" width="30.7323232323232"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="3" width="47.1717171717172"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="3" width="47.4393939393939"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="3" width="80.4444444444444"/>
-    <col collapsed="false" hidden="false" max="1025" min="5" style="3" width="4.40909090909091"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="3" width="30.0656565656566"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="3" width="46.1010101010101"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="3" width="46.3686868686869"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="3" width="78.7070707070707"/>
+    <col collapsed="false" hidden="false" max="1025" min="5" style="3" width="4.27777777777778"/>
   </cols>
   <sheetData>
     <row r="1" s="1" customFormat="true" ht="14.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -37087,28 +37085,28 @@
   </sheetPr>
   <dimension ref="1:19"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D21" activeCellId="0" sqref="D21"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="H6" activeCellId="0" sqref="H6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="9.08585858585859"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="12.5606060606061"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="10.5555555555556"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="37.5505050505051"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="21.9141414141414"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="19.510101010101"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="29.530303030303"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="22.3181818181818"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="7.34848484848485"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="10.4242424242424"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="7.61616161616162"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="13.4949494949495"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="18.5757575757576"/>
-    <col collapsed="false" hidden="false" max="19" min="14" style="0" width="7.61616161616162"/>
-    <col collapsed="false" hidden="false" max="20" min="20" style="0" width="20.4444444444444"/>
-    <col collapsed="false" hidden="false" max="1025" min="21" style="0" width="7.61616161616162"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="8.95454545454546"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="12.2929292929293"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="10.2878787878788"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="36.7474747474747"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="21.3787878787879"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="19.1111111111111"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="28.8636363636364"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="21.7828282828283"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="15.4040404040404"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="10.1565656565657"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="7.34848484848485"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="13.0959595959596"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="18.1717171717172"/>
+    <col collapsed="false" hidden="false" max="19" min="14" style="0" width="7.34848484848485"/>
+    <col collapsed="false" hidden="false" max="20" min="20" style="0" width="19.9090909090909"/>
+    <col collapsed="false" hidden="false" max="1025" min="21" style="0" width="7.34848484848485"/>
   </cols>
   <sheetData>
     <row r="1" s="6" customFormat="true" ht="17.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -37224,7 +37222,9 @@
         <v>24</v>
       </c>
       <c r="H4" s="4"/>
-      <c r="I4" s="3"/>
+      <c r="I4" s="3" t="n">
+        <v>1</v>
+      </c>
       <c r="L4" s="3"/>
     </row>
     <row r="5" customFormat="false" ht="21.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -37415,12 +37415,12 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="16.3030303030303"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="24.7222222222222"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="23.520202020202"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="33.0050505050505"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="49.1767676767677"/>
-    <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="7.61616161616162"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="15.9040404040404"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="24.1868686868687"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="22.9848484848485"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="32.2020202020202"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="48.1060606060606"/>
+    <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="7.34848484848485"/>
   </cols>
   <sheetData>
     <row r="1" s="1" customFormat="true" ht="22.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -38058,18 +38058,18 @@
   </sheetPr>
   <dimension ref="1:104"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A88" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A88" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="C106" activeCellId="0" sqref="C106"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="15.1010101010101"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="17.1060606060606"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="39.2878787878788"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="15.5"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="26.5909090909091"/>
-    <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="7.61616161616162"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="14.6969696969697"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="16.7020202020202"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="38.3535353535354"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="15.1010101010101"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="25.9242424242424"/>
+    <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="7.34848484848485"/>
   </cols>
   <sheetData>
     <row r="1" s="6" customFormat="true" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -38903,9 +38903,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="38.2171717171717"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="44.8989898989899"/>
-    <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="7.61616161616162"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="37.4141414141414"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="43.8282828282828"/>
+    <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="7.34848484848485"/>
   </cols>
   <sheetData>
     <row r="1" s="2" customFormat="true" ht="13.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">

</xml_diff>

<commit_message>
add currently in myanmar
</commit_message>
<xml_diff>
--- a/tables/actor/forms/actor/actor.xlsx
+++ b/tables/actor/forms/actor/actor.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="988" firstSheet="0" activeTab="6"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="988" firstSheet="0" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="initial" sheetId="1" state="visible" r:id="rId2"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="515" uniqueCount="290">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="517" uniqueCount="291">
   <si>
     <t xml:space="preserve">clause</t>
   </si>
@@ -1379,6 +1379,9 @@
     <t xml:space="preserve">currentlyInThailand</t>
   </si>
   <si>
+    <t xml:space="preserve">currentlyInMyanmar</t>
+  </si>
+  <si>
     <t xml:space="preserve">remittances</t>
   </si>
   <si>
@@ -1733,11 +1736,11 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="13.0959595959596"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="8.15151515151515"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="16.7020202020202"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="37.5505050505051"/>
-    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="8.15151515151515"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="12.8282828282828"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="7.88383838383838"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="16.3030303030303"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="36.7474747474747"/>
+    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="7.88383838383838"/>
   </cols>
   <sheetData>
     <row r="1" s="2" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1794,14 +1797,14 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="12.8282828282828"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="12.2929292929293"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="24.5858585858586"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="21.6464646464646"/>
-    <col collapsed="false" hidden="false" max="7" min="5" style="0" width="8.41919191919192"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="24.1868686868687"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="19.2424242424242"/>
-    <col collapsed="false" hidden="false" max="1025" min="10" style="0" width="8.41919191919192"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="12.5606060606061"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="12.0252525252525"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="24.0555555555556"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="21.2474747474747"/>
+    <col collapsed="false" hidden="false" max="7" min="5" style="0" width="8.15151515151515"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="23.520202020202"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="18.8434343434343"/>
+    <col collapsed="false" hidden="false" max="1025" min="10" style="0" width="8.15151515151515"/>
   </cols>
   <sheetData>
     <row r="1" s="2" customFormat="true" ht="18.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1927,12 +1930,12 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="3" width="28.5959595959596"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="3" width="44.0959595959596"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="3" width="66.4141414141414"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="3" width="44.3636363636364"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="3" width="75.3686868686869"/>
-    <col collapsed="false" hidden="false" max="1025" min="6" style="3" width="4.01010101010101"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="3" width="27.9292929292929"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="3" width="43.1616161616162"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="3" width="64.9444444444444"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="3" width="43.4292929292929"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="3" width="73.7626262626263"/>
+    <col collapsed="false" hidden="false" max="1025" min="6" style="3" width="3.87373737373737"/>
   </cols>
   <sheetData>
     <row r="1" s="1" customFormat="true" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -37108,22 +37111,22 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="8.41919191919192"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="11.6262626262626"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="9.75252525252525"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="35.1464646464646"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="20.4444444444444"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="18.3080808080808"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="27.5252525252525"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="20.8484848484848"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="14.6969696969697"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="9.62121212121212"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="8.41919191919192"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="12.5606060606061"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="17.1060606060606"/>
-    <col collapsed="false" hidden="false" max="19" min="14" style="0" width="8.41919191919192"/>
-    <col collapsed="false" hidden="false" max="20" min="20" style="0" width="18.9747474747475"/>
-    <col collapsed="false" hidden="false" max="1025" min="21" style="0" width="8.41919191919192"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="8.15151515151515"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="11.2272727272727"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="9.48989898989899"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="34.3434343434343"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="19.9090909090909"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="17.9040404040404"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="26.9949494949495"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="20.3131313131313"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="14.2979797979798"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="9.35353535353535"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="8.15151515151515"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="12.2929292929293"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="16.7020202020202"/>
+    <col collapsed="false" hidden="false" max="19" min="14" style="0" width="8.15151515151515"/>
+    <col collapsed="false" hidden="false" max="20" min="20" style="0" width="18.5757575757576"/>
+    <col collapsed="false" hidden="false" max="1025" min="21" style="0" width="8.15151515151515"/>
   </cols>
   <sheetData>
     <row r="1" s="6" customFormat="true" ht="17.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -37432,12 +37435,12 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="15.1010101010101"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="22.9848484848485"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="21.9141414141414"/>
-    <col collapsed="false" hidden="false" max="5" min="4" style="0" width="30.7323232323232"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="45.969696969697"/>
-    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="8.41919191919192"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="14.6969696969697"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="22.4494949494949"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="21.3787878787879"/>
+    <col collapsed="false" hidden="false" max="5" min="4" style="0" width="30.0656565656566"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="45.030303030303"/>
+    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="8.15151515151515"/>
   </cols>
   <sheetData>
     <row r="1" s="1" customFormat="true" ht="22.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -38117,20 +38120,20 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="1:104"/>
+  <dimension ref="1:105"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A88" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C106" activeCellId="0" sqref="C106"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A38" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C53" activeCellId="0" sqref="C53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="13.8989898989899"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="15.9040404040404"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="36.6161616161616"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="14.2979797979798"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="24.7222222222222"/>
-    <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="8.41919191919192"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="13.4949494949495"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="15.5"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="35.8131313131313"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="13.8989898989899"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="24.1868686868687"/>
+    <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="8.15151515151515"/>
   </cols>
   <sheetData>
     <row r="1" s="6" customFormat="true" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -38612,11 +38615,11 @@
         <v>241</v>
       </c>
     </row>
-    <row r="63" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B63" s="3" t="s">
+    <row r="62" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B62" s="3" t="s">
         <v>80</v>
       </c>
-      <c r="C63" s="3" t="s">
+      <c r="C62" s="3" t="s">
         <v>242</v>
       </c>
     </row>
@@ -38772,11 +38775,11 @@
         <v>261</v>
       </c>
     </row>
-    <row r="84" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B84" s="3" t="s">
+    <row r="83" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B83" s="3" t="s">
         <v>80</v>
       </c>
-      <c r="C84" s="3" t="s">
+      <c r="C83" s="3" t="s">
         <v>262</v>
       </c>
     </row>
@@ -38933,11 +38936,19 @@
       </c>
     </row>
     <row r="104" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B104" s="7" t="s">
+      <c r="B104" s="3" t="s">
         <v>80</v>
       </c>
-      <c r="C104" s="7" t="s">
+      <c r="C104" s="3" t="s">
         <v>282</v>
+      </c>
+    </row>
+    <row r="105" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B105" s="7" t="s">
+        <v>80</v>
+      </c>
+      <c r="C105" s="7" t="s">
+        <v>283</v>
       </c>
     </row>
   </sheetData>
@@ -38958,20 +38969,20 @@
   </sheetPr>
   <dimension ref="A1:B5"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A11" activeCellId="0" sqref="A11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="35.8131313131313"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="41.959595959596"/>
-    <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="8.41919191919192"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="35.010101010101"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="41.0252525252525"/>
+    <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="8.15151515151515"/>
   </cols>
   <sheetData>
     <row r="1" s="2" customFormat="true" ht="13.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
-        <v>283</v>
+        <v>284</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>68</v>
@@ -38979,26 +38990,26 @@
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="7" t="s">
-        <v>284</v>
+        <v>285</v>
       </c>
       <c r="B3" s="7" t="s">
-        <v>285</v>
+        <v>286</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="7" t="s">
-        <v>286</v>
+        <v>287</v>
       </c>
       <c r="B4" s="7" t="s">
-        <v>287</v>
+        <v>288</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="7" t="s">
-        <v>288</v>
+        <v>289</v>
       </c>
       <c r="B5" s="7" t="s">
-        <v>289</v>
+        <v>290</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
add arrange travel documentation before/after
</commit_message>
<xml_diff>
--- a/tables/actor/forms/actor/actor.xlsx
+++ b/tables/actor/forms/actor/actor.xlsx
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="517" uniqueCount="291">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="519" uniqueCount="292">
   <si>
     <t xml:space="preserve">clause</t>
   </si>
@@ -1316,7 +1316,10 @@
     <t xml:space="preserve">arrangedContractAfter</t>
   </si>
   <si>
-    <t xml:space="preserve">arrangedTravelDocumentation</t>
+    <t xml:space="preserve">arrangedTravelDocumentationBefore</t>
+  </si>
+  <si>
+    <t xml:space="preserve">arrangedTravelDocumentationAfter</t>
   </si>
   <si>
     <t xml:space="preserve">arrangedTransportation</t>
@@ -38120,10 +38123,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="1:105"/>
+  <dimension ref="1:106"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A38" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C53" activeCellId="0" sqref="C53"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A18" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C35" activeCellId="0" sqref="C35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -38623,11 +38626,11 @@
         <v>242</v>
       </c>
     </row>
-    <row r="64" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B64" s="3" t="s">
+    <row r="63" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B63" s="3" t="s">
         <v>80</v>
       </c>
-      <c r="C64" s="3" t="s">
+      <c r="C63" s="3" t="s">
         <v>243</v>
       </c>
     </row>
@@ -38783,11 +38786,11 @@
         <v>262</v>
       </c>
     </row>
-    <row r="85" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B85" s="3" t="s">
+    <row r="84" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B84" s="3" t="s">
         <v>80</v>
       </c>
-      <c r="C85" s="3" t="s">
+      <c r="C84" s="3" t="s">
         <v>263</v>
       </c>
     </row>
@@ -38944,11 +38947,19 @@
       </c>
     </row>
     <row r="105" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B105" s="7" t="s">
+      <c r="B105" s="3" t="s">
         <v>80</v>
       </c>
-      <c r="C105" s="7" t="s">
+      <c r="C105" s="3" t="s">
         <v>283</v>
+      </c>
+    </row>
+    <row r="106" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B106" s="7" t="s">
+        <v>80</v>
+      </c>
+      <c r="C106" s="7" t="s">
+        <v>284</v>
       </c>
     </row>
   </sheetData>
@@ -38982,7 +38993,7 @@
   <sheetData>
     <row r="1" s="2" customFormat="true" ht="13.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
-        <v>284</v>
+        <v>285</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>68</v>
@@ -38990,26 +39001,26 @@
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="7" t="s">
-        <v>285</v>
+        <v>286</v>
       </c>
       <c r="B3" s="7" t="s">
-        <v>286</v>
+        <v>287</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="7" t="s">
-        <v>287</v>
+        <v>288</v>
       </c>
       <c r="B4" s="7" t="s">
-        <v>288</v>
+        <v>289</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="7" t="s">
-        <v>289</v>
+        <v>290</v>
       </c>
       <c r="B5" s="7" t="s">
-        <v>290</v>
+        <v>291</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
add previous smuggler or transporter
</commit_message>
<xml_diff>
--- a/tables/actor/forms/actor/actor.xlsx
+++ b/tables/actor/forms/actor/actor.xlsx
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="521" uniqueCount="293">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="523" uniqueCount="294">
   <si>
     <t xml:space="preserve">clause</t>
   </si>
@@ -1538,6 +1538,9 @@
     <t xml:space="preserve">organization</t>
   </si>
   <si>
+    <t xml:space="preserve">previousSmugglerOrTransporter</t>
+  </si>
+  <si>
     <t xml:space="preserve">calculation_name</t>
   </si>
   <si>
@@ -1566,7 +1569,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="7">
+  <fonts count="8">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -1608,6 +1611,12 @@
       <name val="Myanmar3"/>
       <family val="0"/>
       <charset val="1"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Myanmar3"/>
+      <family val="0"/>
     </font>
   </fonts>
   <fills count="4">
@@ -1664,7 +1673,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="14">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1714,6 +1723,10 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -38126,10 +38139,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="1:107"/>
+  <dimension ref="1:109"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A18" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C36" activeCellId="0" sqref="C36"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A96" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C111" activeCellId="0" sqref="C111"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -38971,6 +38984,14 @@
       </c>
       <c r="C107" s="7" t="s">
         <v>285</v>
+      </c>
+    </row>
+    <row r="109" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B109" s="7" t="s">
+        <v>80</v>
+      </c>
+      <c r="C109" s="13" t="s">
+        <v>286</v>
       </c>
     </row>
   </sheetData>
@@ -39004,7 +39025,7 @@
   <sheetData>
     <row r="1" s="2" customFormat="true" ht="13.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
-        <v>286</v>
+        <v>287</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>68</v>
@@ -39012,26 +39033,26 @@
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="7" t="s">
-        <v>287</v>
+        <v>288</v>
       </c>
       <c r="B3" s="7" t="s">
-        <v>288</v>
+        <v>289</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="7" t="s">
-        <v>289</v>
+        <v>290</v>
       </c>
       <c r="B4" s="7" t="s">
-        <v>290</v>
+        <v>291</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="7" t="s">
-        <v>291</v>
+        <v>292</v>
       </c>
       <c r="B5" s="7" t="s">
-        <v>292</v>
+        <v>293</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
add smuggler or transporter
</commit_message>
<xml_diff>
--- a/tables/actor/forms/actor/actor.xlsx
+++ b/tables/actor/forms/actor/actor.xlsx
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="523" uniqueCount="294">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="525" uniqueCount="295">
   <si>
     <t xml:space="preserve">clause</t>
   </si>
@@ -1539,6 +1539,9 @@
   </si>
   <si>
     <t xml:space="preserve">previousSmugglerOrTransporter</t>
+  </si>
+  <si>
+    <t xml:space="preserve">smugglerOrTransporterForMigrant</t>
   </si>
   <si>
     <t xml:space="preserve">calculation_name</t>
@@ -38139,10 +38142,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="1:109"/>
+  <dimension ref="1:110"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A96" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C111" activeCellId="0" sqref="C111"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A98" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C112" activeCellId="0" sqref="C112"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -38992,6 +38995,14 @@
       </c>
       <c r="C109" s="13" t="s">
         <v>286</v>
+      </c>
+    </row>
+    <row r="110" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B110" s="7" t="s">
+        <v>80</v>
+      </c>
+      <c r="C110" s="7" t="s">
+        <v>287</v>
       </c>
     </row>
   </sheetData>
@@ -39025,7 +39036,7 @@
   <sheetData>
     <row r="1" s="2" customFormat="true" ht="13.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
-        <v>287</v>
+        <v>288</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>68</v>
@@ -39033,26 +39044,26 @@
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="7" t="s">
-        <v>288</v>
+        <v>289</v>
       </c>
       <c r="B3" s="7" t="s">
-        <v>289</v>
+        <v>290</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="7" t="s">
-        <v>290</v>
+        <v>291</v>
       </c>
       <c r="B4" s="7" t="s">
-        <v>291</v>
+        <v>292</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="7" t="s">
-        <v>292</v>
+        <v>293</v>
       </c>
       <c r="B5" s="7" t="s">
-        <v>293</v>
+        <v>294</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
add intentionally caused harm
</commit_message>
<xml_diff>
--- a/tables/actor/forms/actor/actor.xlsx
+++ b/tables/actor/forms/actor/actor.xlsx
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="525" uniqueCount="295">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="527" uniqueCount="296">
   <si>
     <t xml:space="preserve">clause</t>
   </si>
@@ -1413,6 +1413,9 @@
   </si>
   <si>
     <t xml:space="preserve">causedProblems</t>
+  </si>
+  <si>
+    <t xml:space="preserve">intentionallyCausedProblems</t>
   </si>
   <si>
     <t xml:space="preserve">expectationsDestination</t>
@@ -38142,10 +38145,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="1:110"/>
+  <dimension ref="1:111"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A98" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C112" activeCellId="0" sqref="C112"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A59" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B66" activeCellId="0" sqref="B66"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -38661,11 +38664,11 @@
         <v>244</v>
       </c>
     </row>
-    <row r="66" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B66" s="3" t="s">
+    <row r="65" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B65" s="3" t="s">
         <v>80</v>
       </c>
-      <c r="C66" s="3" t="s">
+      <c r="C65" s="3" t="s">
         <v>245</v>
       </c>
     </row>
@@ -38821,11 +38824,11 @@
         <v>264</v>
       </c>
     </row>
-    <row r="87" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B87" s="3" t="s">
+    <row r="86" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B86" s="3" t="s">
         <v>80</v>
       </c>
-      <c r="C87" s="3" t="s">
+      <c r="C86" s="3" t="s">
         <v>265</v>
       </c>
     </row>
@@ -38982,18 +38985,18 @@
       </c>
     </row>
     <row r="107" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B107" s="7" t="s">
+      <c r="B107" s="3" t="s">
         <v>80</v>
       </c>
-      <c r="C107" s="7" t="s">
+      <c r="C107" s="3" t="s">
         <v>285</v>
       </c>
     </row>
-    <row r="109" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B109" s="7" t="s">
+    <row r="108" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B108" s="7" t="s">
         <v>80</v>
       </c>
-      <c r="C109" s="13" t="s">
+      <c r="C108" s="7" t="s">
         <v>286</v>
       </c>
     </row>
@@ -39001,8 +39004,16 @@
       <c r="B110" s="7" t="s">
         <v>80</v>
       </c>
-      <c r="C110" s="7" t="s">
+      <c r="C110" s="13" t="s">
         <v>287</v>
+      </c>
+    </row>
+    <row r="111" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B111" s="7" t="s">
+        <v>80</v>
+      </c>
+      <c r="C111" s="7" t="s">
+        <v>288</v>
       </c>
     </row>
   </sheetData>
@@ -39036,7 +39047,7 @@
   <sheetData>
     <row r="1" s="2" customFormat="true" ht="13.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
-        <v>288</v>
+        <v>289</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>68</v>
@@ -39044,26 +39055,26 @@
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="7" t="s">
-        <v>289</v>
+        <v>290</v>
       </c>
       <c r="B3" s="7" t="s">
-        <v>290</v>
+        <v>291</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="7" t="s">
-        <v>291</v>
+        <v>292</v>
       </c>
       <c r="B4" s="7" t="s">
-        <v>292</v>
+        <v>293</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="7" t="s">
-        <v>293</v>
+        <v>294</v>
       </c>
       <c r="B5" s="7" t="s">
-        <v>294</v>
+        <v>295</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
add 2 part suggestion
</commit_message>
<xml_diff>
--- a/tables/actor/forms/actor/actor.xlsx
+++ b/tables/actor/forms/actor/actor.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="988" firstSheet="0" activeTab="5"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="968" firstSheet="0" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="initial" sheetId="1" state="visible" r:id="rId2"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="527" uniqueCount="296">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="529" uniqueCount="297">
   <si>
     <t xml:space="preserve">clause</t>
   </si>
@@ -1277,6 +1277,9 @@
     <t xml:space="preserve">firstSuggestion</t>
   </si>
   <si>
+    <t xml:space="preserve">firstTold</t>
+  </si>
+  <si>
     <t xml:space="preserve">neededPermission</t>
   </si>
   <si>
@@ -1575,7 +1578,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="8">
+  <fonts count="7">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -1617,12 +1620,6 @@
       <name val="Myanmar3"/>
       <family val="0"/>
       <charset val="1"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color rgb="FF000000"/>
-      <name val="Myanmar3"/>
-      <family val="0"/>
     </font>
   </fonts>
   <fills count="4">
@@ -1679,7 +1676,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="13">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1732,10 +1729,6 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
   </cellXfs>
   <cellStyles count="6">
     <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="false"/>
@@ -1761,11 +1754,11 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="12.8282828282828"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="7.88383838383838"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="16.3030303030303"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="36.7474747474747"/>
-    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="7.88383838383838"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="12.5606060606061"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="7.61616161616162"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="15.9040404040404"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="35.9444444444444"/>
+    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="7.61616161616162"/>
   </cols>
   <sheetData>
     <row r="1" s="2" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1822,14 +1815,14 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="12.5606060606061"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="12.0252525252525"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="24.0555555555556"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="21.2474747474747"/>
-    <col collapsed="false" hidden="false" max="7" min="5" style="0" width="8.15151515151515"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="23.520202020202"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="18.8434343434343"/>
-    <col collapsed="false" hidden="false" max="1025" min="10" style="0" width="8.15151515151515"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="12.2929292929293"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="11.6262626262626"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="23.3838383838384"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="20.8484848484848"/>
+    <col collapsed="false" hidden="false" max="7" min="5" style="0" width="7.88383838383838"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="22.9848484848485"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="18.4393939393939"/>
+    <col collapsed="false" hidden="false" max="1025" min="10" style="0" width="7.88383838383838"/>
   </cols>
   <sheetData>
     <row r="1" s="2" customFormat="true" ht="18.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1955,12 +1948,12 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="3" width="27.9292929292929"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="3" width="43.1616161616162"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="3" width="64.9444444444444"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="3" width="43.4292929292929"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="3" width="73.7626262626263"/>
-    <col collapsed="false" hidden="false" max="1025" min="6" style="3" width="3.87373737373737"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="3" width="27.2626262626263"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="3" width="42.2272727272727"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="3" width="63.6060606060606"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="3" width="42.4949494949495"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="3" width="72.1616161616162"/>
+    <col collapsed="false" hidden="false" max="1025" min="6" style="3" width="3.74242424242424"/>
   </cols>
   <sheetData>
     <row r="1" s="1" customFormat="true" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -37136,22 +37129,22 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="8.15151515151515"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="11.2272727272727"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="9.48989898989899"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="34.3434343434343"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="19.9090909090909"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="17.9040404040404"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="26.9949494949495"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="20.3131313131313"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="14.2979797979798"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="9.35353535353535"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="8.15151515151515"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="12.2929292929293"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="16.7020202020202"/>
-    <col collapsed="false" hidden="false" max="19" min="14" style="0" width="8.15151515151515"/>
-    <col collapsed="false" hidden="false" max="20" min="20" style="0" width="18.5757575757576"/>
-    <col collapsed="false" hidden="false" max="1025" min="21" style="0" width="8.15151515151515"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="7.88383838383838"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="10.959595959596"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="9.22222222222222"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="33.540404040404"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="19.3737373737374"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="17.3737373737374"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="26.3232323232323"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="19.7777777777778"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="13.8989898989899"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="9.08585858585859"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="7.88383838383838"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="12.0252525252525"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="16.3030303030303"/>
+    <col collapsed="false" hidden="false" max="19" min="14" style="0" width="7.88383838383838"/>
+    <col collapsed="false" hidden="false" max="20" min="20" style="0" width="18.1717171717172"/>
+    <col collapsed="false" hidden="false" max="1025" min="21" style="0" width="7.88383838383838"/>
   </cols>
   <sheetData>
     <row r="1" s="6" customFormat="true" ht="17.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -37460,12 +37453,12 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="14.6969696969697"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="22.4494949494949"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="21.3787878787879"/>
-    <col collapsed="false" hidden="false" max="5" min="4" style="0" width="30.0656565656566"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="45.030303030303"/>
-    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="8.15151515151515"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="14.2979797979798"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="21.9141414141414"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="20.979797979798"/>
+    <col collapsed="false" hidden="false" max="5" min="4" style="0" width="29.2626262626263"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="43.9646464646465"/>
+    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="7.88383838383838"/>
   </cols>
   <sheetData>
     <row r="1" s="1" customFormat="true" ht="22.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -38145,20 +38138,20 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="1:111"/>
+  <dimension ref="1:112"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A59" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B66" activeCellId="0" sqref="B66"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C19" activeCellId="0" sqref="C19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="13.4949494949495"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="15.5"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="35.8131313131313"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="13.8989898989899"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="24.1868686868687"/>
-    <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="8.15151515151515"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="13.0959595959596"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="15.1010101010101"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="35.010101010101"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="13.4949494949495"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="23.520202020202"/>
+    <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="7.88383838383838"/>
   </cols>
   <sheetData>
     <row r="1" s="6" customFormat="true" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -38672,11 +38665,11 @@
         <v>245</v>
       </c>
     </row>
-    <row r="67" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B67" s="3" t="s">
+    <row r="66" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B66" s="3" t="s">
         <v>80</v>
       </c>
-      <c r="C67" s="3" t="s">
+      <c r="C66" s="3" t="s">
         <v>246</v>
       </c>
     </row>
@@ -38832,11 +38825,11 @@
         <v>265</v>
       </c>
     </row>
-    <row r="88" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B88" s="3" t="s">
+    <row r="87" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B87" s="3" t="s">
         <v>80</v>
       </c>
-      <c r="C88" s="3" t="s">
+      <c r="C87" s="3" t="s">
         <v>266</v>
       </c>
     </row>
@@ -38993,18 +38986,18 @@
       </c>
     </row>
     <row r="108" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B108" s="7" t="s">
+      <c r="B108" s="3" t="s">
         <v>80</v>
       </c>
-      <c r="C108" s="7" t="s">
+      <c r="C108" s="3" t="s">
         <v>286</v>
       </c>
     </row>
-    <row r="110" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B110" s="7" t="s">
+    <row r="109" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B109" s="7" t="s">
         <v>80</v>
       </c>
-      <c r="C110" s="13" t="s">
+      <c r="C109" s="7" t="s">
         <v>287</v>
       </c>
     </row>
@@ -39012,8 +39005,16 @@
       <c r="B111" s="7" t="s">
         <v>80</v>
       </c>
-      <c r="C111" s="7" t="s">
+      <c r="C111" s="3" t="s">
         <v>288</v>
+      </c>
+    </row>
+    <row r="112" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B112" s="7" t="s">
+        <v>80</v>
+      </c>
+      <c r="C112" s="7" t="s">
+        <v>289</v>
       </c>
     </row>
   </sheetData>
@@ -39040,14 +39041,14 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="35.010101010101"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="41.0252525252525"/>
-    <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="8.15151515151515"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="34.2070707070707"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="40.0909090909091"/>
+    <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="7.88383838383838"/>
   </cols>
   <sheetData>
     <row r="1" s="2" customFormat="true" ht="13.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
-        <v>289</v>
+        <v>290</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>68</v>
@@ -39055,26 +39056,26 @@
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="7" t="s">
-        <v>290</v>
+        <v>291</v>
       </c>
       <c r="B3" s="7" t="s">
-        <v>291</v>
+        <v>292</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="7" t="s">
-        <v>292</v>
+        <v>293</v>
       </c>
       <c r="B4" s="7" t="s">
-        <v>293</v>
+        <v>294</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="7" t="s">
-        <v>294</v>
+        <v>295</v>
       </c>
       <c r="B5" s="7" t="s">
-        <v>295</v>
+        <v>296</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
update Burmese and English for actor attributes
</commit_message>
<xml_diff>
--- a/tables/actor/forms/actor/actor.xlsx
+++ b/tables/actor/forms/actor/actor.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="968" firstSheet="0" activeTab="5"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="988" firstSheet="0" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="initial" sheetId="1" state="visible" r:id="rId2"/>
@@ -106,13 +106,16 @@
     <t xml:space="preserve">string_token</t>
   </si>
   <si>
+    <t xml:space="preserve">text.en</t>
+  </si>
+  <si>
     <t xml:space="preserve">text.my</t>
   </si>
   <si>
-    <t xml:space="preserve">text.en</t>
+    <t xml:space="preserve">node_attribute_A</t>
   </si>
   <si>
-    <t xml:space="preserve">node_attribute_A</t>
+    <t xml:space="preserve">Short Name: </t>
   </si>
   <si>
     <r>
@@ -136,19 +139,19 @@
     </r>
   </si>
   <si>
-    <t xml:space="preserve">Short Name: </t>
-  </si>
-  <si>
     <t xml:space="preserve">node_attribute_B</t>
   </si>
   <si>
-    <t xml:space="preserve">ခန့်မှန်းခြေအသက်</t>
+    <t xml:space="preserve">Approximate Age Currently:</t>
   </si>
   <si>
-    <t xml:space="preserve">Approximate Age:</t>
+    <t xml:space="preserve">ခန့်မှန်းခြေအသက် (ယခု):</t>
   </si>
   <si>
     <t xml:space="preserve">age_approximate_age</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Approximate age: Specify*</t>
   </si>
   <si>
     <r>
@@ -191,10 +194,10 @@
     </r>
   </si>
   <si>
-    <t xml:space="preserve">Approximate age: Specify*</t>
+    <t xml:space="preserve">age_birth_year_myanmar</t>
   </si>
   <si>
-    <t xml:space="preserve">age_birth_year_myanmar</t>
+    <t xml:space="preserve">Year of Birth: Myanmar BE Calendar*</t>
   </si>
   <si>
     <r>
@@ -256,10 +259,10 @@
     </r>
   </si>
   <si>
-    <t xml:space="preserve">Year of Birth: Myanmar BE Calendar*</t>
+    <t xml:space="preserve">age_birth_year_thailand</t>
   </si>
   <si>
-    <t xml:space="preserve">age_birth_year_thailand</t>
+    <t xml:space="preserve">Year of Birth: Thai BE*</t>
   </si>
   <si>
     <r>
@@ -321,10 +324,10 @@
     </r>
   </si>
   <si>
-    <t xml:space="preserve">Year of Birth: Thai BE*</t>
+    <t xml:space="preserve">age_birth_year_english</t>
   </si>
   <si>
-    <t xml:space="preserve">age_birth_year_english</t>
+    <t xml:space="preserve">Year of Birth: English Calendar*</t>
   </si>
   <si>
     <r>
@@ -386,10 +389,10 @@
     </r>
   </si>
   <si>
-    <t xml:space="preserve">Year of Birth: English Calendar*</t>
+    <t xml:space="preserve">node_attribute_C</t>
   </si>
   <si>
-    <t xml:space="preserve">node_attribute_C</t>
+    <t xml:space="preserve">Gender:</t>
   </si>
   <si>
     <r>
@@ -441,10 +444,10 @@
     </r>
   </si>
   <si>
-    <t xml:space="preserve">Gender:</t>
+    <t xml:space="preserve">other_gender</t>
   </si>
   <si>
-    <t xml:space="preserve">other_gender</t>
+    <t xml:space="preserve">Other: Specify*</t>
   </si>
   <si>
     <r>
@@ -487,10 +490,10 @@
     </r>
   </si>
   <si>
-    <t xml:space="preserve">Other: Specify*</t>
+    <t xml:space="preserve">node_attribute_D</t>
   </si>
   <si>
-    <t xml:space="preserve">node_attribute_D</t>
+    <t xml:space="preserve">Relationship to you: (check all that apply)</t>
   </si>
   <si>
     <r>
@@ -533,22 +536,22 @@
     </r>
   </si>
   <si>
-    <t xml:space="preserve">Relationship to you: (check all that apply)</t>
-  </si>
-  <si>
     <t xml:space="preserve">other_relationship</t>
   </si>
   <si>
     <t xml:space="preserve">node_attribute_E</t>
   </si>
   <si>
+    <t xml:space="preserve">How frequently do you go to this person when you need advice on personal matters?</t>
+  </si>
+  <si>
     <t xml:space="preserve">ကိုယ်ရေးကိုယ်တာ ကိစ္စတွေ အကြောင်း အကြံဉာဏ်လိုအပ်တဲ့အချိန်မှာ အဲ့ဒီသူဆီကို ဘယ်လောက်တစ်ကြိမ် သွားလေ့ ရှိခဲ့သလဲ။</t>
   </si>
   <si>
-    <t xml:space="preserve">How frequently do you go to this person when you need advice on personal matters?</t>
+    <t xml:space="preserve">node_attribute_F</t>
   </si>
   <si>
-    <t xml:space="preserve">node_attribute_F</t>
+    <t xml:space="preserve">Wealth compared to you before migration:</t>
   </si>
   <si>
     <r>
@@ -558,7 +561,7 @@
         <rFont val="Myanmar3"/>
         <family val="2"/>
       </rPr>
-      <t xml:space="preserve">ခင်ဗျားကိုယ်ပိုင်ပိုင်ဆိုင်မှုနဲ့ ဆက်စပ်ပြီး အဲ့ဒီလူရဲ့ ပိုင်ဆိုင်မှုကို ဘယ်လို ဖော်ပြနိုင်မလဲ။ </t>
+      <t xml:space="preserve">ခင်ဗျားမရွေ့ပြောင်းမှီအချိန်မှာခင်ဗျားကိုယ်ပိုင်ပိုင်ဆိုင်မှုနဲ့ ဆက်စပ်ပြီး အဲ့ဒီလူရဲ့ ပိုင်ဆိုင်မှုကို ဘယ်လို ဖော်ပြနိုင်မလဲ။ </t>
     </r>
     <r>
       <rPr>
@@ -589,9 +592,6 @@
       </rPr>
       <t xml:space="preserve">)</t>
     </r>
-  </si>
-  <si>
-    <t xml:space="preserve">Wealth compared to you:</t>
   </si>
   <si>
     <t xml:space="preserve">branch_label</t>
@@ -1754,11 +1754,11 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="12.5606060606061"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="7.61616161616162"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="15.9040404040404"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="35.9444444444444"/>
-    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="7.61616161616162"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="12.2929292929293"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="7.34848484848485"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="15.5"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="35.1464646464646"/>
+    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="7.34848484848485"/>
   </cols>
   <sheetData>
     <row r="1" s="2" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1815,14 +1815,14 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="12.2929292929293"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="11.6262626262626"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="23.3838383838384"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="20.8484848484848"/>
-    <col collapsed="false" hidden="false" max="7" min="5" style="0" width="7.88383838383838"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="22.9848484848485"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="18.4393939393939"/>
-    <col collapsed="false" hidden="false" max="1025" min="10" style="0" width="7.88383838383838"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="12.0252525252525"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="11.2272727272727"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="22.8484848484848"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="20.3131313131313"/>
+    <col collapsed="false" hidden="false" max="7" min="5" style="0" width="7.61616161616162"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="22.4494949494949"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="18.040404040404"/>
+    <col collapsed="false" hidden="false" max="1025" min="10" style="0" width="7.61616161616162"/>
   </cols>
   <sheetData>
     <row r="1" s="2" customFormat="true" ht="18.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1942,18 +1942,18 @@
   </sheetPr>
   <dimension ref="1:65"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C18" activeCellId="0" sqref="C18"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C20" activeCellId="0" sqref="C20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="3" width="27.2626262626263"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="3" width="42.2272727272727"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="3" width="63.6060606060606"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="3" width="42.4949494949495"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="3" width="72.1616161616162"/>
-    <col collapsed="false" hidden="false" max="1025" min="6" style="3" width="3.74242424242424"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="3" width="26.5909090909091"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="3" width="41.2929292929293"/>
+    <col collapsed="false" hidden="false" max="4" min="3" style="3" width="62.1363636363636"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="3" width="70.5555555555556"/>
+    <col collapsed="false" hidden="false" max="1023" min="6" style="3" width="3.60606060606061"/>
+    <col collapsed="false" hidden="false" max="1025" min="1024" style="0" width="3.60606060606061"/>
   </cols>
   <sheetData>
     <row r="1" s="1" customFormat="true" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1971,6 +1971,7 @@
       </c>
       <c r="E1" s="10"/>
       <c r="F1" s="10"/>
+      <c r="AMJ1" s="0"/>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0"/>
@@ -2996,17 +2997,16 @@
       <c r="AMG2" s="0"/>
       <c r="AMH2" s="0"/>
       <c r="AMI2" s="0"/>
-      <c r="AMJ2" s="0"/>
     </row>
     <row r="3" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="4"/>
       <c r="B3" s="9" t="s">
         <v>28</v>
       </c>
-      <c r="C3" s="8" t="s">
+      <c r="C3" s="9" t="s">
         <v>29</v>
       </c>
-      <c r="D3" s="9" t="s">
+      <c r="D3" s="8" t="s">
         <v>30</v>
       </c>
       <c r="E3" s="8"/>
@@ -4028,17 +4028,16 @@
       <c r="AMG3" s="0"/>
       <c r="AMH3" s="0"/>
       <c r="AMI3" s="0"/>
-      <c r="AMJ3" s="0"/>
     </row>
     <row r="4" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="4"/>
       <c r="B4" s="9" t="s">
         <v>31</v>
       </c>
-      <c r="C4" s="8" t="s">
+      <c r="C4" s="9" t="s">
         <v>32</v>
       </c>
-      <c r="D4" s="9" t="s">
+      <c r="D4" s="8" t="s">
         <v>33</v>
       </c>
       <c r="E4" s="8"/>
@@ -5060,17 +5059,16 @@
       <c r="AMG4" s="0"/>
       <c r="AMH4" s="0"/>
       <c r="AMI4" s="0"/>
-      <c r="AMJ4" s="0"/>
     </row>
     <row r="5" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0"/>
       <c r="B5" s="9" t="s">
         <v>34</v>
       </c>
-      <c r="C5" s="8" t="s">
+      <c r="C5" s="9" t="s">
         <v>35</v>
       </c>
-      <c r="D5" s="9" t="s">
+      <c r="D5" s="8" t="s">
         <v>36</v>
       </c>
       <c r="E5" s="8"/>
@@ -6092,17 +6090,16 @@
       <c r="AMG5" s="0"/>
       <c r="AMH5" s="0"/>
       <c r="AMI5" s="0"/>
-      <c r="AMJ5" s="0"/>
     </row>
     <row r="6" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0"/>
       <c r="B6" s="9" t="s">
         <v>37</v>
       </c>
-      <c r="C6" s="8" t="s">
+      <c r="C6" s="9" t="s">
         <v>38</v>
       </c>
-      <c r="D6" s="9" t="s">
+      <c r="D6" s="8" t="s">
         <v>39</v>
       </c>
       <c r="E6" s="8"/>
@@ -7124,17 +7121,16 @@
       <c r="AMG6" s="0"/>
       <c r="AMH6" s="0"/>
       <c r="AMI6" s="0"/>
-      <c r="AMJ6" s="0"/>
     </row>
     <row r="7" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0"/>
       <c r="B7" s="9" t="s">
         <v>40</v>
       </c>
-      <c r="C7" s="8" t="s">
+      <c r="C7" s="9" t="s">
         <v>41</v>
       </c>
-      <c r="D7" s="9" t="s">
+      <c r="D7" s="8" t="s">
         <v>42</v>
       </c>
       <c r="E7" s="8"/>
@@ -8156,17 +8152,16 @@
       <c r="AMG7" s="0"/>
       <c r="AMH7" s="0"/>
       <c r="AMI7" s="0"/>
-      <c r="AMJ7" s="0"/>
     </row>
     <row r="8" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0"/>
       <c r="B8" s="9" t="s">
         <v>43</v>
       </c>
-      <c r="C8" s="8" t="s">
+      <c r="C8" s="9" t="s">
         <v>44</v>
       </c>
-      <c r="D8" s="9" t="s">
+      <c r="D8" s="8" t="s">
         <v>45</v>
       </c>
       <c r="E8" s="8"/>
@@ -9188,17 +9183,16 @@
       <c r="AMG8" s="0"/>
       <c r="AMH8" s="0"/>
       <c r="AMI8" s="0"/>
-      <c r="AMJ8" s="0"/>
     </row>
     <row r="9" customFormat="false" ht="14.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A9" s="0"/>
       <c r="B9" s="9" t="s">
         <v>46</v>
       </c>
-      <c r="C9" s="8" t="s">
+      <c r="C9" s="9" t="s">
         <v>47</v>
       </c>
-      <c r="D9" s="9" t="s">
+      <c r="D9" s="8" t="s">
         <v>48</v>
       </c>
       <c r="E9" s="8"/>
@@ -10220,17 +10214,16 @@
       <c r="AMG9" s="0"/>
       <c r="AMH9" s="0"/>
       <c r="AMI9" s="0"/>
-      <c r="AMJ9" s="0"/>
     </row>
     <row r="10" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0"/>
       <c r="B10" s="9" t="s">
         <v>49</v>
       </c>
-      <c r="C10" s="8" t="s">
+      <c r="C10" s="9" t="s">
         <v>50</v>
       </c>
-      <c r="D10" s="9" t="s">
+      <c r="D10" s="8" t="s">
         <v>51</v>
       </c>
       <c r="E10" s="8"/>
@@ -11252,17 +11245,16 @@
       <c r="AMG10" s="0"/>
       <c r="AMH10" s="0"/>
       <c r="AMI10" s="0"/>
-      <c r="AMJ10" s="0"/>
     </row>
     <row r="11" customFormat="false" ht="15.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A11" s="0"/>
       <c r="B11" s="9" t="s">
         <v>52</v>
       </c>
-      <c r="C11" s="8" t="s">
+      <c r="C11" s="9" t="s">
         <v>53</v>
       </c>
-      <c r="D11" s="9" t="s">
+      <c r="D11" s="8" t="s">
         <v>54</v>
       </c>
       <c r="E11" s="8"/>
@@ -12284,17 +12276,16 @@
       <c r="AMG11" s="0"/>
       <c r="AMH11" s="0"/>
       <c r="AMI11" s="0"/>
-      <c r="AMJ11" s="0"/>
     </row>
     <row r="12" customFormat="false" ht="15.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A12" s="0"/>
       <c r="B12" s="9" t="s">
         <v>55</v>
       </c>
-      <c r="C12" s="8" t="s">
+      <c r="C12" s="9" t="s">
         <v>50</v>
       </c>
-      <c r="D12" s="9" t="s">
+      <c r="D12" s="8" t="s">
         <v>51</v>
       </c>
       <c r="E12" s="8"/>
@@ -13316,17 +13307,16 @@
       <c r="AMG12" s="0"/>
       <c r="AMH12" s="0"/>
       <c r="AMI12" s="0"/>
-      <c r="AMJ12" s="0"/>
     </row>
     <row r="13" customFormat="false" ht="27.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A13" s="0"/>
       <c r="B13" s="9" t="s">
         <v>56</v>
       </c>
-      <c r="C13" s="8" t="s">
+      <c r="C13" s="9" t="s">
         <v>57</v>
       </c>
-      <c r="D13" s="9" t="s">
+      <c r="D13" s="8" t="s">
         <v>58</v>
       </c>
       <c r="E13" s="8"/>
@@ -14348,17 +14338,16 @@
       <c r="AMG13" s="0"/>
       <c r="AMH13" s="0"/>
       <c r="AMI13" s="0"/>
-      <c r="AMJ13" s="0"/>
     </row>
     <row r="14" customFormat="false" ht="17.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A14" s="0"/>
       <c r="B14" s="9" t="s">
         <v>59</v>
       </c>
-      <c r="C14" s="8" t="s">
+      <c r="C14" s="9" t="s">
         <v>60</v>
       </c>
-      <c r="D14" s="9" t="s">
+      <c r="D14" s="8" t="s">
         <v>61</v>
       </c>
       <c r="E14" s="8"/>
@@ -15380,7 +15369,6 @@
       <c r="AMG14" s="0"/>
       <c r="AMH14" s="0"/>
       <c r="AMI14" s="0"/>
-      <c r="AMJ14" s="0"/>
     </row>
     <row r="15" customFormat="false" ht="12.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A15" s="0"/>
@@ -16406,7 +16394,6 @@
       <c r="AMG15" s="0"/>
       <c r="AMH15" s="0"/>
       <c r="AMI15" s="0"/>
-      <c r="AMJ15" s="0"/>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="0"/>
@@ -17432,7 +17419,6 @@
       <c r="AMG16" s="0"/>
       <c r="AMH16" s="0"/>
       <c r="AMI16" s="0"/>
-      <c r="AMJ16" s="0"/>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="0"/>
@@ -18458,13 +18444,12 @@
       <c r="AMG17" s="0"/>
       <c r="AMH17" s="0"/>
       <c r="AMI17" s="0"/>
-      <c r="AMJ17" s="0"/>
     </row>
-    <row r="18" customFormat="false" ht="14.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="18" customFormat="false" ht="65.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A18" s="0"/>
-      <c r="B18" s="8"/>
-      <c r="C18" s="8"/>
-      <c r="D18" s="8"/>
+      <c r="B18" s="9"/>
+      <c r="C18" s="0"/>
+      <c r="D18" s="0"/>
       <c r="E18" s="0"/>
       <c r="F18" s="0"/>
       <c r="G18" s="0"/>
@@ -19484,7 +19469,6 @@
       <c r="AMG18" s="0"/>
       <c r="AMH18" s="0"/>
       <c r="AMI18" s="0"/>
-      <c r="AMJ18" s="0"/>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="0"/>
@@ -20510,7 +20494,6 @@
       <c r="AMG19" s="0"/>
       <c r="AMH19" s="0"/>
       <c r="AMI19" s="0"/>
-      <c r="AMJ19" s="0"/>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="0"/>
@@ -21536,13 +21519,12 @@
       <c r="AMG20" s="0"/>
       <c r="AMH20" s="0"/>
       <c r="AMI20" s="0"/>
-      <c r="AMJ20" s="0"/>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="0"/>
       <c r="B21" s="0"/>
       <c r="C21" s="0"/>
-      <c r="D21" s="8"/>
+      <c r="D21" s="0"/>
       <c r="E21" s="0"/>
       <c r="F21" s="0"/>
       <c r="G21" s="0"/>
@@ -22562,7 +22544,6 @@
       <c r="AMG21" s="0"/>
       <c r="AMH21" s="0"/>
       <c r="AMI21" s="0"/>
-      <c r="AMJ21" s="0"/>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="0"/>
@@ -23588,7 +23569,6 @@
       <c r="AMG22" s="0"/>
       <c r="AMH22" s="0"/>
       <c r="AMI22" s="0"/>
-      <c r="AMJ22" s="0"/>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="0"/>
@@ -24614,7 +24594,6 @@
       <c r="AMG23" s="0"/>
       <c r="AMH23" s="0"/>
       <c r="AMI23" s="0"/>
-      <c r="AMJ23" s="0"/>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="0"/>
@@ -25640,13 +25619,12 @@
       <c r="AMG24" s="0"/>
       <c r="AMH24" s="0"/>
       <c r="AMI24" s="0"/>
-      <c r="AMJ24" s="0"/>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="0"/>
       <c r="B25" s="4"/>
       <c r="C25" s="4"/>
-      <c r="D25" s="8"/>
+      <c r="D25" s="4"/>
       <c r="E25" s="0"/>
       <c r="F25" s="0"/>
       <c r="G25" s="0"/>
@@ -26666,13 +26644,12 @@
       <c r="AMG25" s="0"/>
       <c r="AMH25" s="0"/>
       <c r="AMI25" s="0"/>
-      <c r="AMJ25" s="0"/>
     </row>
     <row r="26" customFormat="false" ht="29.2" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A26" s="0"/>
       <c r="B26" s="4"/>
       <c r="C26" s="4"/>
-      <c r="D26" s="8"/>
+      <c r="D26" s="4"/>
       <c r="E26" s="0"/>
       <c r="F26" s="0"/>
       <c r="G26" s="0"/>
@@ -27692,7 +27669,6 @@
       <c r="AMG26" s="0"/>
       <c r="AMH26" s="0"/>
       <c r="AMI26" s="0"/>
-      <c r="AMJ26" s="0"/>
     </row>
     <row r="27" customFormat="false" ht="23.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A27" s="0"/>
@@ -28718,13 +28694,12 @@
       <c r="AMG27" s="0"/>
       <c r="AMH27" s="0"/>
       <c r="AMI27" s="0"/>
-      <c r="AMJ27" s="0"/>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="0"/>
       <c r="B28" s="4"/>
       <c r="C28" s="4"/>
-      <c r="D28" s="0"/>
+      <c r="D28" s="4"/>
       <c r="E28" s="0"/>
       <c r="F28" s="0"/>
       <c r="G28" s="0"/>
@@ -29744,13 +29719,12 @@
       <c r="AMG28" s="0"/>
       <c r="AMH28" s="0"/>
       <c r="AMI28" s="0"/>
-      <c r="AMJ28" s="0"/>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="0"/>
       <c r="B29" s="4"/>
       <c r="C29" s="4"/>
-      <c r="D29" s="8"/>
+      <c r="D29" s="4"/>
       <c r="E29" s="0"/>
       <c r="F29" s="0"/>
       <c r="G29" s="0"/>
@@ -30770,13 +30744,12 @@
       <c r="AMG29" s="0"/>
       <c r="AMH29" s="0"/>
       <c r="AMI29" s="0"/>
-      <c r="AMJ29" s="0"/>
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="0"/>
       <c r="B30" s="4"/>
       <c r="C30" s="4"/>
-      <c r="D30" s="8"/>
+      <c r="D30" s="4"/>
       <c r="E30" s="0"/>
       <c r="F30" s="0"/>
       <c r="G30" s="0"/>
@@ -31796,13 +31769,12 @@
       <c r="AMG30" s="0"/>
       <c r="AMH30" s="0"/>
       <c r="AMI30" s="0"/>
-      <c r="AMJ30" s="0"/>
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="0"/>
       <c r="B31" s="4"/>
       <c r="C31" s="4"/>
-      <c r="D31" s="8"/>
+      <c r="D31" s="4"/>
       <c r="E31" s="0"/>
       <c r="F31" s="0"/>
       <c r="G31" s="0"/>
@@ -32822,13 +32794,12 @@
       <c r="AMG31" s="0"/>
       <c r="AMH31" s="0"/>
       <c r="AMI31" s="0"/>
-      <c r="AMJ31" s="0"/>
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="0"/>
       <c r="B32" s="4"/>
       <c r="C32" s="4"/>
-      <c r="D32" s="8"/>
+      <c r="D32" s="4"/>
       <c r="E32" s="0"/>
       <c r="F32" s="0"/>
       <c r="G32" s="0"/>
@@ -33848,7 +33819,6 @@
       <c r="AMG32" s="0"/>
       <c r="AMH32" s="0"/>
       <c r="AMI32" s="0"/>
-      <c r="AMJ32" s="0"/>
     </row>
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="0"/>
@@ -34874,13 +34844,12 @@
       <c r="AMG33" s="0"/>
       <c r="AMH33" s="0"/>
       <c r="AMI33" s="0"/>
-      <c r="AMJ33" s="0"/>
     </row>
     <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="0"/>
       <c r="B34" s="4"/>
       <c r="C34" s="4"/>
-      <c r="D34" s="8"/>
+      <c r="D34" s="4"/>
       <c r="E34" s="0"/>
       <c r="F34" s="0"/>
       <c r="G34" s="0"/>
@@ -35900,7 +35869,6 @@
       <c r="AMG34" s="0"/>
       <c r="AMH34" s="0"/>
       <c r="AMI34" s="0"/>
-      <c r="AMJ34" s="0"/>
     </row>
     <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="0"/>
@@ -36926,10 +36894,9 @@
       <c r="AMG35" s="0"/>
       <c r="AMH35" s="0"/>
       <c r="AMI35" s="0"/>
-      <c r="AMJ35" s="0"/>
     </row>
     <row r="36" s="4" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D36" s="8"/>
+      <c r="AMJ36" s="0"/>
     </row>
     <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="0"/>
@@ -37129,22 +37096,22 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="7.88383838383838"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="10.959595959596"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="9.22222222222222"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="33.540404040404"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="19.3737373737374"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="17.3737373737374"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="26.3232323232323"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="19.7777777777778"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="13.8989898989899"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="9.08585858585859"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="7.88383838383838"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="12.0252525252525"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="16.3030303030303"/>
-    <col collapsed="false" hidden="false" max="19" min="14" style="0" width="7.88383838383838"/>
-    <col collapsed="false" hidden="false" max="20" min="20" style="0" width="18.1717171717172"/>
-    <col collapsed="false" hidden="false" max="1025" min="21" style="0" width="7.88383838383838"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="7.61616161616162"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="10.6919191919192"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="9.08585858585859"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="32.8737373737374"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="18.9747474747475"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="16.969696969697"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="25.6565656565657"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="19.2424242424242"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="13.4949494949495"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="8.95454545454546"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="7.61616161616162"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="11.6262626262626"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="15.9040404040404"/>
+    <col collapsed="false" hidden="false" max="19" min="14" style="0" width="7.61616161616162"/>
+    <col collapsed="false" hidden="false" max="20" min="20" style="0" width="17.6414141414141"/>
+    <col collapsed="false" hidden="false" max="1025" min="21" style="0" width="7.61616161616162"/>
   </cols>
   <sheetData>
     <row r="1" s="6" customFormat="true" ht="17.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -37453,12 +37420,12 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="14.2979797979798"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="21.9141414141414"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="20.979797979798"/>
-    <col collapsed="false" hidden="false" max="5" min="4" style="0" width="29.2626262626263"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="43.9646464646465"/>
-    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="7.88383838383838"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="13.8989898989899"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="21.3787878787879"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="20.4444444444444"/>
+    <col collapsed="false" hidden="false" max="5" min="4" style="0" width="28.5959595959596"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="43.030303030303"/>
+    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="7.61616161616162"/>
   </cols>
   <sheetData>
     <row r="1" s="1" customFormat="true" ht="22.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -37486,10 +37453,10 @@
         <v>101</v>
       </c>
       <c r="D3" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="E3" s="9" t="s">
         <v>35</v>
-      </c>
-      <c r="E3" s="9" t="s">
-        <v>36</v>
       </c>
       <c r="F3" s="8"/>
     </row>
@@ -37568,10 +37535,10 @@
         <v>114</v>
       </c>
       <c r="D9" s="8" t="s">
+        <v>51</v>
+      </c>
+      <c r="E9" s="9" t="s">
         <v>50</v>
-      </c>
-      <c r="E9" s="9" t="s">
-        <v>51</v>
       </c>
       <c r="F9" s="8"/>
     </row>
@@ -37913,10 +37880,10 @@
         <v>114</v>
       </c>
       <c r="D33" s="8" t="s">
+        <v>51</v>
+      </c>
+      <c r="E33" s="9" t="s">
         <v>50</v>
-      </c>
-      <c r="E33" s="9" t="s">
-        <v>51</v>
       </c>
       <c r="F33" s="8"/>
     </row>
@@ -38140,18 +38107,18 @@
   </sheetPr>
   <dimension ref="1:112"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="C19" activeCellId="0" sqref="C19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="13.0959595959596"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="15.1010101010101"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="35.010101010101"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="13.4949494949495"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="23.520202020202"/>
-    <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="7.88383838383838"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="12.8282828282828"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="14.6969696969697"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="34.2070707070707"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="13.0959595959596"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="22.9848484848485"/>
+    <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="7.61616161616162"/>
   </cols>
   <sheetData>
     <row r="1" s="6" customFormat="true" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -39041,9 +39008,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="34.2070707070707"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="40.0909090909091"/>
-    <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="7.88383838383838"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="33.4090909090909"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="39.2878787878788"/>
+    <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="7.61616161616162"/>
   </cols>
   <sheetData>
     <row r="1" s="2" customFormat="true" ht="13.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">

</xml_diff>

<commit_message>
update answers and prompts
</commit_message>
<xml_diff>
--- a/tables/actor/forms/actor/actor.xlsx
+++ b/tables/actor/forms/actor/actor.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="968" firstSheet="0" activeTab="5"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="988" firstSheet="0" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="initial" sheetId="1" state="visible" r:id="rId2"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="529" uniqueCount="297">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="533" uniqueCount="299">
   <si>
     <t xml:space="preserve">clause</t>
   </si>
@@ -106,13 +106,16 @@
     <t xml:space="preserve">string_token</t>
   </si>
   <si>
+    <t xml:space="preserve">text.en</t>
+  </si>
+  <si>
     <t xml:space="preserve">text.my</t>
   </si>
   <si>
-    <t xml:space="preserve">text.en</t>
+    <t xml:space="preserve">node_attribute_A</t>
   </si>
   <si>
-    <t xml:space="preserve">node_attribute_A</t>
+    <t xml:space="preserve">Short Name: </t>
   </si>
   <si>
     <r>
@@ -136,19 +139,56 @@
     </r>
   </si>
   <si>
-    <t xml:space="preserve">Short Name: </t>
-  </si>
-  <si>
     <t xml:space="preserve">node_attribute_B</t>
   </si>
   <si>
-    <t xml:space="preserve">ခန့်မှန်းခြေအသက်</t>
+    <t xml:space="preserve">Approximate Age Currently</t>
   </si>
   <si>
-    <t xml:space="preserve">Approximate Age:</t>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Myanmar3"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">ခန့်မှန်းခြေအသက် </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Myanmar3"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">(</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Myanmar3"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">ယခု</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Myanmar3"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">)</t>
+    </r>
   </si>
   <si>
     <t xml:space="preserve">age_approximate_age</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Approximate age: Specify*</t>
   </si>
   <si>
     <r>
@@ -191,10 +231,10 @@
     </r>
   </si>
   <si>
-    <t xml:space="preserve">Approximate age: Specify*</t>
+    <t xml:space="preserve">age_birth_year_myanmar</t>
   </si>
   <si>
-    <t xml:space="preserve">age_birth_year_myanmar</t>
+    <t xml:space="preserve">Year of Birth: Myanmar BE Calendar*</t>
   </si>
   <si>
     <r>
@@ -256,10 +296,10 @@
     </r>
   </si>
   <si>
-    <t xml:space="preserve">Year of Birth: Myanmar BE Calendar*</t>
+    <t xml:space="preserve">age_birth_year_thailand</t>
   </si>
   <si>
-    <t xml:space="preserve">age_birth_year_thailand</t>
+    <t xml:space="preserve">Year of Birth: Thai BE*</t>
   </si>
   <si>
     <r>
@@ -321,10 +361,10 @@
     </r>
   </si>
   <si>
-    <t xml:space="preserve">Year of Birth: Thai BE*</t>
+    <t xml:space="preserve">age_birth_year_english</t>
   </si>
   <si>
-    <t xml:space="preserve">age_birth_year_english</t>
+    <t xml:space="preserve">Year of Birth: English Calendar*</t>
   </si>
   <si>
     <r>
@@ -386,10 +426,10 @@
     </r>
   </si>
   <si>
-    <t xml:space="preserve">Year of Birth: English Calendar*</t>
+    <t xml:space="preserve">node_attribute_C</t>
   </si>
   <si>
-    <t xml:space="preserve">node_attribute_C</t>
+    <t xml:space="preserve">Gender:</t>
   </si>
   <si>
     <r>
@@ -441,10 +481,10 @@
     </r>
   </si>
   <si>
-    <t xml:space="preserve">Gender:</t>
+    <t xml:space="preserve">other_gender</t>
   </si>
   <si>
-    <t xml:space="preserve">other_gender</t>
+    <t xml:space="preserve">Other: Specify*</t>
   </si>
   <si>
     <r>
@@ -487,10 +527,10 @@
     </r>
   </si>
   <si>
-    <t xml:space="preserve">Other: Specify*</t>
+    <t xml:space="preserve">node_attribute_D</t>
   </si>
   <si>
-    <t xml:space="preserve">node_attribute_D</t>
+    <t xml:space="preserve">Relationship to you: (check all that apply)</t>
   </si>
   <si>
     <r>
@@ -533,22 +573,22 @@
     </r>
   </si>
   <si>
-    <t xml:space="preserve">Relationship to you: (check all that apply)</t>
-  </si>
-  <si>
     <t xml:space="preserve">other_relationship</t>
   </si>
   <si>
     <t xml:space="preserve">node_attribute_E</t>
   </si>
   <si>
+    <t xml:space="preserve">How frequently do you go to this person when you need advice on personal matters?</t>
+  </si>
+  <si>
     <t xml:space="preserve">ကိုယ်ရေးကိုယ်တာ ကိစ္စတွေ အကြောင်း အကြံဉာဏ်လိုအပ်တဲ့အချိန်မှာ အဲ့ဒီသူဆီကို ဘယ်လောက်တစ်ကြိမ် သွားလေ့ ရှိခဲ့သလဲ။</t>
   </si>
   <si>
-    <t xml:space="preserve">How frequently do you go to this person when you need advice on personal matters?</t>
+    <t xml:space="preserve">node_attribute_F</t>
   </si>
   <si>
-    <t xml:space="preserve">node_attribute_F</t>
+    <t xml:space="preserve">Wealth compared to you before migration:</t>
   </si>
   <si>
     <r>
@@ -558,7 +598,7 @@
         <rFont val="Myanmar3"/>
         <family val="2"/>
       </rPr>
-      <t xml:space="preserve">ခင်ဗျားကိုယ်ပိုင်ပိုင်ဆိုင်မှုနဲ့ ဆက်စပ်ပြီး အဲ့ဒီလူရဲ့ ပိုင်ဆိုင်မှုကို ဘယ်လို ဖော်ပြနိုင်မလဲ။ </t>
+      <t xml:space="preserve">ခင်ဗျားမရွေ့ပြောင်းမှီအချိန်မှာခင်ဗျားကိုယ်ပိုင်ပိုင်ဆိုင်မှုနဲ့ ဆက်စပ်ပြီး အဲ့ဒီလူရဲ့ ပိုင်ဆိုင်မှုကို ဘယ်လို ဖော်ပြနိုင်မလဲ။ </t>
     </r>
     <r>
       <rPr>
@@ -589,9 +629,6 @@
       </rPr>
       <t xml:space="preserve">)</t>
     </r>
-  </si>
-  <si>
-    <t xml:space="preserve">Wealth compared to you:</t>
   </si>
   <si>
     <t xml:space="preserve">branch_label</t>
@@ -1023,6 +1060,12 @@
   </si>
   <si>
     <t xml:space="preserve">ပွဲစား</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Any type of Agent </t>
+  </si>
+  <si>
+    <t xml:space="preserve">ရွေ့ပြောင်းမှုတွင်အကျိုးဆောင်သူအားလုံး </t>
   </si>
   <si>
     <t xml:space="preserve">never</t>
@@ -1754,11 +1797,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="12.5606060606061"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="7.61616161616162"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="15.9040404040404"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="35.9444444444444"/>
-    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="7.61616161616162"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="12.0252525252525"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="15.1010101010101"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="34.3434343434343"/>
   </cols>
   <sheetData>
     <row r="1" s="2" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1815,14 +1856,14 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="12.2929292929293"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="11.6262626262626"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="23.3838383838384"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="20.8484848484848"/>
-    <col collapsed="false" hidden="false" max="7" min="5" style="0" width="7.88383838383838"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="22.9848484848485"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="18.4393939393939"/>
-    <col collapsed="false" hidden="false" max="1025" min="10" style="0" width="7.88383838383838"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="11.6262626262626"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="10.959595959596"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="22.3181818181818"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="19.7777777777778"/>
+    <col collapsed="false" hidden="false" max="7" min="5" style="0" width="7.34848484848485"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="21.9141414141414"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="17.5050505050505"/>
+    <col collapsed="false" hidden="false" max="1025" min="10" style="0" width="7.34848484848485"/>
   </cols>
   <sheetData>
     <row r="1" s="2" customFormat="true" ht="18.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1943,17 +1984,17 @@
   <dimension ref="1:65"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C18" activeCellId="0" sqref="C18"/>
+      <selection pane="topLeft" activeCell="C14" activeCellId="0" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="3" width="27.2626262626263"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="3" width="42.2272727272727"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="3" width="63.6060606060606"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="3" width="42.4949494949495"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="3" width="72.1616161616162"/>
-    <col collapsed="false" hidden="false" max="1025" min="6" style="3" width="3.74242424242424"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="3" width="25.9242424242424"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="3" width="40.3535353535354"/>
+    <col collapsed="false" hidden="false" max="4" min="3" style="3" width="60.8030303030303"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="3" width="69.0858585858586"/>
+    <col collapsed="false" hidden="false" max="1023" min="6" style="3" width="3.47474747474747"/>
+    <col collapsed="false" hidden="false" max="1025" min="1024" style="0" width="3.47474747474747"/>
   </cols>
   <sheetData>
     <row r="1" s="1" customFormat="true" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1971,6 +2012,7 @@
       </c>
       <c r="E1" s="10"/>
       <c r="F1" s="10"/>
+      <c r="AMJ1" s="0"/>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0"/>
@@ -2996,17 +3038,16 @@
       <c r="AMG2" s="0"/>
       <c r="AMH2" s="0"/>
       <c r="AMI2" s="0"/>
-      <c r="AMJ2" s="0"/>
     </row>
     <row r="3" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="4"/>
       <c r="B3" s="9" t="s">
         <v>28</v>
       </c>
-      <c r="C3" s="8" t="s">
+      <c r="C3" s="9" t="s">
         <v>29</v>
       </c>
-      <c r="D3" s="9" t="s">
+      <c r="D3" s="8" t="s">
         <v>30</v>
       </c>
       <c r="E3" s="8"/>
@@ -4028,17 +4069,16 @@
       <c r="AMG3" s="0"/>
       <c r="AMH3" s="0"/>
       <c r="AMI3" s="0"/>
-      <c r="AMJ3" s="0"/>
     </row>
-    <row r="4" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="4" customFormat="false" ht="14.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="4"/>
       <c r="B4" s="9" t="s">
         <v>31</v>
       </c>
-      <c r="C4" s="8" t="s">
+      <c r="C4" s="9" t="s">
         <v>32</v>
       </c>
-      <c r="D4" s="9" t="s">
+      <c r="D4" s="8" t="s">
         <v>33</v>
       </c>
       <c r="E4" s="8"/>
@@ -5060,17 +5100,16 @@
       <c r="AMG4" s="0"/>
       <c r="AMH4" s="0"/>
       <c r="AMI4" s="0"/>
-      <c r="AMJ4" s="0"/>
     </row>
     <row r="5" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0"/>
       <c r="B5" s="9" t="s">
         <v>34</v>
       </c>
-      <c r="C5" s="8" t="s">
+      <c r="C5" s="9" t="s">
         <v>35</v>
       </c>
-      <c r="D5" s="9" t="s">
+      <c r="D5" s="8" t="s">
         <v>36</v>
       </c>
       <c r="E5" s="8"/>
@@ -6092,17 +6131,16 @@
       <c r="AMG5" s="0"/>
       <c r="AMH5" s="0"/>
       <c r="AMI5" s="0"/>
-      <c r="AMJ5" s="0"/>
     </row>
     <row r="6" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0"/>
       <c r="B6" s="9" t="s">
         <v>37</v>
       </c>
-      <c r="C6" s="8" t="s">
+      <c r="C6" s="9" t="s">
         <v>38</v>
       </c>
-      <c r="D6" s="9" t="s">
+      <c r="D6" s="8" t="s">
         <v>39</v>
       </c>
       <c r="E6" s="8"/>
@@ -7124,17 +7162,16 @@
       <c r="AMG6" s="0"/>
       <c r="AMH6" s="0"/>
       <c r="AMI6" s="0"/>
-      <c r="AMJ6" s="0"/>
     </row>
     <row r="7" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0"/>
       <c r="B7" s="9" t="s">
         <v>40</v>
       </c>
-      <c r="C7" s="8" t="s">
+      <c r="C7" s="9" t="s">
         <v>41</v>
       </c>
-      <c r="D7" s="9" t="s">
+      <c r="D7" s="8" t="s">
         <v>42</v>
       </c>
       <c r="E7" s="8"/>
@@ -8156,17 +8193,16 @@
       <c r="AMG7" s="0"/>
       <c r="AMH7" s="0"/>
       <c r="AMI7" s="0"/>
-      <c r="AMJ7" s="0"/>
     </row>
     <row r="8" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0"/>
       <c r="B8" s="9" t="s">
         <v>43</v>
       </c>
-      <c r="C8" s="8" t="s">
+      <c r="C8" s="9" t="s">
         <v>44</v>
       </c>
-      <c r="D8" s="9" t="s">
+      <c r="D8" s="8" t="s">
         <v>45</v>
       </c>
       <c r="E8" s="8"/>
@@ -9188,17 +9224,16 @@
       <c r="AMG8" s="0"/>
       <c r="AMH8" s="0"/>
       <c r="AMI8" s="0"/>
-      <c r="AMJ8" s="0"/>
     </row>
     <row r="9" customFormat="false" ht="14.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A9" s="0"/>
       <c r="B9" s="9" t="s">
         <v>46</v>
       </c>
-      <c r="C9" s="8" t="s">
+      <c r="C9" s="9" t="s">
         <v>47</v>
       </c>
-      <c r="D9" s="9" t="s">
+      <c r="D9" s="8" t="s">
         <v>48</v>
       </c>
       <c r="E9" s="8"/>
@@ -10220,17 +10255,16 @@
       <c r="AMG9" s="0"/>
       <c r="AMH9" s="0"/>
       <c r="AMI9" s="0"/>
-      <c r="AMJ9" s="0"/>
     </row>
     <row r="10" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0"/>
       <c r="B10" s="9" t="s">
         <v>49</v>
       </c>
-      <c r="C10" s="8" t="s">
+      <c r="C10" s="9" t="s">
         <v>50</v>
       </c>
-      <c r="D10" s="9" t="s">
+      <c r="D10" s="8" t="s">
         <v>51</v>
       </c>
       <c r="E10" s="8"/>
@@ -11252,17 +11286,16 @@
       <c r="AMG10" s="0"/>
       <c r="AMH10" s="0"/>
       <c r="AMI10" s="0"/>
-      <c r="AMJ10" s="0"/>
     </row>
     <row r="11" customFormat="false" ht="15.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A11" s="0"/>
       <c r="B11" s="9" t="s">
         <v>52</v>
       </c>
-      <c r="C11" s="8" t="s">
+      <c r="C11" s="9" t="s">
         <v>53</v>
       </c>
-      <c r="D11" s="9" t="s">
+      <c r="D11" s="8" t="s">
         <v>54</v>
       </c>
       <c r="E11" s="8"/>
@@ -12284,17 +12317,16 @@
       <c r="AMG11" s="0"/>
       <c r="AMH11" s="0"/>
       <c r="AMI11" s="0"/>
-      <c r="AMJ11" s="0"/>
     </row>
     <row r="12" customFormat="false" ht="15.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A12" s="0"/>
       <c r="B12" s="9" t="s">
         <v>55</v>
       </c>
-      <c r="C12" s="8" t="s">
+      <c r="C12" s="9" t="s">
         <v>50</v>
       </c>
-      <c r="D12" s="9" t="s">
+      <c r="D12" s="8" t="s">
         <v>51</v>
       </c>
       <c r="E12" s="8"/>
@@ -13316,17 +13348,16 @@
       <c r="AMG12" s="0"/>
       <c r="AMH12" s="0"/>
       <c r="AMI12" s="0"/>
-      <c r="AMJ12" s="0"/>
     </row>
     <row r="13" customFormat="false" ht="27.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A13" s="0"/>
       <c r="B13" s="9" t="s">
         <v>56</v>
       </c>
-      <c r="C13" s="8" t="s">
+      <c r="C13" s="9" t="s">
         <v>57</v>
       </c>
-      <c r="D13" s="9" t="s">
+      <c r="D13" s="8" t="s">
         <v>58</v>
       </c>
       <c r="E13" s="8"/>
@@ -14348,17 +14379,16 @@
       <c r="AMG13" s="0"/>
       <c r="AMH13" s="0"/>
       <c r="AMI13" s="0"/>
-      <c r="AMJ13" s="0"/>
     </row>
     <row r="14" customFormat="false" ht="17.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A14" s="0"/>
       <c r="B14" s="9" t="s">
         <v>59</v>
       </c>
-      <c r="C14" s="8" t="s">
+      <c r="C14" s="9" t="s">
         <v>60</v>
       </c>
-      <c r="D14" s="9" t="s">
+      <c r="D14" s="8" t="s">
         <v>61</v>
       </c>
       <c r="E14" s="8"/>
@@ -15380,7 +15410,6 @@
       <c r="AMG14" s="0"/>
       <c r="AMH14" s="0"/>
       <c r="AMI14" s="0"/>
-      <c r="AMJ14" s="0"/>
     </row>
     <row r="15" customFormat="false" ht="12.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A15" s="0"/>
@@ -16406,7 +16435,6 @@
       <c r="AMG15" s="0"/>
       <c r="AMH15" s="0"/>
       <c r="AMI15" s="0"/>
-      <c r="AMJ15" s="0"/>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="0"/>
@@ -17432,7 +17460,6 @@
       <c r="AMG16" s="0"/>
       <c r="AMH16" s="0"/>
       <c r="AMI16" s="0"/>
-      <c r="AMJ16" s="0"/>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="0"/>
@@ -18458,7 +18485,6 @@
       <c r="AMG17" s="0"/>
       <c r="AMH17" s="0"/>
       <c r="AMI17" s="0"/>
-      <c r="AMJ17" s="0"/>
     </row>
     <row r="18" customFormat="false" ht="14.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A18" s="0"/>
@@ -19484,7 +19510,6 @@
       <c r="AMG18" s="0"/>
       <c r="AMH18" s="0"/>
       <c r="AMI18" s="0"/>
-      <c r="AMJ18" s="0"/>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="0"/>
@@ -20510,7 +20535,6 @@
       <c r="AMG19" s="0"/>
       <c r="AMH19" s="0"/>
       <c r="AMI19" s="0"/>
-      <c r="AMJ19" s="0"/>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="0"/>
@@ -21536,13 +21560,12 @@
       <c r="AMG20" s="0"/>
       <c r="AMH20" s="0"/>
       <c r="AMI20" s="0"/>
-      <c r="AMJ20" s="0"/>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="0"/>
       <c r="B21" s="0"/>
-      <c r="C21" s="0"/>
-      <c r="D21" s="8"/>
+      <c r="C21" s="8"/>
+      <c r="D21" s="0"/>
       <c r="E21" s="0"/>
       <c r="F21" s="0"/>
       <c r="G21" s="0"/>
@@ -22562,7 +22585,6 @@
       <c r="AMG21" s="0"/>
       <c r="AMH21" s="0"/>
       <c r="AMI21" s="0"/>
-      <c r="AMJ21" s="0"/>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="0"/>
@@ -23588,13 +23610,12 @@
       <c r="AMG22" s="0"/>
       <c r="AMH22" s="0"/>
       <c r="AMI22" s="0"/>
-      <c r="AMJ22" s="0"/>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="0"/>
       <c r="B23" s="4"/>
-      <c r="C23" s="4"/>
-      <c r="D23" s="4"/>
+      <c r="C23" s="0"/>
+      <c r="D23" s="0"/>
       <c r="E23" s="0"/>
       <c r="F23" s="0"/>
       <c r="G23" s="0"/>
@@ -24614,7 +24635,6 @@
       <c r="AMG23" s="0"/>
       <c r="AMH23" s="0"/>
       <c r="AMI23" s="0"/>
-      <c r="AMJ23" s="0"/>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="0"/>
@@ -25640,13 +25660,12 @@
       <c r="AMG24" s="0"/>
       <c r="AMH24" s="0"/>
       <c r="AMI24" s="0"/>
-      <c r="AMJ24" s="0"/>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="0"/>
       <c r="B25" s="4"/>
       <c r="C25" s="4"/>
-      <c r="D25" s="8"/>
+      <c r="D25" s="4"/>
       <c r="E25" s="0"/>
       <c r="F25" s="0"/>
       <c r="G25" s="0"/>
@@ -26666,13 +26685,12 @@
       <c r="AMG25" s="0"/>
       <c r="AMH25" s="0"/>
       <c r="AMI25" s="0"/>
-      <c r="AMJ25" s="0"/>
     </row>
     <row r="26" customFormat="false" ht="29.2" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A26" s="0"/>
       <c r="B26" s="4"/>
       <c r="C26" s="4"/>
-      <c r="D26" s="8"/>
+      <c r="D26" s="4"/>
       <c r="E26" s="0"/>
       <c r="F26" s="0"/>
       <c r="G26" s="0"/>
@@ -27692,7 +27710,6 @@
       <c r="AMG26" s="0"/>
       <c r="AMH26" s="0"/>
       <c r="AMI26" s="0"/>
-      <c r="AMJ26" s="0"/>
     </row>
     <row r="27" customFormat="false" ht="23.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A27" s="0"/>
@@ -28718,13 +28735,12 @@
       <c r="AMG27" s="0"/>
       <c r="AMH27" s="0"/>
       <c r="AMI27" s="0"/>
-      <c r="AMJ27" s="0"/>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="0"/>
       <c r="B28" s="4"/>
       <c r="C28" s="4"/>
-      <c r="D28" s="0"/>
+      <c r="D28" s="4"/>
       <c r="E28" s="0"/>
       <c r="F28" s="0"/>
       <c r="G28" s="0"/>
@@ -29744,13 +29760,12 @@
       <c r="AMG28" s="0"/>
       <c r="AMH28" s="0"/>
       <c r="AMI28" s="0"/>
-      <c r="AMJ28" s="0"/>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="0"/>
       <c r="B29" s="4"/>
       <c r="C29" s="4"/>
-      <c r="D29" s="8"/>
+      <c r="D29" s="4"/>
       <c r="E29" s="0"/>
       <c r="F29" s="0"/>
       <c r="G29" s="0"/>
@@ -30770,13 +30785,12 @@
       <c r="AMG29" s="0"/>
       <c r="AMH29" s="0"/>
       <c r="AMI29" s="0"/>
-      <c r="AMJ29" s="0"/>
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="0"/>
       <c r="B30" s="4"/>
       <c r="C30" s="4"/>
-      <c r="D30" s="8"/>
+      <c r="D30" s="4"/>
       <c r="E30" s="0"/>
       <c r="F30" s="0"/>
       <c r="G30" s="0"/>
@@ -31796,13 +31810,12 @@
       <c r="AMG30" s="0"/>
       <c r="AMH30" s="0"/>
       <c r="AMI30" s="0"/>
-      <c r="AMJ30" s="0"/>
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="0"/>
       <c r="B31" s="4"/>
       <c r="C31" s="4"/>
-      <c r="D31" s="8"/>
+      <c r="D31" s="4"/>
       <c r="E31" s="0"/>
       <c r="F31" s="0"/>
       <c r="G31" s="0"/>
@@ -32822,13 +32835,12 @@
       <c r="AMG31" s="0"/>
       <c r="AMH31" s="0"/>
       <c r="AMI31" s="0"/>
-      <c r="AMJ31" s="0"/>
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="0"/>
       <c r="B32" s="4"/>
       <c r="C32" s="4"/>
-      <c r="D32" s="8"/>
+      <c r="D32" s="4"/>
       <c r="E32" s="0"/>
       <c r="F32" s="0"/>
       <c r="G32" s="0"/>
@@ -33848,7 +33860,6 @@
       <c r="AMG32" s="0"/>
       <c r="AMH32" s="0"/>
       <c r="AMI32" s="0"/>
-      <c r="AMJ32" s="0"/>
     </row>
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="0"/>
@@ -34874,13 +34885,12 @@
       <c r="AMG33" s="0"/>
       <c r="AMH33" s="0"/>
       <c r="AMI33" s="0"/>
-      <c r="AMJ33" s="0"/>
     </row>
     <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="0"/>
       <c r="B34" s="4"/>
       <c r="C34" s="4"/>
-      <c r="D34" s="8"/>
+      <c r="D34" s="4"/>
       <c r="E34" s="0"/>
       <c r="F34" s="0"/>
       <c r="G34" s="0"/>
@@ -35900,7 +35910,6 @@
       <c r="AMG34" s="0"/>
       <c r="AMH34" s="0"/>
       <c r="AMI34" s="0"/>
-      <c r="AMJ34" s="0"/>
     </row>
     <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="0"/>
@@ -36926,10 +36935,9 @@
       <c r="AMG35" s="0"/>
       <c r="AMH35" s="0"/>
       <c r="AMI35" s="0"/>
-      <c r="AMJ35" s="0"/>
     </row>
     <row r="36" s="4" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D36" s="8"/>
+      <c r="AMJ36" s="0"/>
     </row>
     <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="0"/>
@@ -37129,22 +37137,22 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="7.88383838383838"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="10.959595959596"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="9.22222222222222"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="33.540404040404"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="19.3737373737374"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="17.3737373737374"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="26.3232323232323"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="19.7777777777778"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="13.8989898989899"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="9.08585858585859"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="7.88383838383838"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="12.0252525252525"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="16.3030303030303"/>
-    <col collapsed="false" hidden="false" max="19" min="14" style="0" width="7.88383838383838"/>
-    <col collapsed="false" hidden="false" max="20" min="20" style="0" width="18.1717171717172"/>
-    <col collapsed="false" hidden="false" max="1025" min="21" style="0" width="7.88383838383838"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="7.34848484848485"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="10.4242424242424"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="8.95454545454546"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="32.0707070707071"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="18.5757575757576"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="16.5707070707071"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="25.1212121212121"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="18.8434343434343"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="13.0959595959596"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="8.68686868686869"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="7.34848484848485"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="11.2272727272727"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="15.5"/>
+    <col collapsed="false" hidden="false" max="19" min="14" style="0" width="7.34848484848485"/>
+    <col collapsed="false" hidden="false" max="20" min="20" style="0" width="17.1060606060606"/>
+    <col collapsed="false" hidden="false" max="1025" min="21" style="0" width="7.34848484848485"/>
   </cols>
   <sheetData>
     <row r="1" s="6" customFormat="true" ht="17.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -37445,20 +37453,20 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:F48"/>
+  <dimension ref="A1:F49"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E6" activeCellId="0" sqref="E6"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A13" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B33" activeCellId="0" sqref="B33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="14.2979797979798"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="21.9141414141414"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="20.979797979798"/>
-    <col collapsed="false" hidden="false" max="5" min="4" style="0" width="29.2626262626263"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="43.9646464646465"/>
-    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="7.88383838383838"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="13.4949494949495"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="20.979797979798"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="19.9090909090909"/>
+    <col collapsed="false" hidden="false" max="5" min="4" style="0" width="27.9292929292929"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="42.0909090909091"/>
+    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="7.34848484848485"/>
   </cols>
   <sheetData>
     <row r="1" s="1" customFormat="true" ht="22.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -37486,10 +37494,10 @@
         <v>101</v>
       </c>
       <c r="D3" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="E3" s="9" t="s">
         <v>35</v>
-      </c>
-      <c r="E3" s="9" t="s">
-        <v>36</v>
       </c>
       <c r="F3" s="8"/>
     </row>
@@ -37568,10 +37576,10 @@
         <v>114</v>
       </c>
       <c r="D9" s="8" t="s">
+        <v>51</v>
+      </c>
+      <c r="E9" s="9" t="s">
         <v>50</v>
-      </c>
-      <c r="E9" s="9" t="s">
-        <v>51</v>
       </c>
       <c r="F9" s="8"/>
     </row>
@@ -37910,13 +37918,13 @@
         <v>91</v>
       </c>
       <c r="C33" s="9" t="s">
-        <v>114</v>
-      </c>
-      <c r="D33" s="8" t="s">
-        <v>50</v>
-      </c>
-      <c r="E33" s="9" t="s">
-        <v>51</v>
+        <v>160</v>
+      </c>
+      <c r="D33" s="9" t="s">
+        <v>160</v>
+      </c>
+      <c r="E33" s="8" t="s">
+        <v>161</v>
       </c>
       <c r="F33" s="8"/>
     </row>
@@ -37925,50 +37933,50 @@
         <v>91</v>
       </c>
       <c r="C34" s="9" t="s">
-        <v>105</v>
+        <v>114</v>
       </c>
       <c r="D34" s="8" t="s">
-        <v>106</v>
+        <v>51</v>
       </c>
       <c r="E34" s="9" t="s">
-        <v>107</v>
+        <v>50</v>
       </c>
       <c r="F34" s="8"/>
     </row>
-    <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B35" s="7"/>
-      <c r="C35" s="7"/>
-      <c r="D35" s="7"/>
-      <c r="E35" s="7"/>
-      <c r="F35" s="7"/>
+    <row r="35" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B35" s="9" t="s">
+        <v>91</v>
+      </c>
+      <c r="C35" s="9" t="s">
+        <v>105</v>
+      </c>
+      <c r="D35" s="8" t="s">
+        <v>106</v>
+      </c>
+      <c r="E35" s="9" t="s">
+        <v>107</v>
+      </c>
+      <c r="F35" s="8"/>
     </row>
-    <row r="36" customFormat="false" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B36" s="9" t="s">
-        <v>95</v>
-      </c>
-      <c r="C36" s="9" t="s">
-        <v>160</v>
-      </c>
-      <c r="D36" s="8" t="s">
-        <v>161</v>
-      </c>
-      <c r="E36" s="9" t="s">
-        <v>162</v>
-      </c>
-      <c r="F36" s="8"/>
+    <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B36" s="7"/>
+      <c r="C36" s="7"/>
+      <c r="D36" s="7"/>
+      <c r="E36" s="7"/>
+      <c r="F36" s="7"/>
     </row>
     <row r="37" customFormat="false" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B37" s="9" t="s">
         <v>95</v>
       </c>
       <c r="C37" s="9" t="s">
+        <v>162</v>
+      </c>
+      <c r="D37" s="8" t="s">
         <v>163</v>
       </c>
-      <c r="D37" s="8" t="s">
+      <c r="E37" s="9" t="s">
         <v>164</v>
-      </c>
-      <c r="E37" s="9" t="s">
-        <v>165</v>
       </c>
       <c r="F37" s="8"/>
     </row>
@@ -37977,13 +37985,13 @@
         <v>95</v>
       </c>
       <c r="C38" s="9" t="s">
+        <v>165</v>
+      </c>
+      <c r="D38" s="8" t="s">
         <v>166</v>
       </c>
-      <c r="D38" s="8" t="s">
+      <c r="E38" s="9" t="s">
         <v>167</v>
-      </c>
-      <c r="E38" s="9" t="s">
-        <v>168</v>
       </c>
       <c r="F38" s="8"/>
     </row>
@@ -37992,13 +38000,13 @@
         <v>95</v>
       </c>
       <c r="C39" s="9" t="s">
+        <v>168</v>
+      </c>
+      <c r="D39" s="8" t="s">
         <v>169</v>
       </c>
-      <c r="D39" s="8" t="s">
+      <c r="E39" s="9" t="s">
         <v>170</v>
-      </c>
-      <c r="E39" s="9" t="s">
-        <v>171</v>
       </c>
       <c r="F39" s="8"/>
     </row>
@@ -38007,43 +38015,43 @@
         <v>95</v>
       </c>
       <c r="C40" s="9" t="s">
+        <v>171</v>
+      </c>
+      <c r="D40" s="8" t="s">
         <v>172</v>
       </c>
-      <c r="D40" s="8" t="s">
+      <c r="E40" s="9" t="s">
         <v>173</v>
-      </c>
-      <c r="E40" s="9" t="s">
-        <v>174</v>
       </c>
       <c r="F40" s="8"/>
     </row>
-    <row r="42" customFormat="false" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B42" s="9" t="s">
-        <v>97</v>
-      </c>
-      <c r="C42" s="9" t="s">
+    <row r="41" customFormat="false" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B41" s="9" t="s">
+        <v>95</v>
+      </c>
+      <c r="C41" s="9" t="s">
+        <v>174</v>
+      </c>
+      <c r="D41" s="8" t="s">
         <v>175</v>
       </c>
-      <c r="D42" s="8" t="s">
+      <c r="E41" s="9" t="s">
         <v>176</v>
       </c>
-      <c r="E42" s="9" t="s">
-        <v>177</v>
-      </c>
-      <c r="F42" s="8"/>
+      <c r="F41" s="8"/>
     </row>
     <row r="43" customFormat="false" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B43" s="9" t="s">
         <v>97</v>
       </c>
       <c r="C43" s="9" t="s">
+        <v>177</v>
+      </c>
+      <c r="D43" s="8" t="s">
         <v>178</v>
       </c>
-      <c r="D43" s="8" t="s">
+      <c r="E43" s="9" t="s">
         <v>179</v>
-      </c>
-      <c r="E43" s="9" t="s">
-        <v>180</v>
       </c>
       <c r="F43" s="8"/>
     </row>
@@ -38052,13 +38060,13 @@
         <v>97</v>
       </c>
       <c r="C44" s="9" t="s">
+        <v>180</v>
+      </c>
+      <c r="D44" s="8" t="s">
         <v>181</v>
       </c>
-      <c r="D44" s="8" t="s">
+      <c r="E44" s="9" t="s">
         <v>182</v>
-      </c>
-      <c r="E44" s="9" t="s">
-        <v>183</v>
       </c>
       <c r="F44" s="8"/>
     </row>
@@ -38067,13 +38075,13 @@
         <v>97</v>
       </c>
       <c r="C45" s="9" t="s">
+        <v>183</v>
+      </c>
+      <c r="D45" s="8" t="s">
         <v>184</v>
       </c>
-      <c r="D45" s="8" t="s">
+      <c r="E45" s="9" t="s">
         <v>185</v>
-      </c>
-      <c r="E45" s="9" t="s">
-        <v>186</v>
       </c>
       <c r="F45" s="8"/>
     </row>
@@ -38082,28 +38090,28 @@
         <v>97</v>
       </c>
       <c r="C46" s="9" t="s">
+        <v>186</v>
+      </c>
+      <c r="D46" s="8" t="s">
         <v>187</v>
       </c>
-      <c r="D46" s="8" t="s">
+      <c r="E46" s="9" t="s">
         <v>188</v>
-      </c>
-      <c r="E46" s="9" t="s">
-        <v>189</v>
       </c>
       <c r="F46" s="8"/>
     </row>
-    <row r="47" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="47" customFormat="false" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B47" s="9" t="s">
         <v>97</v>
       </c>
       <c r="C47" s="9" t="s">
+        <v>189</v>
+      </c>
+      <c r="D47" s="8" t="s">
         <v>190</v>
       </c>
-      <c r="D47" s="8" t="s">
-        <v>103</v>
-      </c>
       <c r="E47" s="9" t="s">
-        <v>104</v>
+        <v>191</v>
       </c>
       <c r="F47" s="8"/>
     </row>
@@ -38112,15 +38120,30 @@
         <v>97</v>
       </c>
       <c r="C48" s="9" t="s">
-        <v>191</v>
+        <v>192</v>
       </c>
       <c r="D48" s="8" t="s">
+        <v>103</v>
+      </c>
+      <c r="E48" s="9" t="s">
+        <v>104</v>
+      </c>
+      <c r="F48" s="8"/>
+    </row>
+    <row r="49" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B49" s="9" t="s">
+        <v>97</v>
+      </c>
+      <c r="C49" s="9" t="s">
+        <v>193</v>
+      </c>
+      <c r="D49" s="8" t="s">
         <v>106</v>
       </c>
-      <c r="E48" s="9" t="s">
+      <c r="E49" s="9" t="s">
         <v>107</v>
       </c>
-      <c r="F48" s="8"/>
+      <c r="F49" s="8"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
@@ -38140,23 +38163,23 @@
   </sheetPr>
   <dimension ref="1:112"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A100" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="C19" activeCellId="0" sqref="C19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="13.0959595959596"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="15.1010101010101"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="35.010101010101"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="13.4949494949495"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="23.520202020202"/>
-    <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="7.88383838383838"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="12.5606060606061"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="14.2979797979798"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="33.4090909090909"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="12.8282828282828"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="22.4494949494949"/>
+    <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="7.34848484848485"/>
   </cols>
   <sheetData>
     <row r="1" s="6" customFormat="true" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
-        <v>192</v>
+        <v>194</v>
       </c>
       <c r="B1" s="12" t="s">
         <v>1</v>
@@ -38168,13 +38191,13 @@
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="3" t="s">
-        <v>193</v>
+        <v>195</v>
       </c>
       <c r="B2" s="3" t="s">
         <v>79</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>194</v>
+        <v>196</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -38210,7 +38233,7 @@
         <v>84</v>
       </c>
       <c r="C7" s="7" t="s">
-        <v>195</v>
+        <v>197</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -38218,7 +38241,7 @@
         <v>84</v>
       </c>
       <c r="C8" s="7" t="s">
-        <v>196</v>
+        <v>198</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -38226,7 +38249,7 @@
         <v>84</v>
       </c>
       <c r="C9" s="7" t="s">
-        <v>197</v>
+        <v>199</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -38286,7 +38309,7 @@
         <v>80</v>
       </c>
       <c r="C18" s="3" t="s">
-        <v>198</v>
+        <v>200</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -38294,7 +38317,7 @@
         <v>80</v>
       </c>
       <c r="C19" s="3" t="s">
-        <v>199</v>
+        <v>201</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -38302,7 +38325,7 @@
         <v>80</v>
       </c>
       <c r="C20" s="3" t="s">
-        <v>200</v>
+        <v>202</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -38310,7 +38333,7 @@
         <v>80</v>
       </c>
       <c r="C21" s="3" t="s">
-        <v>201</v>
+        <v>203</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -38318,7 +38341,7 @@
         <v>80</v>
       </c>
       <c r="C22" s="3" t="s">
-        <v>202</v>
+        <v>204</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -38326,7 +38349,7 @@
         <v>80</v>
       </c>
       <c r="C23" s="3" t="s">
-        <v>203</v>
+        <v>205</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -38334,7 +38357,7 @@
         <v>80</v>
       </c>
       <c r="C24" s="3" t="s">
-        <v>204</v>
+        <v>206</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -38342,7 +38365,7 @@
         <v>80</v>
       </c>
       <c r="C25" s="3" t="s">
-        <v>205</v>
+        <v>207</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -38350,7 +38373,7 @@
         <v>80</v>
       </c>
       <c r="C26" s="3" t="s">
-        <v>206</v>
+        <v>208</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -38358,7 +38381,7 @@
         <v>80</v>
       </c>
       <c r="C27" s="3" t="s">
-        <v>207</v>
+        <v>209</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -38366,7 +38389,7 @@
         <v>80</v>
       </c>
       <c r="C28" s="3" t="s">
-        <v>208</v>
+        <v>210</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -38374,7 +38397,7 @@
         <v>80</v>
       </c>
       <c r="C29" s="3" t="s">
-        <v>209</v>
+        <v>211</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -38382,7 +38405,7 @@
         <v>80</v>
       </c>
       <c r="C30" s="3" t="s">
-        <v>210</v>
+        <v>212</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -38390,7 +38413,7 @@
         <v>80</v>
       </c>
       <c r="C31" s="3" t="s">
-        <v>211</v>
+        <v>213</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -38398,7 +38421,7 @@
         <v>80</v>
       </c>
       <c r="C32" s="3" t="s">
-        <v>212</v>
+        <v>214</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -38406,7 +38429,7 @@
         <v>80</v>
       </c>
       <c r="C33" s="3" t="s">
-        <v>213</v>
+        <v>215</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -38414,7 +38437,7 @@
         <v>80</v>
       </c>
       <c r="C34" s="3" t="s">
-        <v>214</v>
+        <v>216</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -38422,7 +38445,7 @@
         <v>80</v>
       </c>
       <c r="C35" s="3" t="s">
-        <v>215</v>
+        <v>217</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -38430,7 +38453,7 @@
         <v>80</v>
       </c>
       <c r="C36" s="3" t="s">
-        <v>216</v>
+        <v>218</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -38438,7 +38461,7 @@
         <v>80</v>
       </c>
       <c r="C37" s="3" t="s">
-        <v>217</v>
+        <v>219</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -38446,7 +38469,7 @@
         <v>80</v>
       </c>
       <c r="C38" s="3" t="s">
-        <v>218</v>
+        <v>220</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -38454,7 +38477,7 @@
         <v>80</v>
       </c>
       <c r="C39" s="3" t="s">
-        <v>219</v>
+        <v>221</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -38462,7 +38485,7 @@
         <v>80</v>
       </c>
       <c r="C40" s="3" t="s">
-        <v>220</v>
+        <v>222</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -38470,7 +38493,7 @@
         <v>80</v>
       </c>
       <c r="C41" s="3" t="s">
-        <v>221</v>
+        <v>223</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -38478,7 +38501,7 @@
         <v>80</v>
       </c>
       <c r="C42" s="3" t="s">
-        <v>222</v>
+        <v>224</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -38486,7 +38509,7 @@
         <v>80</v>
       </c>
       <c r="C43" s="3" t="s">
-        <v>223</v>
+        <v>225</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -38494,7 +38517,7 @@
         <v>80</v>
       </c>
       <c r="C44" s="3" t="s">
-        <v>224</v>
+        <v>226</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -38502,7 +38525,7 @@
         <v>80</v>
       </c>
       <c r="C45" s="3" t="s">
-        <v>225</v>
+        <v>227</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -38510,7 +38533,7 @@
         <v>80</v>
       </c>
       <c r="C46" s="3" t="s">
-        <v>226</v>
+        <v>228</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -38518,7 +38541,7 @@
         <v>80</v>
       </c>
       <c r="C47" s="3" t="s">
-        <v>227</v>
+        <v>229</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -38526,7 +38549,7 @@
         <v>80</v>
       </c>
       <c r="C48" s="3" t="s">
-        <v>228</v>
+        <v>230</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -38534,7 +38557,7 @@
         <v>80</v>
       </c>
       <c r="C49" s="3" t="s">
-        <v>229</v>
+        <v>231</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -38542,7 +38565,7 @@
         <v>80</v>
       </c>
       <c r="C50" s="3" t="s">
-        <v>230</v>
+        <v>232</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -38550,7 +38573,7 @@
         <v>80</v>
       </c>
       <c r="C51" s="3" t="s">
-        <v>231</v>
+        <v>233</v>
       </c>
     </row>
     <row r="52" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -38558,7 +38581,7 @@
         <v>80</v>
       </c>
       <c r="C52" s="3" t="s">
-        <v>232</v>
+        <v>234</v>
       </c>
     </row>
     <row r="53" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -38566,7 +38589,7 @@
         <v>80</v>
       </c>
       <c r="C53" s="3" t="s">
-        <v>233</v>
+        <v>235</v>
       </c>
     </row>
     <row r="54" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -38574,7 +38597,7 @@
         <v>80</v>
       </c>
       <c r="C54" s="3" t="s">
-        <v>234</v>
+        <v>236</v>
       </c>
     </row>
     <row r="55" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -38582,7 +38605,7 @@
         <v>80</v>
       </c>
       <c r="C55" s="3" t="s">
-        <v>235</v>
+        <v>237</v>
       </c>
     </row>
     <row r="56" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -38590,7 +38613,7 @@
         <v>80</v>
       </c>
       <c r="C56" s="3" t="s">
-        <v>236</v>
+        <v>238</v>
       </c>
     </row>
     <row r="57" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -38598,7 +38621,7 @@
         <v>80</v>
       </c>
       <c r="C57" s="3" t="s">
-        <v>237</v>
+        <v>239</v>
       </c>
     </row>
     <row r="58" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -38606,7 +38629,7 @@
         <v>80</v>
       </c>
       <c r="C58" s="3" t="s">
-        <v>238</v>
+        <v>240</v>
       </c>
     </row>
     <row r="59" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -38614,7 +38637,7 @@
         <v>80</v>
       </c>
       <c r="C59" s="3" t="s">
-        <v>239</v>
+        <v>241</v>
       </c>
     </row>
     <row r="60" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -38622,7 +38645,7 @@
         <v>80</v>
       </c>
       <c r="C60" s="3" t="s">
-        <v>240</v>
+        <v>242</v>
       </c>
     </row>
     <row r="61" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -38630,7 +38653,7 @@
         <v>80</v>
       </c>
       <c r="C61" s="3" t="s">
-        <v>241</v>
+        <v>243</v>
       </c>
     </row>
     <row r="62" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -38638,7 +38661,7 @@
         <v>80</v>
       </c>
       <c r="C62" s="3" t="s">
-        <v>242</v>
+        <v>244</v>
       </c>
     </row>
     <row r="63" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -38646,7 +38669,7 @@
         <v>80</v>
       </c>
       <c r="C63" s="3" t="s">
-        <v>243</v>
+        <v>245</v>
       </c>
     </row>
     <row r="64" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -38654,7 +38677,7 @@
         <v>80</v>
       </c>
       <c r="C64" s="3" t="s">
-        <v>244</v>
+        <v>246</v>
       </c>
     </row>
     <row r="65" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -38662,7 +38685,7 @@
         <v>80</v>
       </c>
       <c r="C65" s="3" t="s">
-        <v>245</v>
+        <v>247</v>
       </c>
     </row>
     <row r="66" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -38670,7 +38693,7 @@
         <v>80</v>
       </c>
       <c r="C66" s="3" t="s">
-        <v>246</v>
+        <v>248</v>
       </c>
     </row>
     <row r="68" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -38678,7 +38701,7 @@
         <v>80</v>
       </c>
       <c r="C68" s="3" t="s">
-        <v>247</v>
+        <v>249</v>
       </c>
     </row>
     <row r="69" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -38686,7 +38709,7 @@
         <v>80</v>
       </c>
       <c r="C69" s="3" t="s">
-        <v>248</v>
+        <v>250</v>
       </c>
     </row>
     <row r="70" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -38694,7 +38717,7 @@
         <v>80</v>
       </c>
       <c r="C70" s="3" t="s">
-        <v>249</v>
+        <v>251</v>
       </c>
     </row>
     <row r="71" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -38702,7 +38725,7 @@
         <v>80</v>
       </c>
       <c r="C71" s="3" t="s">
-        <v>250</v>
+        <v>252</v>
       </c>
     </row>
     <row r="72" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -38710,7 +38733,7 @@
         <v>80</v>
       </c>
       <c r="C72" s="3" t="s">
-        <v>251</v>
+        <v>253</v>
       </c>
     </row>
     <row r="73" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -38718,7 +38741,7 @@
         <v>80</v>
       </c>
       <c r="C73" s="3" t="s">
-        <v>252</v>
+        <v>254</v>
       </c>
     </row>
     <row r="74" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -38726,7 +38749,7 @@
         <v>80</v>
       </c>
       <c r="C74" s="3" t="s">
-        <v>253</v>
+        <v>255</v>
       </c>
     </row>
     <row r="75" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -38734,7 +38757,7 @@
         <v>80</v>
       </c>
       <c r="C75" s="3" t="s">
-        <v>254</v>
+        <v>256</v>
       </c>
     </row>
     <row r="76" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -38742,7 +38765,7 @@
         <v>80</v>
       </c>
       <c r="C76" s="3" t="s">
-        <v>255</v>
+        <v>257</v>
       </c>
     </row>
     <row r="77" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -38750,7 +38773,7 @@
         <v>80</v>
       </c>
       <c r="C77" s="3" t="s">
-        <v>256</v>
+        <v>258</v>
       </c>
     </row>
     <row r="78" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -38758,7 +38781,7 @@
         <v>80</v>
       </c>
       <c r="C78" s="3" t="s">
-        <v>257</v>
+        <v>259</v>
       </c>
     </row>
     <row r="79" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -38766,7 +38789,7 @@
         <v>80</v>
       </c>
       <c r="C79" s="3" t="s">
-        <v>258</v>
+        <v>260</v>
       </c>
     </row>
     <row r="80" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -38774,7 +38797,7 @@
         <v>80</v>
       </c>
       <c r="C80" s="3" t="s">
-        <v>259</v>
+        <v>261</v>
       </c>
     </row>
     <row r="81" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -38782,7 +38805,7 @@
         <v>80</v>
       </c>
       <c r="C81" s="3" t="s">
-        <v>260</v>
+        <v>262</v>
       </c>
     </row>
     <row r="82" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -38790,7 +38813,7 @@
         <v>80</v>
       </c>
       <c r="C82" s="3" t="s">
-        <v>261</v>
+        <v>263</v>
       </c>
     </row>
     <row r="83" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -38798,7 +38821,7 @@
         <v>80</v>
       </c>
       <c r="C83" s="3" t="s">
-        <v>262</v>
+        <v>264</v>
       </c>
     </row>
     <row r="84" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -38806,7 +38829,7 @@
         <v>80</v>
       </c>
       <c r="C84" s="3" t="s">
-        <v>263</v>
+        <v>265</v>
       </c>
     </row>
     <row r="85" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -38814,7 +38837,7 @@
         <v>80</v>
       </c>
       <c r="C85" s="3" t="s">
-        <v>264</v>
+        <v>266</v>
       </c>
     </row>
     <row r="86" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -38822,7 +38845,7 @@
         <v>80</v>
       </c>
       <c r="C86" s="3" t="s">
-        <v>265</v>
+        <v>267</v>
       </c>
     </row>
     <row r="87" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -38830,7 +38853,7 @@
         <v>80</v>
       </c>
       <c r="C87" s="3" t="s">
-        <v>266</v>
+        <v>268</v>
       </c>
     </row>
     <row r="89" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -38838,7 +38861,7 @@
         <v>80</v>
       </c>
       <c r="C89" s="3" t="s">
-        <v>267</v>
+        <v>269</v>
       </c>
     </row>
     <row r="90" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -38846,7 +38869,7 @@
         <v>80</v>
       </c>
       <c r="C90" s="3" t="s">
-        <v>268</v>
+        <v>270</v>
       </c>
     </row>
     <row r="91" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -38854,7 +38877,7 @@
         <v>80</v>
       </c>
       <c r="C91" s="3" t="s">
-        <v>269</v>
+        <v>271</v>
       </c>
     </row>
     <row r="92" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -38862,7 +38885,7 @@
         <v>80</v>
       </c>
       <c r="C92" s="3" t="s">
-        <v>270</v>
+        <v>272</v>
       </c>
     </row>
     <row r="93" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -38870,7 +38893,7 @@
         <v>80</v>
       </c>
       <c r="C93" s="3" t="s">
-        <v>271</v>
+        <v>273</v>
       </c>
     </row>
     <row r="94" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -38878,7 +38901,7 @@
         <v>80</v>
       </c>
       <c r="C94" s="3" t="s">
-        <v>272</v>
+        <v>274</v>
       </c>
     </row>
     <row r="95" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -38886,7 +38909,7 @@
         <v>80</v>
       </c>
       <c r="C95" s="3" t="s">
-        <v>273</v>
+        <v>275</v>
       </c>
     </row>
     <row r="96" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -38894,7 +38917,7 @@
         <v>80</v>
       </c>
       <c r="C96" s="3" t="s">
-        <v>274</v>
+        <v>276</v>
       </c>
     </row>
     <row r="97" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -38902,7 +38925,7 @@
         <v>80</v>
       </c>
       <c r="C97" s="3" t="s">
-        <v>275</v>
+        <v>277</v>
       </c>
     </row>
     <row r="98" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -38910,7 +38933,7 @@
         <v>80</v>
       </c>
       <c r="C98" s="3" t="s">
-        <v>276</v>
+        <v>278</v>
       </c>
     </row>
     <row r="99" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -38918,7 +38941,7 @@
         <v>80</v>
       </c>
       <c r="C99" s="3" t="s">
-        <v>277</v>
+        <v>279</v>
       </c>
     </row>
     <row r="100" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -38926,7 +38949,7 @@
         <v>80</v>
       </c>
       <c r="C100" s="3" t="s">
-        <v>278</v>
+        <v>280</v>
       </c>
     </row>
     <row r="101" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -38934,7 +38957,7 @@
         <v>80</v>
       </c>
       <c r="C101" s="3" t="s">
-        <v>279</v>
+        <v>281</v>
       </c>
     </row>
     <row r="102" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -38942,7 +38965,7 @@
         <v>80</v>
       </c>
       <c r="C102" s="3" t="s">
-        <v>280</v>
+        <v>282</v>
       </c>
     </row>
     <row r="103" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -38950,7 +38973,7 @@
         <v>80</v>
       </c>
       <c r="C103" s="3" t="s">
-        <v>281</v>
+        <v>283</v>
       </c>
     </row>
     <row r="104" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -38958,7 +38981,7 @@
         <v>80</v>
       </c>
       <c r="C104" s="3" t="s">
-        <v>282</v>
+        <v>284</v>
       </c>
     </row>
     <row r="105" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -38966,7 +38989,7 @@
         <v>80</v>
       </c>
       <c r="C105" s="3" t="s">
-        <v>283</v>
+        <v>285</v>
       </c>
     </row>
     <row r="106" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -38974,7 +38997,7 @@
         <v>80</v>
       </c>
       <c r="C106" s="3" t="s">
-        <v>284</v>
+        <v>286</v>
       </c>
     </row>
     <row r="107" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -38982,7 +39005,7 @@
         <v>80</v>
       </c>
       <c r="C107" s="3" t="s">
-        <v>285</v>
+        <v>287</v>
       </c>
     </row>
     <row r="108" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -38990,7 +39013,7 @@
         <v>80</v>
       </c>
       <c r="C108" s="3" t="s">
-        <v>286</v>
+        <v>288</v>
       </c>
     </row>
     <row r="109" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -38998,7 +39021,7 @@
         <v>80</v>
       </c>
       <c r="C109" s="7" t="s">
-        <v>287</v>
+        <v>289</v>
       </c>
     </row>
     <row r="111" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -39006,7 +39029,7 @@
         <v>80</v>
       </c>
       <c r="C111" s="3" t="s">
-        <v>288</v>
+        <v>290</v>
       </c>
     </row>
     <row r="112" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -39014,7 +39037,7 @@
         <v>80</v>
       </c>
       <c r="C112" s="7" t="s">
-        <v>289</v>
+        <v>291</v>
       </c>
     </row>
   </sheetData>
@@ -39041,14 +39064,14 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="34.2070707070707"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="40.0909090909091"/>
-    <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="7.88383838383838"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="32.6060606060606"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="38.3535353535354"/>
+    <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="7.34848484848485"/>
   </cols>
   <sheetData>
     <row r="1" s="2" customFormat="true" ht="13.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
-        <v>290</v>
+        <v>292</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>68</v>
@@ -39056,26 +39079,26 @@
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="7" t="s">
-        <v>291</v>
+        <v>293</v>
       </c>
       <c r="B3" s="7" t="s">
-        <v>292</v>
+        <v>294</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="7" t="s">
-        <v>293</v>
+        <v>295</v>
       </c>
       <c r="B4" s="7" t="s">
-        <v>294</v>
+        <v>296</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="7" t="s">
-        <v>295</v>
+        <v>297</v>
       </c>
       <c r="B5" s="7" t="s">
-        <v>296</v>
+        <v>298</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
update section 10 prompts and section 7 answers
</commit_message>
<xml_diff>
--- a/tables/actor/forms/actor/actor.xlsx
+++ b/tables/actor/forms/actor/actor.xlsx
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="533" uniqueCount="299">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="529" uniqueCount="297">
   <si>
     <t xml:space="preserve">clause</t>
   </si>
@@ -1056,12 +1056,6 @@
     <t xml:space="preserve">အတူရွေ့ပြောင်းတဲ့ အဖော်</t>
   </si>
   <si>
-    <t xml:space="preserve">Broker</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ပွဲစား</t>
-  </si>
-  <si>
     <t xml:space="preserve">Any type of Agent </t>
   </si>
   <si>
@@ -1797,9 +1791,11 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="12.0252525252525"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="15.1010101010101"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="34.3434343434343"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="11.6262626262626"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="8.41919191919192"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="14.6969696969697"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="33.540404040404"/>
+    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="8.41919191919192"/>
   </cols>
   <sheetData>
     <row r="1" s="2" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1856,14 +1852,12 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="11.6262626262626"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="10.959595959596"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="22.3181818181818"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="19.7777777777778"/>
-    <col collapsed="false" hidden="false" max="7" min="5" style="0" width="7.34848484848485"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="21.9141414141414"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="17.5050505050505"/>
-    <col collapsed="false" hidden="false" max="1025" min="10" style="0" width="7.34848484848485"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="11.2272727272727"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="10.6919191919192"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="21.7828282828283"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="19.2424242424242"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="21.3787878787879"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="17.1060606060606"/>
   </cols>
   <sheetData>
     <row r="1" s="2" customFormat="true" ht="18.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1989,12 +1983,12 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="3" width="25.9242424242424"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="3" width="40.3535353535354"/>
-    <col collapsed="false" hidden="false" max="4" min="3" style="3" width="60.8030303030303"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="3" width="69.0858585858586"/>
-    <col collapsed="false" hidden="false" max="1023" min="6" style="3" width="3.47474747474747"/>
-    <col collapsed="false" hidden="false" max="1025" min="1024" style="0" width="3.47474747474747"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="3" width="25.2575757575758"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="3" width="39.4191919191919"/>
+    <col collapsed="false" hidden="false" max="4" min="3" style="3" width="59.5959595959596"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="3" width="67.6161616161616"/>
+    <col collapsed="false" hidden="false" max="1023" min="6" style="3" width="3.33838383838384"/>
+    <col collapsed="false" hidden="false" max="1025" min="1024" style="0" width="3.33838383838384"/>
   </cols>
   <sheetData>
     <row r="1" s="1" customFormat="true" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -37137,22 +37131,18 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="7.34848484848485"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="10.4242424242424"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="8.95454545454546"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="32.0707070707071"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="18.5757575757576"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="16.5707070707071"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="25.1212121212121"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="18.8434343434343"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="13.0959595959596"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="8.68686868686869"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="7.34848484848485"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="11.2272727272727"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="15.5"/>
-    <col collapsed="false" hidden="false" max="19" min="14" style="0" width="7.34848484848485"/>
-    <col collapsed="false" hidden="false" max="20" min="20" style="0" width="17.1060606060606"/>
-    <col collapsed="false" hidden="false" max="1025" min="21" style="0" width="7.34848484848485"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="10.1565656565657"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="8.68686868686869"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="31.2676767676768"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="18.1717171717172"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="16.1666666666667"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="24.5858585858586"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="18.4393939393939"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="12.8282828282828"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="8.41919191919192"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="10.959595959596"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="15.1010101010101"/>
+    <col collapsed="false" hidden="false" max="20" min="20" style="0" width="16.7020202020202"/>
   </cols>
   <sheetData>
     <row r="1" s="6" customFormat="true" ht="17.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -37453,20 +37443,19 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:F49"/>
+  <dimension ref="A1:F48"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A13" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B33" activeCellId="0" sqref="B33"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B21" activeCellId="0" sqref="B21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="13.4949494949495"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="20.979797979798"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="19.9090909090909"/>
-    <col collapsed="false" hidden="false" max="5" min="4" style="0" width="27.9292929292929"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="42.0909090909091"/>
-    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="7.34848484848485"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="13.0959595959596"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="36.5808080808081"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="19.3737373737374"/>
+    <col collapsed="false" hidden="false" max="5" min="4" style="0" width="27.2626262626263"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="41.1565656565657"/>
   </cols>
   <sheetData>
     <row r="1" s="1" customFormat="true" ht="22.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -37898,7 +37887,7 @@
       </c>
       <c r="F31" s="8"/>
     </row>
-    <row r="32" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="32" customFormat="false" ht="14.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B32" s="9" t="s">
         <v>91</v>
       </c>
@@ -37918,13 +37907,13 @@
         <v>91</v>
       </c>
       <c r="C33" s="9" t="s">
-        <v>160</v>
-      </c>
-      <c r="D33" s="9" t="s">
-        <v>160</v>
-      </c>
-      <c r="E33" s="8" t="s">
-        <v>161</v>
+        <v>114</v>
+      </c>
+      <c r="D33" s="8" t="s">
+        <v>51</v>
+      </c>
+      <c r="E33" s="9" t="s">
+        <v>50</v>
       </c>
       <c r="F33" s="8"/>
     </row>
@@ -37933,50 +37922,48 @@
         <v>91</v>
       </c>
       <c r="C34" s="9" t="s">
-        <v>114</v>
+        <v>105</v>
       </c>
       <c r="D34" s="8" t="s">
-        <v>51</v>
+        <v>106</v>
       </c>
       <c r="E34" s="9" t="s">
-        <v>50</v>
+        <v>107</v>
       </c>
       <c r="F34" s="8"/>
     </row>
-    <row r="35" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B35" s="9" t="s">
-        <v>91</v>
-      </c>
-      <c r="C35" s="9" t="s">
-        <v>105</v>
-      </c>
-      <c r="D35" s="8" t="s">
-        <v>106</v>
-      </c>
-      <c r="E35" s="9" t="s">
-        <v>107</v>
-      </c>
-      <c r="F35" s="8"/>
+    <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B35" s="7"/>
+      <c r="C35" s="7"/>
+      <c r="F35" s="7"/>
     </row>
-    <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B36" s="7"/>
-      <c r="C36" s="7"/>
-      <c r="D36" s="7"/>
-      <c r="E36" s="7"/>
-      <c r="F36" s="7"/>
+    <row r="36" customFormat="false" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B36" s="9" t="s">
+        <v>95</v>
+      </c>
+      <c r="C36" s="9" t="s">
+        <v>160</v>
+      </c>
+      <c r="D36" s="8" t="s">
+        <v>161</v>
+      </c>
+      <c r="E36" s="9" t="s">
+        <v>162</v>
+      </c>
+      <c r="F36" s="8"/>
     </row>
     <row r="37" customFormat="false" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B37" s="9" t="s">
         <v>95</v>
       </c>
       <c r="C37" s="9" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="D37" s="8" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="E37" s="9" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="F37" s="8"/>
     </row>
@@ -37985,13 +37972,13 @@
         <v>95</v>
       </c>
       <c r="C38" s="9" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="D38" s="8" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="E38" s="9" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="F38" s="8"/>
     </row>
@@ -38000,13 +37987,13 @@
         <v>95</v>
       </c>
       <c r="C39" s="9" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="D39" s="8" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="E39" s="9" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="F39" s="8"/>
     </row>
@@ -38015,43 +38002,43 @@
         <v>95</v>
       </c>
       <c r="C40" s="9" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="D40" s="8" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="E40" s="9" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="F40" s="8"/>
     </row>
-    <row r="41" customFormat="false" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B41" s="9" t="s">
-        <v>95</v>
-      </c>
-      <c r="C41" s="9" t="s">
-        <v>174</v>
-      </c>
-      <c r="D41" s="8" t="s">
+    <row r="42" customFormat="false" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B42" s="9" t="s">
+        <v>97</v>
+      </c>
+      <c r="C42" s="9" t="s">
         <v>175</v>
       </c>
-      <c r="E41" s="9" t="s">
+      <c r="D42" s="8" t="s">
         <v>176</v>
       </c>
-      <c r="F41" s="8"/>
+      <c r="E42" s="9" t="s">
+        <v>177</v>
+      </c>
+      <c r="F42" s="8"/>
     </row>
     <row r="43" customFormat="false" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B43" s="9" t="s">
         <v>97</v>
       </c>
       <c r="C43" s="9" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="D43" s="8" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="E43" s="9" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="F43" s="8"/>
     </row>
@@ -38060,13 +38047,13 @@
         <v>97</v>
       </c>
       <c r="C44" s="9" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="D44" s="8" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="E44" s="9" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="F44" s="8"/>
     </row>
@@ -38075,13 +38062,13 @@
         <v>97</v>
       </c>
       <c r="C45" s="9" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
       <c r="D45" s="8" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="E45" s="9" t="s">
-        <v>185</v>
+        <v>186</v>
       </c>
       <c r="F45" s="8"/>
     </row>
@@ -38090,28 +38077,28 @@
         <v>97</v>
       </c>
       <c r="C46" s="9" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="D46" s="8" t="s">
-        <v>187</v>
+        <v>188</v>
       </c>
       <c r="E46" s="9" t="s">
-        <v>188</v>
+        <v>189</v>
       </c>
       <c r="F46" s="8"/>
     </row>
-    <row r="47" customFormat="false" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="47" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B47" s="9" t="s">
         <v>97</v>
       </c>
       <c r="C47" s="9" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
       <c r="D47" s="8" t="s">
-        <v>190</v>
+        <v>103</v>
       </c>
       <c r="E47" s="9" t="s">
-        <v>191</v>
+        <v>104</v>
       </c>
       <c r="F47" s="8"/>
     </row>
@@ -38120,30 +38107,15 @@
         <v>97</v>
       </c>
       <c r="C48" s="9" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="D48" s="8" t="s">
-        <v>103</v>
+        <v>106</v>
       </c>
       <c r="E48" s="9" t="s">
-        <v>104</v>
+        <v>107</v>
       </c>
       <c r="F48" s="8"/>
-    </row>
-    <row r="49" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B49" s="9" t="s">
-        <v>97</v>
-      </c>
-      <c r="C49" s="9" t="s">
-        <v>193</v>
-      </c>
-      <c r="D49" s="8" t="s">
-        <v>106</v>
-      </c>
-      <c r="E49" s="9" t="s">
-        <v>107</v>
-      </c>
-      <c r="F49" s="8"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
@@ -38169,17 +38141,16 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="12.5606060606061"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="14.2979797979798"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="33.4090909090909"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="12.8282828282828"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="22.4494949494949"/>
-    <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="7.34848484848485"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="12.2929292929293"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="13.8989898989899"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="32.6060606060606"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="12.5606060606061"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="21.9141414141414"/>
   </cols>
   <sheetData>
     <row r="1" s="6" customFormat="true" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="B1" s="12" t="s">
         <v>1</v>
@@ -38191,13 +38162,13 @@
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="3" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="B2" s="3" t="s">
         <v>79</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -38233,7 +38204,7 @@
         <v>84</v>
       </c>
       <c r="C7" s="7" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -38241,7 +38212,7 @@
         <v>84</v>
       </c>
       <c r="C8" s="7" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -38249,7 +38220,7 @@
         <v>84</v>
       </c>
       <c r="C9" s="7" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -38309,7 +38280,7 @@
         <v>80</v>
       </c>
       <c r="C18" s="3" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -38317,7 +38288,7 @@
         <v>80</v>
       </c>
       <c r="C19" s="3" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -38325,7 +38296,7 @@
         <v>80</v>
       </c>
       <c r="C20" s="3" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -38333,7 +38304,7 @@
         <v>80</v>
       </c>
       <c r="C21" s="3" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -38341,7 +38312,7 @@
         <v>80</v>
       </c>
       <c r="C22" s="3" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -38349,7 +38320,7 @@
         <v>80</v>
       </c>
       <c r="C23" s="3" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -38357,7 +38328,7 @@
         <v>80</v>
       </c>
       <c r="C24" s="3" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -38365,7 +38336,7 @@
         <v>80</v>
       </c>
       <c r="C25" s="3" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -38373,7 +38344,7 @@
         <v>80</v>
       </c>
       <c r="C26" s="3" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -38381,7 +38352,7 @@
         <v>80</v>
       </c>
       <c r="C27" s="3" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -38389,7 +38360,7 @@
         <v>80</v>
       </c>
       <c r="C28" s="3" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -38397,7 +38368,7 @@
         <v>80</v>
       </c>
       <c r="C29" s="3" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -38405,7 +38376,7 @@
         <v>80</v>
       </c>
       <c r="C30" s="3" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -38413,7 +38384,7 @@
         <v>80</v>
       </c>
       <c r="C31" s="3" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -38421,7 +38392,7 @@
         <v>80</v>
       </c>
       <c r="C32" s="3" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -38429,7 +38400,7 @@
         <v>80</v>
       </c>
       <c r="C33" s="3" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -38437,7 +38408,7 @@
         <v>80</v>
       </c>
       <c r="C34" s="3" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -38445,7 +38416,7 @@
         <v>80</v>
       </c>
       <c r="C35" s="3" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -38453,7 +38424,7 @@
         <v>80</v>
       </c>
       <c r="C36" s="3" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -38461,7 +38432,7 @@
         <v>80</v>
       </c>
       <c r="C37" s="3" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -38469,7 +38440,7 @@
         <v>80</v>
       </c>
       <c r="C38" s="3" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -38477,7 +38448,7 @@
         <v>80</v>
       </c>
       <c r="C39" s="3" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -38485,7 +38456,7 @@
         <v>80</v>
       </c>
       <c r="C40" s="3" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -38493,7 +38464,7 @@
         <v>80</v>
       </c>
       <c r="C41" s="3" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -38501,7 +38472,7 @@
         <v>80</v>
       </c>
       <c r="C42" s="3" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -38509,7 +38480,7 @@
         <v>80</v>
       </c>
       <c r="C43" s="3" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -38517,7 +38488,7 @@
         <v>80</v>
       </c>
       <c r="C44" s="3" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -38525,7 +38496,7 @@
         <v>80</v>
       </c>
       <c r="C45" s="3" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -38533,7 +38504,7 @@
         <v>80</v>
       </c>
       <c r="C46" s="3" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -38541,7 +38512,7 @@
         <v>80</v>
       </c>
       <c r="C47" s="3" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -38549,7 +38520,7 @@
         <v>80</v>
       </c>
       <c r="C48" s="3" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -38557,7 +38528,7 @@
         <v>80</v>
       </c>
       <c r="C49" s="3" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -38565,7 +38536,7 @@
         <v>80</v>
       </c>
       <c r="C50" s="3" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -38573,7 +38544,7 @@
         <v>80</v>
       </c>
       <c r="C51" s="3" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
     </row>
     <row r="52" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -38581,7 +38552,7 @@
         <v>80</v>
       </c>
       <c r="C52" s="3" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
     </row>
     <row r="53" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -38589,7 +38560,7 @@
         <v>80</v>
       </c>
       <c r="C53" s="3" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
     </row>
     <row r="54" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -38597,7 +38568,7 @@
         <v>80</v>
       </c>
       <c r="C54" s="3" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
     </row>
     <row r="55" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -38605,7 +38576,7 @@
         <v>80</v>
       </c>
       <c r="C55" s="3" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
     </row>
     <row r="56" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -38613,7 +38584,7 @@
         <v>80</v>
       </c>
       <c r="C56" s="3" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
     </row>
     <row r="57" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -38621,7 +38592,7 @@
         <v>80</v>
       </c>
       <c r="C57" s="3" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
     </row>
     <row r="58" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -38629,7 +38600,7 @@
         <v>80</v>
       </c>
       <c r="C58" s="3" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
     </row>
     <row r="59" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -38637,7 +38608,7 @@
         <v>80</v>
       </c>
       <c r="C59" s="3" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
     </row>
     <row r="60" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -38645,7 +38616,7 @@
         <v>80</v>
       </c>
       <c r="C60" s="3" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
     </row>
     <row r="61" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -38653,7 +38624,7 @@
         <v>80</v>
       </c>
       <c r="C61" s="3" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
     </row>
     <row r="62" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -38661,7 +38632,7 @@
         <v>80</v>
       </c>
       <c r="C62" s="3" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
     </row>
     <row r="63" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -38669,7 +38640,7 @@
         <v>80</v>
       </c>
       <c r="C63" s="3" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
     </row>
     <row r="64" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -38677,7 +38648,7 @@
         <v>80</v>
       </c>
       <c r="C64" s="3" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
     </row>
     <row r="65" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -38685,7 +38656,7 @@
         <v>80</v>
       </c>
       <c r="C65" s="3" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
     </row>
     <row r="66" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -38693,7 +38664,7 @@
         <v>80</v>
       </c>
       <c r="C66" s="3" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
     </row>
     <row r="68" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -38701,7 +38672,7 @@
         <v>80</v>
       </c>
       <c r="C68" s="3" t="s">
-        <v>249</v>
+        <v>247</v>
       </c>
     </row>
     <row r="69" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -38709,7 +38680,7 @@
         <v>80</v>
       </c>
       <c r="C69" s="3" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
     </row>
     <row r="70" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -38717,7 +38688,7 @@
         <v>80</v>
       </c>
       <c r="C70" s="3" t="s">
-        <v>251</v>
+        <v>249</v>
       </c>
     </row>
     <row r="71" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -38725,7 +38696,7 @@
         <v>80</v>
       </c>
       <c r="C71" s="3" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
     </row>
     <row r="72" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -38733,7 +38704,7 @@
         <v>80</v>
       </c>
       <c r="C72" s="3" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
     </row>
     <row r="73" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -38741,7 +38712,7 @@
         <v>80</v>
       </c>
       <c r="C73" s="3" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
     </row>
     <row r="74" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -38749,7 +38720,7 @@
         <v>80</v>
       </c>
       <c r="C74" s="3" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
     </row>
     <row r="75" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -38757,7 +38728,7 @@
         <v>80</v>
       </c>
       <c r="C75" s="3" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
     </row>
     <row r="76" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -38765,7 +38736,7 @@
         <v>80</v>
       </c>
       <c r="C76" s="3" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
     </row>
     <row r="77" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -38773,7 +38744,7 @@
         <v>80</v>
       </c>
       <c r="C77" s="3" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
     </row>
     <row r="78" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -38781,7 +38752,7 @@
         <v>80</v>
       </c>
       <c r="C78" s="3" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
     </row>
     <row r="79" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -38789,7 +38760,7 @@
         <v>80</v>
       </c>
       <c r="C79" s="3" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
     </row>
     <row r="80" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -38797,7 +38768,7 @@
         <v>80</v>
       </c>
       <c r="C80" s="3" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
     </row>
     <row r="81" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -38805,7 +38776,7 @@
         <v>80</v>
       </c>
       <c r="C81" s="3" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
     </row>
     <row r="82" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -38813,7 +38784,7 @@
         <v>80</v>
       </c>
       <c r="C82" s="3" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
     </row>
     <row r="83" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -38821,7 +38792,7 @@
         <v>80</v>
       </c>
       <c r="C83" s="3" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
     </row>
     <row r="84" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -38829,7 +38800,7 @@
         <v>80</v>
       </c>
       <c r="C84" s="3" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
     </row>
     <row r="85" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -38837,7 +38808,7 @@
         <v>80</v>
       </c>
       <c r="C85" s="3" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
     </row>
     <row r="86" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -38845,7 +38816,7 @@
         <v>80</v>
       </c>
       <c r="C86" s="3" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
     </row>
     <row r="87" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -38853,7 +38824,7 @@
         <v>80</v>
       </c>
       <c r="C87" s="3" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
     </row>
     <row r="89" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -38861,7 +38832,7 @@
         <v>80</v>
       </c>
       <c r="C89" s="3" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
     </row>
     <row r="90" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -38869,7 +38840,7 @@
         <v>80</v>
       </c>
       <c r="C90" s="3" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
     </row>
     <row r="91" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -38877,7 +38848,7 @@
         <v>80</v>
       </c>
       <c r="C91" s="3" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
     </row>
     <row r="92" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -38885,7 +38856,7 @@
         <v>80</v>
       </c>
       <c r="C92" s="3" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
     </row>
     <row r="93" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -38893,7 +38864,7 @@
         <v>80</v>
       </c>
       <c r="C93" s="3" t="s">
-        <v>273</v>
+        <v>271</v>
       </c>
     </row>
     <row r="94" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -38901,7 +38872,7 @@
         <v>80</v>
       </c>
       <c r="C94" s="3" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
     </row>
     <row r="95" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -38909,7 +38880,7 @@
         <v>80</v>
       </c>
       <c r="C95" s="3" t="s">
-        <v>275</v>
+        <v>273</v>
       </c>
     </row>
     <row r="96" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -38917,7 +38888,7 @@
         <v>80</v>
       </c>
       <c r="C96" s="3" t="s">
-        <v>276</v>
+        <v>274</v>
       </c>
     </row>
     <row r="97" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -38925,7 +38896,7 @@
         <v>80</v>
       </c>
       <c r="C97" s="3" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
     </row>
     <row r="98" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -38933,7 +38904,7 @@
         <v>80</v>
       </c>
       <c r="C98" s="3" t="s">
-        <v>278</v>
+        <v>276</v>
       </c>
     </row>
     <row r="99" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -38941,7 +38912,7 @@
         <v>80</v>
       </c>
       <c r="C99" s="3" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
     </row>
     <row r="100" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -38949,7 +38920,7 @@
         <v>80</v>
       </c>
       <c r="C100" s="3" t="s">
-        <v>280</v>
+        <v>278</v>
       </c>
     </row>
     <row r="101" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -38957,7 +38928,7 @@
         <v>80</v>
       </c>
       <c r="C101" s="3" t="s">
-        <v>281</v>
+        <v>279</v>
       </c>
     </row>
     <row r="102" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -38965,7 +38936,7 @@
         <v>80</v>
       </c>
       <c r="C102" s="3" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
     </row>
     <row r="103" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -38973,7 +38944,7 @@
         <v>80</v>
       </c>
       <c r="C103" s="3" t="s">
-        <v>283</v>
+        <v>281</v>
       </c>
     </row>
     <row r="104" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -38981,7 +38952,7 @@
         <v>80</v>
       </c>
       <c r="C104" s="3" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
     </row>
     <row r="105" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -38989,7 +38960,7 @@
         <v>80</v>
       </c>
       <c r="C105" s="3" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
     </row>
     <row r="106" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -38997,7 +38968,7 @@
         <v>80</v>
       </c>
       <c r="C106" s="3" t="s">
-        <v>286</v>
+        <v>284</v>
       </c>
     </row>
     <row r="107" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -39005,7 +38976,7 @@
         <v>80</v>
       </c>
       <c r="C107" s="3" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
     </row>
     <row r="108" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -39013,7 +38984,7 @@
         <v>80</v>
       </c>
       <c r="C108" s="3" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
     </row>
     <row r="109" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -39021,7 +38992,7 @@
         <v>80</v>
       </c>
       <c r="C109" s="7" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
     </row>
     <row r="111" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -39029,7 +39000,7 @@
         <v>80</v>
       </c>
       <c r="C111" s="3" t="s">
-        <v>290</v>
+        <v>288</v>
       </c>
     </row>
     <row r="112" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -39037,7 +39008,7 @@
         <v>80</v>
       </c>
       <c r="C112" s="7" t="s">
-        <v>291</v>
+        <v>289</v>
       </c>
     </row>
   </sheetData>
@@ -39064,14 +39035,13 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="32.6060606060606"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="38.3535353535354"/>
-    <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="7.34848484848485"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="31.8030303030303"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="37.4141414141414"/>
   </cols>
   <sheetData>
     <row r="1" s="2" customFormat="true" ht="13.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
-        <v>292</v>
+        <v>290</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>68</v>
@@ -39079,26 +39049,26 @@
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="7" t="s">
-        <v>293</v>
+        <v>291</v>
       </c>
       <c r="B3" s="7" t="s">
-        <v>294</v>
+        <v>292</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="7" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
       <c r="B4" s="7" t="s">
-        <v>296</v>
+        <v>294</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="7" t="s">
-        <v>297</v>
+        <v>295</v>
       </c>
       <c r="B5" s="7" t="s">
-        <v>298</v>
+        <v>296</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
add trafficker and kwosung
</commit_message>
<xml_diff>
--- a/tables/actor/forms/actor/actor.xlsx
+++ b/tables/actor/forms/actor/actor.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="988" firstSheet="0" activeTab="4"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="964" firstSheet="0" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="initial" sheetId="1" state="visible" r:id="rId2"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="529" uniqueCount="297">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="533" uniqueCount="299">
   <si>
     <t xml:space="preserve">clause</t>
   </si>
@@ -1587,6 +1587,12 @@
     <t xml:space="preserve">smugglerOrTransporterForMigrant</t>
   </si>
   <si>
+    <t xml:space="preserve">traffickerForMigrant</t>
+  </si>
+  <si>
+    <t xml:space="preserve">kwoswungForMigrant</t>
+  </si>
+  <si>
     <t xml:space="preserve">calculation_name</t>
   </si>
   <si>
@@ -1791,11 +1797,11 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="11.6262626262626"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="8.41919191919192"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="14.6969696969697"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="33.540404040404"/>
-    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="8.41919191919192"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="11.2272727272727"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="8.15151515151515"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="14.2979797979798"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="32.8737373737374"/>
+    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="8.15151515151515"/>
   </cols>
   <sheetData>
     <row r="1" s="2" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1852,12 +1858,14 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="11.2272727272727"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="10.6919191919192"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="21.7828282828283"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="19.2424242424242"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="21.3787878787879"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="17.1060606060606"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="10.959595959596"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="10.4242424242424"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="21.2474747474747"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="18.8434343434343"/>
+    <col collapsed="false" hidden="false" max="7" min="5" style="0" width="8.41919191919192"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="20.979797979798"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="16.7020202020202"/>
+    <col collapsed="false" hidden="false" max="1025" min="10" style="0" width="8.41919191919192"/>
   </cols>
   <sheetData>
     <row r="1" s="2" customFormat="true" ht="18.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1983,12 +1991,12 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="3" width="25.2575757575758"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="3" width="39.4191919191919"/>
-    <col collapsed="false" hidden="false" max="4" min="3" style="3" width="59.5959595959596"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="3" width="67.6161616161616"/>
-    <col collapsed="false" hidden="false" max="1023" min="6" style="3" width="3.33838383838384"/>
-    <col collapsed="false" hidden="false" max="1025" min="1024" style="0" width="3.33838383838384"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="3" width="24.7222222222222"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="3" width="38.4848484848485"/>
+    <col collapsed="false" hidden="false" max="4" min="3" style="3" width="58.2626262626263"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="3" width="66.1464646464647"/>
+    <col collapsed="false" hidden="false" max="1023" min="6" style="3" width="3.20707070707071"/>
+    <col collapsed="false" hidden="false" max="1025" min="1024" style="0" width="3.20707070707071"/>
   </cols>
   <sheetData>
     <row r="1" s="1" customFormat="true" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -37131,18 +37139,22 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="10.1565656565657"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="8.68686868686869"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="31.2676767676768"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="18.1717171717172"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="16.1666666666667"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="24.5858585858586"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="18.4393939393939"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="12.8282828282828"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="8.41919191919192"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="10.959595959596"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="15.1010101010101"/>
-    <col collapsed="false" hidden="false" max="20" min="20" style="0" width="16.7020202020202"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="8.41919191919192"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="9.88888888888889"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="8.41919191919192"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="30.6010101010101"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="17.6414141414141"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="15.7676767676768"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="24.0555555555556"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="18.040404040404"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="12.5606060606061"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="8.15151515151515"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="8.41919191919192"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="10.6919191919192"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="14.6969696969697"/>
+    <col collapsed="false" hidden="false" max="19" min="14" style="0" width="8.41919191919192"/>
+    <col collapsed="false" hidden="false" max="20" min="20" style="0" width="16.3030303030303"/>
+    <col collapsed="false" hidden="false" max="1025" min="21" style="0" width="8.41919191919192"/>
   </cols>
   <sheetData>
     <row r="1" s="6" customFormat="true" ht="17.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -37445,17 +37457,18 @@
   </sheetPr>
   <dimension ref="A1:F48"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A37" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="B21" activeCellId="0" sqref="B21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="13.0959595959596"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="36.5808080808081"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="19.3737373737374"/>
-    <col collapsed="false" hidden="false" max="5" min="4" style="0" width="27.2626262626263"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="41.1565656565657"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="12.8282828282828"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="35.8131313131313"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="18.9747474747475"/>
+    <col collapsed="false" hidden="false" max="5" min="4" style="0" width="26.5909090909091"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="40.2222222222222"/>
+    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="8.41919191919192"/>
   </cols>
   <sheetData>
     <row r="1" s="1" customFormat="true" ht="22.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -38133,19 +38146,20 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="1:112"/>
+  <dimension ref="1:114"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A100" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C19" activeCellId="0" sqref="C19"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A100" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C117" activeCellId="0" sqref="C117"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="12.2929292929293"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="13.8989898989899"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="32.6060606060606"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="12.5606060606061"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="21.9141414141414"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="12.0252525252525"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="13.4949494949495"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="31.8030303030303"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="12.2929292929293"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="21.3787878787879"/>
+    <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="8.41919191919192"/>
   </cols>
   <sheetData>
     <row r="1" s="6" customFormat="true" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -39009,6 +39023,22 @@
       </c>
       <c r="C112" s="7" t="s">
         <v>289</v>
+      </c>
+    </row>
+    <row r="113" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B113" s="7" t="s">
+        <v>80</v>
+      </c>
+      <c r="C113" s="7" t="s">
+        <v>290</v>
+      </c>
+    </row>
+    <row r="114" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B114" s="7" t="s">
+        <v>80</v>
+      </c>
+      <c r="C114" s="7" t="s">
+        <v>291</v>
       </c>
     </row>
   </sheetData>
@@ -39035,13 +39065,14 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="31.8030303030303"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="37.4141414141414"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="31.1363636363636"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="36.6161616161616"/>
+    <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="8.41919191919192"/>
   </cols>
   <sheetData>
     <row r="1" s="2" customFormat="true" ht="13.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
-        <v>290</v>
+        <v>292</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>68</v>
@@ -39049,26 +39080,26 @@
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="7" t="s">
-        <v>291</v>
+        <v>293</v>
       </c>
       <c r="B3" s="7" t="s">
-        <v>292</v>
+        <v>294</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="7" t="s">
-        <v>293</v>
+        <v>295</v>
       </c>
       <c r="B4" s="7" t="s">
-        <v>294</v>
+        <v>296</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="7" t="s">
-        <v>295</v>
+        <v>297</v>
       </c>
       <c r="B5" s="7" t="s">
-        <v>296</v>
+        <v>298</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
content content review with SES
</commit_message>
<xml_diff>
--- a/tables/actor/forms/actor/actor.xlsx
+++ b/tables/actor/forms/actor/actor.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="964" firstSheet="0" activeTab="5"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="988" firstSheet="0" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="initial" sheetId="1" state="visible" r:id="rId2"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="533" uniqueCount="299">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="543" uniqueCount="306">
   <si>
     <t xml:space="preserve">clause</t>
   </si>
@@ -793,25 +793,7 @@
     <t xml:space="preserve">Spouse</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="Myanmar3"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">[</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="Myanmar3"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">အိမ်ထောင်ဖက်</t>
-    </r>
+    <t xml:space="preserve">အိမ်ထောင်ဖက်</t>
   </si>
   <si>
     <t xml:space="preserve">Boyfriend or Girlfriend</t>
@@ -835,10 +817,76 @@
     <t xml:space="preserve">မောင်နှမအရင်း</t>
   </si>
   <si>
+    <t xml:space="preserve">Aunt/Uncle</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Myanmar3"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">အဒေါ်</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Myanmar3"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">/</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Myanmar3"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">ဦးလေး</t>
+    </r>
+  </si>
+  <si>
     <t xml:space="preserve">Grandparent</t>
   </si>
   <si>
     <t xml:space="preserve">အဖိုးအဖွား</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Parent-in-law</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Myanmar3"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">ယောက်ကထီး</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Myanmar3"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">/</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Myanmar3"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">ယောက်ခမ</t>
+    </r>
   </si>
   <si>
     <t xml:space="preserve">Extended Family</t>
@@ -1060,6 +1108,39 @@
   </si>
   <si>
     <t xml:space="preserve">ရွေ့ပြောင်းမှုတွင်အကျိုးဆောင်သူအားလုံး </t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Myanmar3"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">အခြား</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Myanmar3"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">: </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Myanmar3"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">ဖော်ပြရန်</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">Other: Specify</t>
   </si>
   <si>
     <t xml:space="preserve">never</t>
@@ -1593,6 +1674,9 @@
     <t xml:space="preserve">kwoswungForMigrant</t>
   </si>
   <si>
+    <t xml:space="preserve">paidLikeYou</t>
+  </si>
+  <si>
     <t xml:space="preserve">calculation_name</t>
   </si>
   <si>
@@ -1797,11 +1881,11 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="11.2272727272727"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="8.15151515151515"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="14.2979797979798"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="32.8737373737374"/>
-    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="8.15151515151515"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="10.6919191919192"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="7.61616161616162"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="13.4949494949495"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="31.2676767676768"/>
+    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="7.61616161616162"/>
   </cols>
   <sheetData>
     <row r="1" s="2" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1858,14 +1942,14 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="10.959595959596"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="10.4242424242424"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="21.2474747474747"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="18.8434343434343"/>
-    <col collapsed="false" hidden="false" max="7" min="5" style="0" width="8.41919191919192"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="20.979797979798"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="16.7020202020202"/>
-    <col collapsed="false" hidden="false" max="1025" min="10" style="0" width="8.41919191919192"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="10.4242424242424"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="9.88888888888889"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="20.3131313131313"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="18.040404040404"/>
+    <col collapsed="false" hidden="false" max="7" min="5" style="0" width="7.88383838383838"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="19.9090909090909"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="15.9040404040404"/>
+    <col collapsed="false" hidden="false" max="1025" min="10" style="0" width="7.88383838383838"/>
   </cols>
   <sheetData>
     <row r="1" s="2" customFormat="true" ht="18.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1986,17 +2070,17 @@
   <dimension ref="1:65"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C14" activeCellId="0" sqref="C14"/>
+      <selection pane="topLeft" activeCell="A17" activeCellId="0" sqref="A17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="3" width="24.7222222222222"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="3" width="38.4848484848485"/>
-    <col collapsed="false" hidden="false" max="4" min="3" style="3" width="58.2626262626263"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="3" width="66.1464646464647"/>
-    <col collapsed="false" hidden="false" max="1023" min="6" style="3" width="3.20707070707071"/>
-    <col collapsed="false" hidden="false" max="1025" min="1024" style="0" width="3.20707070707071"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="3" width="23.520202020202"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="3" width="36.7474747474747"/>
+    <col collapsed="false" hidden="false" max="4" min="3" style="3" width="55.7222222222222"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="3" width="63.3383838383838"/>
+    <col collapsed="false" hidden="false" max="1023" min="6" style="3" width="3.07575757575758"/>
+    <col collapsed="false" hidden="false" max="1025" min="1024" style="0" width="8.41919191919192"/>
   </cols>
   <sheetData>
     <row r="1" s="1" customFormat="true" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -37133,28 +37217,27 @@
   </sheetPr>
   <dimension ref="1:19"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H6" activeCellId="0" sqref="H6"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="H10" activeCellId="0" sqref="H10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="8.41919191919192"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="9.88888888888889"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="8.41919191919192"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="30.6010101010101"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="17.6414141414141"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="15.7676767676768"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="24.0555555555556"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="18.040404040404"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="12.5606060606061"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="8.15151515151515"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="8.41919191919192"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="10.6919191919192"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="14.6969696969697"/>
-    <col collapsed="false" hidden="false" max="19" min="14" style="0" width="8.41919191919192"/>
-    <col collapsed="false" hidden="false" max="20" min="20" style="0" width="16.3030303030303"/>
-    <col collapsed="false" hidden="false" max="1025" min="21" style="0" width="8.41919191919192"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="7.88383838383838"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="9.35353535353535"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="7.88383838383838"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="29.2626262626263"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="27.9191919191919"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="22.8232323232323"/>
+    <col collapsed="false" hidden="false" max="8" min="7" style="0" width="33.8333333333333"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="12.0252525252525"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="7.61616161616162"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="7.88383838383838"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="10.1565656565657"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="13.8989898989899"/>
+    <col collapsed="false" hidden="false" max="19" min="14" style="0" width="7.88383838383838"/>
+    <col collapsed="false" hidden="false" max="20" min="20" style="0" width="15.5"/>
+    <col collapsed="false" hidden="false" max="1025" min="21" style="0" width="7.88383838383838"/>
   </cols>
   <sheetData>
     <row r="1" s="6" customFormat="true" ht="17.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -37289,7 +37372,9 @@
       <c r="H5" s="4" t="s">
         <v>81</v>
       </c>
-      <c r="I5" s="3"/>
+      <c r="I5" s="3" t="n">
+        <v>1</v>
+      </c>
       <c r="L5" s="3"/>
     </row>
     <row r="6" customFormat="false" ht="21.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -37339,6 +37424,9 @@
       <c r="H9" s="7" t="s">
         <v>87</v>
       </c>
+      <c r="I9" s="0" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C10" s="7" t="s">
@@ -37379,6 +37467,9 @@
       <c r="H13" s="7" t="s">
         <v>91</v>
       </c>
+      <c r="I13" s="0" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C14" s="7" t="s">
@@ -37419,6 +37510,9 @@
       <c r="H17" s="9" t="s">
         <v>95</v>
       </c>
+      <c r="I17" s="0" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="18" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E18" s="9" t="s">
@@ -37432,6 +37526,9 @@
       </c>
       <c r="H18" s="7" t="s">
         <v>97</v>
+      </c>
+      <c r="I18" s="0" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -37455,20 +37552,21 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:F48"/>
+  <dimension ref="A1:F54"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A37" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B21" activeCellId="0" sqref="B21"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A13" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C39" activeCellId="0" sqref="C39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="12.8282828282828"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="35.8131313131313"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="18.9747474747475"/>
-    <col collapsed="false" hidden="false" max="5" min="4" style="0" width="26.5909090909091"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="40.2222222222222"/>
-    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="8.41919191919192"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="12.2929292929293"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="34.2070707070707"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="29.5656565656566"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="40.0151515151515"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="38.7777777777778"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="38.4848484848485"/>
+    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="7.88383838383838"/>
   </cols>
   <sheetData>
     <row r="1" s="1" customFormat="true" ht="22.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -37600,14 +37698,14 @@
       </c>
       <c r="F10" s="8"/>
     </row>
-    <row r="12" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="12" customFormat="false" ht="14.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B12" s="9" t="s">
         <v>91</v>
       </c>
       <c r="C12" s="9" t="s">
         <v>115</v>
       </c>
-      <c r="D12" s="9" t="s">
+      <c r="D12" s="8" t="s">
         <v>116</v>
       </c>
       <c r="E12" s="9" t="s">
@@ -37630,7 +37728,7 @@
       </c>
       <c r="F13" s="8"/>
     </row>
-    <row r="14" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="14" customFormat="false" ht="14.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B14" s="9" t="s">
         <v>91</v>
       </c>
@@ -37645,7 +37743,7 @@
       </c>
       <c r="F14" s="8"/>
     </row>
-    <row r="15" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="15" customFormat="false" ht="14.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B15" s="9" t="s">
         <v>91</v>
       </c>
@@ -37660,7 +37758,7 @@
       </c>
       <c r="F15" s="8"/>
     </row>
-    <row r="16" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="16" customFormat="false" ht="14.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B16" s="9" t="s">
         <v>91</v>
       </c>
@@ -37675,7 +37773,7 @@
       </c>
       <c r="F16" s="8"/>
     </row>
-    <row r="17" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="17" customFormat="false" ht="14.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B17" s="9" t="s">
         <v>91</v>
       </c>
@@ -37690,7 +37788,7 @@
       </c>
       <c r="F17" s="8"/>
     </row>
-    <row r="18" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="18" customFormat="false" ht="14.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B18" s="9" t="s">
         <v>91</v>
       </c>
@@ -37705,7 +37803,7 @@
       </c>
       <c r="F18" s="8"/>
     </row>
-    <row r="19" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="19" customFormat="false" ht="14.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B19" s="9" t="s">
         <v>91</v>
       </c>
@@ -37720,7 +37818,7 @@
       </c>
       <c r="F19" s="8"/>
     </row>
-    <row r="20" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="20" customFormat="false" ht="14.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B20" s="9" t="s">
         <v>91</v>
       </c>
@@ -37735,7 +37833,7 @@
       </c>
       <c r="F20" s="8"/>
     </row>
-    <row r="21" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="21" customFormat="false" ht="14.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B21" s="9" t="s">
         <v>91</v>
       </c>
@@ -37765,7 +37863,7 @@
       </c>
       <c r="F22" s="8"/>
     </row>
-    <row r="23" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="23" customFormat="false" ht="14.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B23" s="9" t="s">
         <v>91</v>
       </c>
@@ -37780,7 +37878,7 @@
       </c>
       <c r="F23" s="8"/>
     </row>
-    <row r="24" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="24" customFormat="false" ht="14.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B24" s="9" t="s">
         <v>91</v>
       </c>
@@ -37791,41 +37889,41 @@
         <v>141</v>
       </c>
       <c r="E24" s="9" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="F24" s="8"/>
     </row>
-    <row r="25" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="25" customFormat="false" ht="14.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B25" s="9" t="s">
         <v>91</v>
       </c>
       <c r="C25" s="9" t="s">
+        <v>142</v>
+      </c>
+      <c r="D25" s="8" t="s">
         <v>143</v>
       </c>
-      <c r="D25" s="8" t="s">
-        <v>144</v>
-      </c>
       <c r="E25" s="9" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="F25" s="8"/>
     </row>
-    <row r="26" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="26" customFormat="false" ht="14.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B26" s="9" t="s">
         <v>91</v>
       </c>
       <c r="C26" s="9" t="s">
+        <v>144</v>
+      </c>
+      <c r="D26" s="8" t="s">
         <v>145</v>
       </c>
-      <c r="D26" s="8" t="s">
+      <c r="E26" s="9" t="s">
         <v>146</v>
-      </c>
-      <c r="E26" s="9" t="s">
-        <v>145</v>
       </c>
       <c r="F26" s="8"/>
     </row>
-    <row r="27" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="27" customFormat="false" ht="14.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B27" s="9" t="s">
         <v>91</v>
       </c>
@@ -37840,7 +37938,7 @@
       </c>
       <c r="F27" s="8"/>
     </row>
-    <row r="28" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="28" customFormat="false" ht="14.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B28" s="9" t="s">
         <v>91</v>
       </c>
@@ -37881,7 +37979,7 @@
         <v>154</v>
       </c>
       <c r="E30" s="9" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="F30" s="8"/>
     </row>
@@ -37890,245 +37988,303 @@
         <v>91</v>
       </c>
       <c r="C31" s="9" t="s">
+        <v>155</v>
+      </c>
+      <c r="D31" s="8" t="s">
         <v>156</v>
       </c>
-      <c r="D31" s="8" t="s">
-        <v>157</v>
-      </c>
       <c r="E31" s="9" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="F31" s="8"/>
     </row>
-    <row r="32" customFormat="false" ht="14.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="32" customFormat="false" ht="26.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B32" s="9" t="s">
         <v>91</v>
       </c>
       <c r="C32" s="9" t="s">
+        <v>157</v>
+      </c>
+      <c r="D32" s="8" t="s">
         <v>158</v>
       </c>
-      <c r="D32" s="8" t="s">
+      <c r="E32" s="9" t="s">
         <v>159</v>
-      </c>
-      <c r="E32" s="9" t="s">
-        <v>158</v>
       </c>
       <c r="F32" s="8"/>
     </row>
-    <row r="33" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="33" customFormat="false" ht="14.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B33" s="9" t="s">
         <v>91</v>
       </c>
       <c r="C33" s="9" t="s">
-        <v>114</v>
+        <v>160</v>
       </c>
       <c r="D33" s="8" t="s">
-        <v>51</v>
+        <v>161</v>
       </c>
       <c r="E33" s="9" t="s">
-        <v>50</v>
+        <v>160</v>
       </c>
       <c r="F33" s="8"/>
     </row>
-    <row r="34" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="34" customFormat="false" ht="14.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B34" s="9" t="s">
         <v>91</v>
       </c>
       <c r="C34" s="9" t="s">
-        <v>105</v>
+        <v>162</v>
       </c>
       <c r="D34" s="8" t="s">
-        <v>106</v>
+        <v>163</v>
       </c>
       <c r="E34" s="9" t="s">
-        <v>107</v>
+        <v>162</v>
       </c>
       <c r="F34" s="8"/>
     </row>
-    <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B35" s="7"/>
-      <c r="C35" s="7"/>
-      <c r="F35" s="7"/>
+    <row r="35" customFormat="false" ht="14.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B35" s="9" t="s">
+        <v>91</v>
+      </c>
+      <c r="C35" s="9" t="s">
+        <v>114</v>
+      </c>
+      <c r="D35" s="8" t="s">
+        <v>164</v>
+      </c>
+      <c r="E35" s="9" t="s">
+        <v>165</v>
+      </c>
+      <c r="F35" s="8"/>
     </row>
-    <row r="36" customFormat="false" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="36" customFormat="false" ht="14.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B36" s="9" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
       <c r="C36" s="9" t="s">
-        <v>160</v>
+        <v>105</v>
       </c>
       <c r="D36" s="8" t="s">
-        <v>161</v>
+        <v>106</v>
       </c>
       <c r="E36" s="9" t="s">
-        <v>162</v>
+        <v>107</v>
       </c>
       <c r="F36" s="8"/>
     </row>
-    <row r="37" customFormat="false" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B37" s="9" t="s">
-        <v>95</v>
-      </c>
-      <c r="C37" s="9" t="s">
-        <v>163</v>
-      </c>
-      <c r="D37" s="8" t="s">
-        <v>164</v>
-      </c>
-      <c r="E37" s="9" t="s">
-        <v>165</v>
-      </c>
+    <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B37" s="8"/>
+      <c r="C37" s="8"/>
+      <c r="D37" s="8"/>
+      <c r="E37" s="8"/>
       <c r="F37" s="8"/>
     </row>
-    <row r="38" customFormat="false" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B38" s="9" t="s">
-        <v>95</v>
-      </c>
-      <c r="C38" s="9" t="s">
-        <v>166</v>
-      </c>
-      <c r="D38" s="8" t="s">
-        <v>167</v>
-      </c>
-      <c r="E38" s="9" t="s">
-        <v>168</v>
-      </c>
+    <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B38" s="8"/>
+      <c r="C38" s="8"/>
+      <c r="D38" s="8"/>
+      <c r="E38" s="8"/>
       <c r="F38" s="8"/>
     </row>
-    <row r="39" customFormat="false" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B39" s="9" t="s">
-        <v>95</v>
-      </c>
-      <c r="C39" s="9" t="s">
-        <v>169</v>
-      </c>
-      <c r="D39" s="8" t="s">
-        <v>170</v>
-      </c>
-      <c r="E39" s="9" t="s">
-        <v>171</v>
-      </c>
+    <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B39" s="8"/>
+      <c r="C39" s="8"/>
+      <c r="D39" s="8"/>
+      <c r="E39" s="8"/>
       <c r="F39" s="8"/>
     </row>
-    <row r="40" customFormat="false" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B40" s="9" t="s">
-        <v>95</v>
-      </c>
-      <c r="C40" s="9" t="s">
-        <v>172</v>
-      </c>
-      <c r="D40" s="8" t="s">
-        <v>173</v>
-      </c>
-      <c r="E40" s="9" t="s">
-        <v>174</v>
-      </c>
+    <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B40" s="8"/>
+      <c r="C40" s="8"/>
+      <c r="D40" s="8"/>
+      <c r="E40" s="8"/>
       <c r="F40" s="8"/>
+    </row>
+    <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B41" s="7"/>
+      <c r="C41" s="7"/>
+      <c r="F41" s="7"/>
     </row>
     <row r="42" customFormat="false" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B42" s="9" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="C42" s="9" t="s">
-        <v>175</v>
+        <v>166</v>
       </c>
       <c r="D42" s="8" t="s">
-        <v>176</v>
+        <v>167</v>
       </c>
       <c r="E42" s="9" t="s">
-        <v>177</v>
+        <v>168</v>
       </c>
       <c r="F42" s="8"/>
     </row>
     <row r="43" customFormat="false" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B43" s="9" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="C43" s="9" t="s">
-        <v>178</v>
+        <v>169</v>
       </c>
       <c r="D43" s="8" t="s">
-        <v>179</v>
+        <v>170</v>
       </c>
       <c r="E43" s="9" t="s">
-        <v>180</v>
+        <v>171</v>
       </c>
       <c r="F43" s="8"/>
     </row>
     <row r="44" customFormat="false" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B44" s="9" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="C44" s="9" t="s">
-        <v>181</v>
+        <v>172</v>
       </c>
       <c r="D44" s="8" t="s">
-        <v>182</v>
+        <v>173</v>
       </c>
       <c r="E44" s="9" t="s">
-        <v>183</v>
+        <v>174</v>
       </c>
       <c r="F44" s="8"/>
     </row>
     <row r="45" customFormat="false" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B45" s="9" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="C45" s="9" t="s">
-        <v>184</v>
+        <v>175</v>
       </c>
       <c r="D45" s="8" t="s">
-        <v>185</v>
+        <v>176</v>
       </c>
       <c r="E45" s="9" t="s">
-        <v>186</v>
+        <v>177</v>
       </c>
       <c r="F45" s="8"/>
     </row>
     <row r="46" customFormat="false" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B46" s="9" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="C46" s="9" t="s">
-        <v>187</v>
+        <v>178</v>
       </c>
       <c r="D46" s="8" t="s">
-        <v>188</v>
+        <v>179</v>
       </c>
       <c r="E46" s="9" t="s">
-        <v>189</v>
+        <v>180</v>
       </c>
       <c r="F46" s="8"/>
     </row>
-    <row r="47" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B47" s="9" t="s">
-        <v>97</v>
-      </c>
-      <c r="C47" s="9" t="s">
-        <v>190</v>
-      </c>
-      <c r="D47" s="8" t="s">
-        <v>103</v>
-      </c>
-      <c r="E47" s="9" t="s">
-        <v>104</v>
-      </c>
-      <c r="F47" s="8"/>
-    </row>
-    <row r="48" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="48" customFormat="false" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B48" s="9" t="s">
         <v>97</v>
       </c>
       <c r="C48" s="9" t="s">
+        <v>181</v>
+      </c>
+      <c r="D48" s="8" t="s">
+        <v>182</v>
+      </c>
+      <c r="E48" s="9" t="s">
+        <v>183</v>
+      </c>
+      <c r="F48" s="8"/>
+    </row>
+    <row r="49" customFormat="false" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B49" s="9" t="s">
+        <v>97</v>
+      </c>
+      <c r="C49" s="9" t="s">
+        <v>184</v>
+      </c>
+      <c r="D49" s="8" t="s">
+        <v>185</v>
+      </c>
+      <c r="E49" s="9" t="s">
+        <v>186</v>
+      </c>
+      <c r="F49" s="8"/>
+    </row>
+    <row r="50" customFormat="false" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B50" s="9" t="s">
+        <v>97</v>
+      </c>
+      <c r="C50" s="9" t="s">
+        <v>187</v>
+      </c>
+      <c r="D50" s="8" t="s">
+        <v>188</v>
+      </c>
+      <c r="E50" s="9" t="s">
+        <v>189</v>
+      </c>
+      <c r="F50" s="8"/>
+    </row>
+    <row r="51" customFormat="false" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B51" s="9" t="s">
+        <v>97</v>
+      </c>
+      <c r="C51" s="9" t="s">
+        <v>190</v>
+      </c>
+      <c r="D51" s="8" t="s">
         <v>191</v>
       </c>
-      <c r="D48" s="8" t="s">
+      <c r="E51" s="9" t="s">
+        <v>192</v>
+      </c>
+      <c r="F51" s="8"/>
+    </row>
+    <row r="52" customFormat="false" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B52" s="9" t="s">
+        <v>97</v>
+      </c>
+      <c r="C52" s="9" t="s">
+        <v>193</v>
+      </c>
+      <c r="D52" s="8" t="s">
+        <v>194</v>
+      </c>
+      <c r="E52" s="9" t="s">
+        <v>195</v>
+      </c>
+      <c r="F52" s="8"/>
+    </row>
+    <row r="53" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B53" s="9" t="s">
+        <v>97</v>
+      </c>
+      <c r="C53" s="9" t="s">
+        <v>196</v>
+      </c>
+      <c r="D53" s="8" t="s">
+        <v>103</v>
+      </c>
+      <c r="E53" s="9" t="s">
+        <v>104</v>
+      </c>
+      <c r="F53" s="8"/>
+    </row>
+    <row r="54" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B54" s="9" t="s">
+        <v>97</v>
+      </c>
+      <c r="C54" s="9" t="s">
+        <v>197</v>
+      </c>
+      <c r="D54" s="8" t="s">
         <v>106</v>
       </c>
-      <c r="E48" s="9" t="s">
+      <c r="E54" s="9" t="s">
         <v>107</v>
       </c>
-      <c r="F48" s="8"/>
+      <c r="F54" s="8"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
@@ -38146,25 +38302,25 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="1:114"/>
+  <dimension ref="1:116"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A100" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C117" activeCellId="0" sqref="C117"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A100" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B116" activeCellId="0" sqref="B116"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="12.0252525252525"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="13.4949494949495"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="31.8030303030303"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="12.2929292929293"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="21.3787878787879"/>
-    <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="8.41919191919192"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="11.2272727272727"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="12.8282828282828"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="30.469696969697"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="11.6262626262626"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="20.4444444444444"/>
+    <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="7.88383838383838"/>
   </cols>
   <sheetData>
     <row r="1" s="6" customFormat="true" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
-        <v>192</v>
+        <v>198</v>
       </c>
       <c r="B1" s="12" t="s">
         <v>1</v>
@@ -38176,13 +38332,13 @@
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="3" t="s">
-        <v>193</v>
+        <v>199</v>
       </c>
       <c r="B2" s="3" t="s">
         <v>79</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>194</v>
+        <v>200</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -38218,7 +38374,7 @@
         <v>84</v>
       </c>
       <c r="C7" s="7" t="s">
-        <v>195</v>
+        <v>201</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -38226,7 +38382,7 @@
         <v>84</v>
       </c>
       <c r="C8" s="7" t="s">
-        <v>196</v>
+        <v>202</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -38234,7 +38390,7 @@
         <v>84</v>
       </c>
       <c r="C9" s="7" t="s">
-        <v>197</v>
+        <v>203</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -38294,7 +38450,7 @@
         <v>80</v>
       </c>
       <c r="C18" s="3" t="s">
-        <v>198</v>
+        <v>204</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -38302,7 +38458,7 @@
         <v>80</v>
       </c>
       <c r="C19" s="3" t="s">
-        <v>199</v>
+        <v>205</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -38310,7 +38466,7 @@
         <v>80</v>
       </c>
       <c r="C20" s="3" t="s">
-        <v>200</v>
+        <v>206</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -38318,7 +38474,7 @@
         <v>80</v>
       </c>
       <c r="C21" s="3" t="s">
-        <v>201</v>
+        <v>207</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -38326,7 +38482,7 @@
         <v>80</v>
       </c>
       <c r="C22" s="3" t="s">
-        <v>202</v>
+        <v>208</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -38334,7 +38490,7 @@
         <v>80</v>
       </c>
       <c r="C23" s="3" t="s">
-        <v>203</v>
+        <v>209</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -38342,7 +38498,7 @@
         <v>80</v>
       </c>
       <c r="C24" s="3" t="s">
-        <v>204</v>
+        <v>210</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -38350,7 +38506,7 @@
         <v>80</v>
       </c>
       <c r="C25" s="3" t="s">
-        <v>205</v>
+        <v>211</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -38358,7 +38514,7 @@
         <v>80</v>
       </c>
       <c r="C26" s="3" t="s">
-        <v>206</v>
+        <v>212</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -38366,7 +38522,7 @@
         <v>80</v>
       </c>
       <c r="C27" s="3" t="s">
-        <v>207</v>
+        <v>213</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -38374,7 +38530,7 @@
         <v>80</v>
       </c>
       <c r="C28" s="3" t="s">
-        <v>208</v>
+        <v>214</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -38382,7 +38538,7 @@
         <v>80</v>
       </c>
       <c r="C29" s="3" t="s">
-        <v>209</v>
+        <v>215</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -38390,7 +38546,7 @@
         <v>80</v>
       </c>
       <c r="C30" s="3" t="s">
-        <v>210</v>
+        <v>216</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -38398,7 +38554,7 @@
         <v>80</v>
       </c>
       <c r="C31" s="3" t="s">
-        <v>211</v>
+        <v>217</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -38406,7 +38562,7 @@
         <v>80</v>
       </c>
       <c r="C32" s="3" t="s">
-        <v>212</v>
+        <v>218</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -38414,7 +38570,7 @@
         <v>80</v>
       </c>
       <c r="C33" s="3" t="s">
-        <v>213</v>
+        <v>219</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -38422,7 +38578,7 @@
         <v>80</v>
       </c>
       <c r="C34" s="3" t="s">
-        <v>214</v>
+        <v>220</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -38430,7 +38586,7 @@
         <v>80</v>
       </c>
       <c r="C35" s="3" t="s">
-        <v>215</v>
+        <v>221</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -38438,7 +38594,7 @@
         <v>80</v>
       </c>
       <c r="C36" s="3" t="s">
-        <v>216</v>
+        <v>222</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -38446,7 +38602,7 @@
         <v>80</v>
       </c>
       <c r="C37" s="3" t="s">
-        <v>217</v>
+        <v>223</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -38454,7 +38610,7 @@
         <v>80</v>
       </c>
       <c r="C38" s="3" t="s">
-        <v>218</v>
+        <v>224</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -38462,7 +38618,7 @@
         <v>80</v>
       </c>
       <c r="C39" s="3" t="s">
-        <v>219</v>
+        <v>225</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -38470,7 +38626,7 @@
         <v>80</v>
       </c>
       <c r="C40" s="3" t="s">
-        <v>220</v>
+        <v>226</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -38478,7 +38634,7 @@
         <v>80</v>
       </c>
       <c r="C41" s="3" t="s">
-        <v>221</v>
+        <v>227</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -38486,7 +38642,7 @@
         <v>80</v>
       </c>
       <c r="C42" s="3" t="s">
-        <v>222</v>
+        <v>228</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -38494,7 +38650,7 @@
         <v>80</v>
       </c>
       <c r="C43" s="3" t="s">
-        <v>223</v>
+        <v>229</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -38502,7 +38658,7 @@
         <v>80</v>
       </c>
       <c r="C44" s="3" t="s">
-        <v>224</v>
+        <v>230</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -38510,7 +38666,7 @@
         <v>80</v>
       </c>
       <c r="C45" s="3" t="s">
-        <v>225</v>
+        <v>231</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -38518,7 +38674,7 @@
         <v>80</v>
       </c>
       <c r="C46" s="3" t="s">
-        <v>226</v>
+        <v>232</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -38526,7 +38682,7 @@
         <v>80</v>
       </c>
       <c r="C47" s="3" t="s">
-        <v>227</v>
+        <v>233</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -38534,7 +38690,7 @@
         <v>80</v>
       </c>
       <c r="C48" s="3" t="s">
-        <v>228</v>
+        <v>234</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -38542,7 +38698,7 @@
         <v>80</v>
       </c>
       <c r="C49" s="3" t="s">
-        <v>229</v>
+        <v>235</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -38550,7 +38706,7 @@
         <v>80</v>
       </c>
       <c r="C50" s="3" t="s">
-        <v>230</v>
+        <v>236</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -38558,7 +38714,7 @@
         <v>80</v>
       </c>
       <c r="C51" s="3" t="s">
-        <v>231</v>
+        <v>237</v>
       </c>
     </row>
     <row r="52" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -38566,7 +38722,7 @@
         <v>80</v>
       </c>
       <c r="C52" s="3" t="s">
-        <v>232</v>
+        <v>238</v>
       </c>
     </row>
     <row r="53" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -38574,7 +38730,7 @@
         <v>80</v>
       </c>
       <c r="C53" s="3" t="s">
-        <v>233</v>
+        <v>239</v>
       </c>
     </row>
     <row r="54" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -38582,7 +38738,7 @@
         <v>80</v>
       </c>
       <c r="C54" s="3" t="s">
-        <v>234</v>
+        <v>240</v>
       </c>
     </row>
     <row r="55" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -38590,7 +38746,7 @@
         <v>80</v>
       </c>
       <c r="C55" s="3" t="s">
-        <v>235</v>
+        <v>241</v>
       </c>
     </row>
     <row r="56" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -38598,7 +38754,7 @@
         <v>80</v>
       </c>
       <c r="C56" s="3" t="s">
-        <v>236</v>
+        <v>242</v>
       </c>
     </row>
     <row r="57" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -38606,7 +38762,7 @@
         <v>80</v>
       </c>
       <c r="C57" s="3" t="s">
-        <v>237</v>
+        <v>243</v>
       </c>
     </row>
     <row r="58" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -38614,7 +38770,7 @@
         <v>80</v>
       </c>
       <c r="C58" s="3" t="s">
-        <v>238</v>
+        <v>244</v>
       </c>
     </row>
     <row r="59" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -38622,7 +38778,7 @@
         <v>80</v>
       </c>
       <c r="C59" s="3" t="s">
-        <v>239</v>
+        <v>245</v>
       </c>
     </row>
     <row r="60" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -38630,7 +38786,7 @@
         <v>80</v>
       </c>
       <c r="C60" s="3" t="s">
-        <v>240</v>
+        <v>246</v>
       </c>
     </row>
     <row r="61" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -38638,7 +38794,7 @@
         <v>80</v>
       </c>
       <c r="C61" s="3" t="s">
-        <v>241</v>
+        <v>247</v>
       </c>
     </row>
     <row r="62" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -38646,7 +38802,7 @@
         <v>80</v>
       </c>
       <c r="C62" s="3" t="s">
-        <v>242</v>
+        <v>248</v>
       </c>
     </row>
     <row r="63" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -38654,7 +38810,7 @@
         <v>80</v>
       </c>
       <c r="C63" s="3" t="s">
-        <v>243</v>
+        <v>249</v>
       </c>
     </row>
     <row r="64" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -38662,7 +38818,7 @@
         <v>80</v>
       </c>
       <c r="C64" s="3" t="s">
-        <v>244</v>
+        <v>250</v>
       </c>
     </row>
     <row r="65" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -38670,7 +38826,7 @@
         <v>80</v>
       </c>
       <c r="C65" s="3" t="s">
-        <v>245</v>
+        <v>251</v>
       </c>
     </row>
     <row r="66" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -38678,7 +38834,7 @@
         <v>80</v>
       </c>
       <c r="C66" s="3" t="s">
-        <v>246</v>
+        <v>252</v>
       </c>
     </row>
     <row r="68" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -38686,7 +38842,7 @@
         <v>80</v>
       </c>
       <c r="C68" s="3" t="s">
-        <v>247</v>
+        <v>253</v>
       </c>
     </row>
     <row r="69" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -38694,7 +38850,7 @@
         <v>80</v>
       </c>
       <c r="C69" s="3" t="s">
-        <v>248</v>
+        <v>254</v>
       </c>
     </row>
     <row r="70" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -38702,7 +38858,7 @@
         <v>80</v>
       </c>
       <c r="C70" s="3" t="s">
-        <v>249</v>
+        <v>255</v>
       </c>
     </row>
     <row r="71" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -38710,7 +38866,7 @@
         <v>80</v>
       </c>
       <c r="C71" s="3" t="s">
-        <v>250</v>
+        <v>256</v>
       </c>
     </row>
     <row r="72" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -38718,7 +38874,7 @@
         <v>80</v>
       </c>
       <c r="C72" s="3" t="s">
-        <v>251</v>
+        <v>257</v>
       </c>
     </row>
     <row r="73" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -38726,7 +38882,7 @@
         <v>80</v>
       </c>
       <c r="C73" s="3" t="s">
-        <v>252</v>
+        <v>258</v>
       </c>
     </row>
     <row r="74" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -38734,7 +38890,7 @@
         <v>80</v>
       </c>
       <c r="C74" s="3" t="s">
-        <v>253</v>
+        <v>259</v>
       </c>
     </row>
     <row r="75" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -38742,7 +38898,7 @@
         <v>80</v>
       </c>
       <c r="C75" s="3" t="s">
-        <v>254</v>
+        <v>260</v>
       </c>
     </row>
     <row r="76" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -38750,7 +38906,7 @@
         <v>80</v>
       </c>
       <c r="C76" s="3" t="s">
-        <v>255</v>
+        <v>261</v>
       </c>
     </row>
     <row r="77" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -38758,7 +38914,7 @@
         <v>80</v>
       </c>
       <c r="C77" s="3" t="s">
-        <v>256</v>
+        <v>262</v>
       </c>
     </row>
     <row r="78" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -38766,7 +38922,7 @@
         <v>80</v>
       </c>
       <c r="C78" s="3" t="s">
-        <v>257</v>
+        <v>263</v>
       </c>
     </row>
     <row r="79" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -38774,7 +38930,7 @@
         <v>80</v>
       </c>
       <c r="C79" s="3" t="s">
-        <v>258</v>
+        <v>264</v>
       </c>
     </row>
     <row r="80" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -38782,7 +38938,7 @@
         <v>80</v>
       </c>
       <c r="C80" s="3" t="s">
-        <v>259</v>
+        <v>265</v>
       </c>
     </row>
     <row r="81" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -38790,7 +38946,7 @@
         <v>80</v>
       </c>
       <c r="C81" s="3" t="s">
-        <v>260</v>
+        <v>266</v>
       </c>
     </row>
     <row r="82" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -38798,7 +38954,7 @@
         <v>80</v>
       </c>
       <c r="C82" s="3" t="s">
-        <v>261</v>
+        <v>267</v>
       </c>
     </row>
     <row r="83" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -38806,7 +38962,7 @@
         <v>80</v>
       </c>
       <c r="C83" s="3" t="s">
-        <v>262</v>
+        <v>268</v>
       </c>
     </row>
     <row r="84" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -38814,7 +38970,7 @@
         <v>80</v>
       </c>
       <c r="C84" s="3" t="s">
-        <v>263</v>
+        <v>269</v>
       </c>
     </row>
     <row r="85" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -38822,7 +38978,7 @@
         <v>80</v>
       </c>
       <c r="C85" s="3" t="s">
-        <v>264</v>
+        <v>270</v>
       </c>
     </row>
     <row r="86" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -38830,7 +38986,7 @@
         <v>80</v>
       </c>
       <c r="C86" s="3" t="s">
-        <v>265</v>
+        <v>271</v>
       </c>
     </row>
     <row r="87" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -38838,7 +38994,7 @@
         <v>80</v>
       </c>
       <c r="C87" s="3" t="s">
-        <v>266</v>
+        <v>272</v>
       </c>
     </row>
     <row r="89" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -38846,7 +39002,7 @@
         <v>80</v>
       </c>
       <c r="C89" s="3" t="s">
-        <v>267</v>
+        <v>273</v>
       </c>
     </row>
     <row r="90" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -38854,7 +39010,7 @@
         <v>80</v>
       </c>
       <c r="C90" s="3" t="s">
-        <v>268</v>
+        <v>274</v>
       </c>
     </row>
     <row r="91" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -38862,7 +39018,7 @@
         <v>80</v>
       </c>
       <c r="C91" s="3" t="s">
-        <v>269</v>
+        <v>275</v>
       </c>
     </row>
     <row r="92" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -38870,7 +39026,7 @@
         <v>80</v>
       </c>
       <c r="C92" s="3" t="s">
-        <v>270</v>
+        <v>276</v>
       </c>
     </row>
     <row r="93" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -38878,7 +39034,7 @@
         <v>80</v>
       </c>
       <c r="C93" s="3" t="s">
-        <v>271</v>
+        <v>277</v>
       </c>
     </row>
     <row r="94" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -38886,7 +39042,7 @@
         <v>80</v>
       </c>
       <c r="C94" s="3" t="s">
-        <v>272</v>
+        <v>278</v>
       </c>
     </row>
     <row r="95" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -38894,7 +39050,7 @@
         <v>80</v>
       </c>
       <c r="C95" s="3" t="s">
-        <v>273</v>
+        <v>279</v>
       </c>
     </row>
     <row r="96" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -38902,7 +39058,7 @@
         <v>80</v>
       </c>
       <c r="C96" s="3" t="s">
-        <v>274</v>
+        <v>280</v>
       </c>
     </row>
     <row r="97" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -38910,7 +39066,7 @@
         <v>80</v>
       </c>
       <c r="C97" s="3" t="s">
-        <v>275</v>
+        <v>281</v>
       </c>
     </row>
     <row r="98" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -38918,7 +39074,7 @@
         <v>80</v>
       </c>
       <c r="C98" s="3" t="s">
-        <v>276</v>
+        <v>282</v>
       </c>
     </row>
     <row r="99" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -38926,7 +39082,7 @@
         <v>80</v>
       </c>
       <c r="C99" s="3" t="s">
-        <v>277</v>
+        <v>283</v>
       </c>
     </row>
     <row r="100" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -38934,7 +39090,7 @@
         <v>80</v>
       </c>
       <c r="C100" s="3" t="s">
-        <v>278</v>
+        <v>284</v>
       </c>
     </row>
     <row r="101" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -38942,7 +39098,7 @@
         <v>80</v>
       </c>
       <c r="C101" s="3" t="s">
-        <v>279</v>
+        <v>285</v>
       </c>
     </row>
     <row r="102" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -38950,7 +39106,7 @@
         <v>80</v>
       </c>
       <c r="C102" s="3" t="s">
-        <v>280</v>
+        <v>286</v>
       </c>
     </row>
     <row r="103" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -38958,7 +39114,7 @@
         <v>80</v>
       </c>
       <c r="C103" s="3" t="s">
-        <v>281</v>
+        <v>287</v>
       </c>
     </row>
     <row r="104" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -38966,7 +39122,7 @@
         <v>80</v>
       </c>
       <c r="C104" s="3" t="s">
-        <v>282</v>
+        <v>288</v>
       </c>
     </row>
     <row r="105" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -38974,7 +39130,7 @@
         <v>80</v>
       </c>
       <c r="C105" s="3" t="s">
-        <v>283</v>
+        <v>289</v>
       </c>
     </row>
     <row r="106" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -38982,7 +39138,7 @@
         <v>80</v>
       </c>
       <c r="C106" s="3" t="s">
-        <v>284</v>
+        <v>290</v>
       </c>
     </row>
     <row r="107" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -38990,7 +39146,7 @@
         <v>80</v>
       </c>
       <c r="C107" s="3" t="s">
-        <v>285</v>
+        <v>291</v>
       </c>
     </row>
     <row r="108" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -38998,7 +39154,7 @@
         <v>80</v>
       </c>
       <c r="C108" s="3" t="s">
-        <v>286</v>
+        <v>292</v>
       </c>
     </row>
     <row r="109" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -39006,7 +39162,7 @@
         <v>80</v>
       </c>
       <c r="C109" s="7" t="s">
-        <v>287</v>
+        <v>293</v>
       </c>
     </row>
     <row r="111" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -39014,7 +39170,7 @@
         <v>80</v>
       </c>
       <c r="C111" s="3" t="s">
-        <v>288</v>
+        <v>294</v>
       </c>
     </row>
     <row r="112" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -39022,7 +39178,7 @@
         <v>80</v>
       </c>
       <c r="C112" s="7" t="s">
-        <v>289</v>
+        <v>295</v>
       </c>
     </row>
     <row r="113" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -39030,7 +39186,7 @@
         <v>80</v>
       </c>
       <c r="C113" s="7" t="s">
-        <v>290</v>
+        <v>296</v>
       </c>
     </row>
     <row r="114" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -39038,7 +39194,15 @@
         <v>80</v>
       </c>
       <c r="C114" s="7" t="s">
-        <v>291</v>
+        <v>297</v>
+      </c>
+    </row>
+    <row r="116" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B116" s="7" t="s">
+        <v>80</v>
+      </c>
+      <c r="C116" s="7" t="s">
+        <v>298</v>
       </c>
     </row>
   </sheetData>
@@ -39065,14 +39229,14 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="31.1363636363636"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="36.6161616161616"/>
-    <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="8.41919191919192"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="29.7979797979798"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="35.010101010101"/>
+    <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="7.88383838383838"/>
   </cols>
   <sheetData>
     <row r="1" s="2" customFormat="true" ht="13.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
-        <v>292</v>
+        <v>299</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>68</v>
@@ -39080,26 +39244,26 @@
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="7" t="s">
-        <v>293</v>
+        <v>300</v>
       </c>
       <c r="B3" s="7" t="s">
-        <v>294</v>
+        <v>301</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="7" t="s">
-        <v>295</v>
+        <v>302</v>
       </c>
       <c r="B4" s="7" t="s">
-        <v>296</v>
+        <v>303</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="7" t="s">
-        <v>297</v>
+        <v>304</v>
       </c>
       <c r="B5" s="7" t="s">
-        <v>298</v>
+        <v>305</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
adds document restriction questions
</commit_message>
<xml_diff>
--- a/tables/actor/forms/actor/actor.xlsx
+++ b/tables/actor/forms/actor/actor.xlsx
@@ -533,44 +533,7 @@
     <t xml:space="preserve">Relationship to you: (check all that apply)</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="Myanmar3"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">အဲ့ဒီသူနဲ့ ခင်ဗျား ဘယ်လို တော်စပ်သလဲ။ </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="Myanmar3"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">(</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="Myanmar3"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">သက်ဆိုင်တာ အားလုံးကို ရွေးပါ</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="Myanmar3"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">) </t>
-    </r>
+    <t xml:space="preserve">အဲ့ဒီသူနဲ့ ခင်ဗျား ဘယ်လို တော်စပ်သလဲ။</t>
   </si>
   <si>
     <t xml:space="preserve">other_relationship</t>
@@ -1881,11 +1844,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="10.6919191919192"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="7.61616161616162"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="13.4949494949495"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="31.2676767676768"/>
-    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="7.61616161616162"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="10.1565656565657"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="12.8282828282828"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="29.9343434343434"/>
   </cols>
   <sheetData>
     <row r="1" s="2" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1942,14 +1903,14 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="10.4242424242424"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="9.88888888888889"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="20.3131313131313"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="18.040404040404"/>
-    <col collapsed="false" hidden="false" max="7" min="5" style="0" width="7.88383838383838"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="19.9090909090909"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="15.9040404040404"/>
-    <col collapsed="false" hidden="false" max="1025" min="10" style="0" width="7.88383838383838"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="9.88888888888889"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="9.35353535353535"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="19.2424242424242"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="17.1060606060606"/>
+    <col collapsed="false" hidden="false" max="7" min="5" style="0" width="7.34848484848485"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="18.9747474747475"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="15.1010101010101"/>
+    <col collapsed="false" hidden="false" max="1025" min="10" style="0" width="7.34848484848485"/>
   </cols>
   <sheetData>
     <row r="1" s="2" customFormat="true" ht="18.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -2070,17 +2031,17 @@
   <dimension ref="1:65"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A17" activeCellId="0" sqref="A17"/>
+      <selection pane="topLeft" activeCell="C11" activeCellId="0" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="3" width="23.520202020202"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="3" width="36.7474747474747"/>
-    <col collapsed="false" hidden="false" max="4" min="3" style="3" width="55.7222222222222"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="3" width="63.3383838383838"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="3" width="22.4494949494949"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="3" width="35.1464646464646"/>
+    <col collapsed="false" hidden="false" max="4" min="3" style="3" width="53.3181818181818"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="3" width="60.5353535353535"/>
     <col collapsed="false" hidden="false" max="1023" min="6" style="3" width="3.07575757575758"/>
-    <col collapsed="false" hidden="false" max="1025" min="1024" style="0" width="8.41919191919192"/>
+    <col collapsed="false" hidden="false" max="1025" min="1024" style="0" width="7.88383838383838"/>
   </cols>
   <sheetData>
     <row r="1" s="1" customFormat="true" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -37217,27 +37178,26 @@
   </sheetPr>
   <dimension ref="1:19"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H10" activeCellId="0" sqref="H10"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="D1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="I19" activeCellId="0" sqref="I19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="7.88383838383838"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="9.35353535353535"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="7.88383838383838"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="29.2626262626263"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="27.9191919191919"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="22.8232323232323"/>
-    <col collapsed="false" hidden="false" max="8" min="7" style="0" width="33.8333333333333"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="12.0252525252525"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="7.61616161616162"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="7.88383838383838"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="10.1565656565657"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="13.8989898989899"/>
-    <col collapsed="false" hidden="false" max="19" min="14" style="0" width="7.88383838383838"/>
-    <col collapsed="false" hidden="false" max="20" min="20" style="0" width="15.5"/>
-    <col collapsed="false" hidden="false" max="1025" min="21" style="0" width="7.88383838383838"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="7.34848484848485"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="8.95454545454546"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="7.34848484848485"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="27.9292929292929"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="26.5909090909091"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="21.7828282828283"/>
+    <col collapsed="false" hidden="false" max="8" min="7" style="0" width="32.3383838383838"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="11.2272727272727"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="7.34848484848485"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="9.62121212121212"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="13.0959595959596"/>
+    <col collapsed="false" hidden="false" max="19" min="14" style="0" width="7.34848484848485"/>
+    <col collapsed="false" hidden="false" max="20" min="20" style="0" width="14.6969696969697"/>
+    <col collapsed="false" hidden="false" max="1025" min="21" style="0" width="7.34848484848485"/>
   </cols>
   <sheetData>
     <row r="1" s="6" customFormat="true" ht="17.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -37372,9 +37332,7 @@
       <c r="H5" s="4" t="s">
         <v>81</v>
       </c>
-      <c r="I5" s="3" t="n">
-        <v>1</v>
-      </c>
+      <c r="I5" s="3"/>
       <c r="L5" s="3"/>
     </row>
     <row r="6" customFormat="false" ht="21.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -37424,9 +37382,6 @@
       <c r="H9" s="7" t="s">
         <v>87</v>
       </c>
-      <c r="I9" s="0" t="n">
-        <v>1</v>
-      </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C10" s="7" t="s">
@@ -37467,9 +37422,6 @@
       <c r="H13" s="7" t="s">
         <v>91</v>
       </c>
-      <c r="I13" s="0" t="n">
-        <v>1</v>
-      </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C14" s="7" t="s">
@@ -37510,9 +37462,6 @@
       <c r="H17" s="9" t="s">
         <v>95</v>
       </c>
-      <c r="I17" s="0" t="n">
-        <v>1</v>
-      </c>
     </row>
     <row r="18" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E18" s="9" t="s">
@@ -37526,9 +37475,6 @@
       </c>
       <c r="H18" s="7" t="s">
         <v>97</v>
-      </c>
-      <c r="I18" s="0" t="n">
-        <v>1</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -37560,13 +37506,13 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="12.2929292929293"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="34.2070707070707"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="29.5656565656566"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="40.0151515151515"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="38.7777777777778"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="38.4848484848485"/>
-    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="7.88383838383838"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="11.6262626262626"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="32.6060606060606"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="28.1969696969697"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="38.2171717171717"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="37.0151515151515"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="36.7474747474747"/>
+    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="7.34848484848485"/>
   </cols>
   <sheetData>
     <row r="1" s="1" customFormat="true" ht="22.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -38310,12 +38256,12 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="11.2272727272727"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="12.8282828282828"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="30.469696969697"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="11.6262626262626"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="20.4444444444444"/>
-    <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="7.88383838383838"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="10.6919191919192"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="12.2929292929293"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="29.1313131313131"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="10.959595959596"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="19.3737373737374"/>
+    <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="7.34848484848485"/>
   </cols>
   <sheetData>
     <row r="1" s="6" customFormat="true" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -39229,9 +39175,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="29.7979797979798"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="35.010101010101"/>
-    <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="7.88383838383838"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="28.4646464646465"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="33.4090909090909"/>
+    <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="7.34848484848485"/>
   </cols>
   <sheetData>
     <row r="1" s="2" customFormat="true" ht="13.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">

</xml_diff>